<commit_message>
Updates to the DU
</commit_message>
<xml_diff>
--- a/metrics/du.xlsx
+++ b/metrics/du.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\GitHub\project-g4t6\metrics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C651DA3E-A253-42D5-8BD1-95EAFDB77E0C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{813690D2-47C5-419E-AAAB-67871B357675}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="492" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="466" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="496" uniqueCount="65">
   <si>
     <t>Question</t>
   </si>
@@ -296,7 +296,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -343,19 +343,22 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -683,36 +686,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="23" t="s">
+      <c r="C1" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
-      <c r="H1" s="23"/>
-      <c r="I1" s="23"/>
-      <c r="J1" s="20" t="s">
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="21"/>
+      <c r="H1" s="21"/>
+      <c r="I1" s="21"/>
+      <c r="J1" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="K1" s="18" t="s">
+      <c r="K1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="L1" s="23" t="s">
+      <c r="L1" s="21" t="s">
         <v>40</v>
       </c>
-      <c r="M1" s="23"/>
-      <c r="N1" s="23"/>
-      <c r="O1" s="23"/>
-      <c r="P1" s="23"/>
-      <c r="Q1" s="23"/>
-      <c r="R1" s="23"/>
+      <c r="M1" s="21"/>
+      <c r="N1" s="21"/>
+      <c r="O1" s="21"/>
+      <c r="P1" s="21"/>
+      <c r="Q1" s="21"/>
+      <c r="R1" s="21"/>
       <c r="S1" s="1"/>
       <c r="T1" s="1"/>
       <c r="U1" s="1"/>
@@ -723,8 +726,8 @@
       <c r="Z1" s="1"/>
     </row>
     <row r="2" spans="1:26" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A2" s="19"/>
-      <c r="B2" s="19"/>
+      <c r="A2" s="20"/>
+      <c r="B2" s="20"/>
       <c r="C2" s="3" t="s">
         <v>2</v>
       </c>
@@ -746,8 +749,8 @@
       <c r="I2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="J2" s="19"/>
-      <c r="K2" s="19"/>
+      <c r="J2" s="20"/>
+      <c r="K2" s="20"/>
       <c r="L2" s="3" t="s">
         <v>2</v>
       </c>
@@ -779,7 +782,7 @@
       <c r="Z2" s="1"/>
     </row>
     <row r="3" spans="1:26" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="21" t="s">
+      <c r="A3" s="22" t="s">
         <v>13</v>
       </c>
       <c r="B3" s="4" t="s">
@@ -798,7 +801,7 @@
       <c r="I3" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="J3" s="21" t="s">
+      <c r="J3" s="22" t="s">
         <v>13</v>
       </c>
       <c r="K3" s="4" t="s">
@@ -827,7 +830,7 @@
       </c>
     </row>
     <row r="4" spans="1:26" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="22"/>
+      <c r="A4" s="23"/>
       <c r="B4" s="4" t="s">
         <v>12</v>
       </c>
@@ -844,7 +847,7 @@
       <c r="I4" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="J4" s="22"/>
+      <c r="J4" s="23"/>
       <c r="K4" s="4" t="s">
         <v>12</v>
       </c>
@@ -871,7 +874,7 @@
       </c>
     </row>
     <row r="5" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="22"/>
+      <c r="A5" s="23"/>
       <c r="B5" s="4" t="s">
         <v>9</v>
       </c>
@@ -888,7 +891,7 @@
       <c r="I5" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="J5" s="22"/>
+      <c r="J5" s="23"/>
       <c r="K5" s="4" t="s">
         <v>9</v>
       </c>
@@ -915,7 +918,7 @@
       </c>
     </row>
     <row r="6" spans="1:26" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="21" t="s">
+      <c r="A6" s="22" t="s">
         <v>14</v>
       </c>
       <c r="B6" s="4" t="s">
@@ -934,7 +937,7 @@
       <c r="I6" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="J6" s="21" t="s">
+      <c r="J6" s="22" t="s">
         <v>14</v>
       </c>
       <c r="K6" s="4" t="s">
@@ -963,7 +966,7 @@
       </c>
     </row>
     <row r="7" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="22"/>
+      <c r="A7" s="23"/>
       <c r="B7" s="4" t="s">
         <v>8</v>
       </c>
@@ -980,7 +983,7 @@
       <c r="I7" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="J7" s="22"/>
+      <c r="J7" s="23"/>
       <c r="K7" s="4" t="s">
         <v>8</v>
       </c>
@@ -1007,7 +1010,7 @@
       </c>
     </row>
     <row r="8" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="22"/>
+      <c r="A8" s="23"/>
       <c r="B8" s="4" t="s">
         <v>9</v>
       </c>
@@ -1024,7 +1027,7 @@
       <c r="I8" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="J8" s="22"/>
+      <c r="J8" s="23"/>
       <c r="K8" s="4" t="s">
         <v>9</v>
       </c>
@@ -1051,7 +1054,7 @@
       </c>
     </row>
     <row r="9" spans="1:26" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="21" t="s">
+      <c r="A9" s="22" t="s">
         <v>15</v>
       </c>
       <c r="B9" s="4" t="s">
@@ -1070,7 +1073,7 @@
       <c r="I9" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="J9" s="21" t="s">
+      <c r="J9" s="22" t="s">
         <v>15</v>
       </c>
       <c r="K9" s="4" t="s">
@@ -1099,7 +1102,7 @@
       </c>
     </row>
     <row r="10" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="22"/>
+      <c r="A10" s="23"/>
       <c r="B10" s="4" t="s">
         <v>8</v>
       </c>
@@ -1116,7 +1119,7 @@
       <c r="I10" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="J10" s="22"/>
+      <c r="J10" s="23"/>
       <c r="K10" s="4" t="s">
         <v>8</v>
       </c>
@@ -1143,7 +1146,7 @@
       </c>
     </row>
     <row r="11" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="22"/>
+      <c r="A11" s="23"/>
       <c r="B11" s="4" t="s">
         <v>9</v>
       </c>
@@ -1160,7 +1163,7 @@
       <c r="I11" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="J11" s="22"/>
+      <c r="J11" s="23"/>
       <c r="K11" s="4" t="s">
         <v>9</v>
       </c>
@@ -1187,7 +1190,7 @@
       </c>
     </row>
     <row r="12" spans="1:26" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="21" t="s">
+      <c r="A12" s="22" t="s">
         <v>16</v>
       </c>
       <c r="B12" s="4" t="s">
@@ -1206,7 +1209,7 @@
       <c r="I12" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="J12" s="21" t="s">
+      <c r="J12" s="22" t="s">
         <v>16</v>
       </c>
       <c r="K12" s="4" t="s">
@@ -1235,7 +1238,7 @@
       </c>
     </row>
     <row r="13" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="22"/>
+      <c r="A13" s="23"/>
       <c r="B13" s="4" t="s">
         <v>8</v>
       </c>
@@ -1252,7 +1255,7 @@
       <c r="I13" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="J13" s="22"/>
+      <c r="J13" s="23"/>
       <c r="K13" s="4" t="s">
         <v>8</v>
       </c>
@@ -1279,7 +1282,7 @@
       </c>
     </row>
     <row r="14" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="22"/>
+      <c r="A14" s="23"/>
       <c r="B14" s="4" t="s">
         <v>9</v>
       </c>
@@ -1296,7 +1299,7 @@
       <c r="I14" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="J14" s="22"/>
+      <c r="J14" s="23"/>
       <c r="K14" s="4" t="s">
         <v>9</v>
       </c>
@@ -1323,7 +1326,7 @@
       </c>
     </row>
     <row r="15" spans="1:26" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="21" t="s">
+      <c r="A15" s="22" t="s">
         <v>17</v>
       </c>
       <c r="B15" s="4" t="s">
@@ -1342,7 +1345,7 @@
       <c r="I15" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="J15" s="21" t="s">
+      <c r="J15" s="22" t="s">
         <v>17</v>
       </c>
       <c r="K15" s="4" t="s">
@@ -1371,7 +1374,7 @@
       </c>
     </row>
     <row r="16" spans="1:26" ht="77.400000000000006" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="22"/>
+      <c r="A16" s="23"/>
       <c r="B16" s="4" t="s">
         <v>8</v>
       </c>
@@ -1388,7 +1391,7 @@
       <c r="I16" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="J16" s="22"/>
+      <c r="J16" s="23"/>
       <c r="K16" s="4" t="s">
         <v>8</v>
       </c>
@@ -1415,7 +1418,7 @@
       </c>
     </row>
     <row r="17" spans="1:18" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="22"/>
+      <c r="A17" s="23"/>
       <c r="B17" s="4" t="s">
         <v>9</v>
       </c>
@@ -1432,7 +1435,7 @@
       <c r="I17" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="J17" s="22"/>
+      <c r="J17" s="23"/>
       <c r="K17" s="4" t="s">
         <v>9</v>
       </c>
@@ -5396,11 +5399,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="K1:K2"/>
-    <mergeCell ref="L1:R1"/>
-    <mergeCell ref="J3:J5"/>
-    <mergeCell ref="J6:J8"/>
-    <mergeCell ref="C1:I1"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="J15:J17"/>
@@ -5412,6 +5410,11 @@
     <mergeCell ref="A3:A5"/>
     <mergeCell ref="A6:A8"/>
     <mergeCell ref="A9:A11"/>
+    <mergeCell ref="K1:K2"/>
+    <mergeCell ref="L1:R1"/>
+    <mergeCell ref="J3:J5"/>
+    <mergeCell ref="J6:J8"/>
+    <mergeCell ref="C1:I1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -5445,24 +5448,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="C1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="23" t="s">
+      <c r="D1" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
-      <c r="H1" s="23"/>
-      <c r="I1" s="23"/>
-      <c r="J1" s="23"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="21"/>
+      <c r="H1" s="21"/>
+      <c r="I1" s="21"/>
+      <c r="J1" s="21"/>
       <c r="S1" s="1"/>
       <c r="T1" s="1"/>
       <c r="U1" s="1"/>
@@ -5473,9 +5476,9 @@
       <c r="Z1" s="1"/>
     </row>
     <row r="2" spans="1:26" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A2" s="19"/>
-      <c r="B2" s="19"/>
-      <c r="C2" s="19"/>
+      <c r="A2" s="20"/>
+      <c r="B2" s="20"/>
+      <c r="C2" s="20"/>
       <c r="D2" s="3" t="s">
         <v>2</v>
       </c>
@@ -5507,7 +5510,7 @@
       <c r="Z2" s="1"/>
     </row>
     <row r="3" spans="1:26" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="21" t="s">
+      <c r="A3" s="22" t="s">
         <v>13</v>
       </c>
       <c r="B3" s="4" t="s">
@@ -5539,7 +5542,7 @@
       </c>
     </row>
     <row r="4" spans="1:26" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="22"/>
+      <c r="A4" s="23"/>
       <c r="B4" s="4" t="s">
         <v>12</v>
       </c>
@@ -5569,7 +5572,7 @@
       </c>
     </row>
     <row r="5" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="22"/>
+      <c r="A5" s="23"/>
       <c r="B5" s="4" t="s">
         <v>9</v>
       </c>
@@ -5599,7 +5602,7 @@
       </c>
     </row>
     <row r="6" spans="1:26" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="21" t="s">
+      <c r="A6" s="22" t="s">
         <v>14</v>
       </c>
       <c r="B6" s="4" t="s">
@@ -5631,7 +5634,7 @@
       </c>
     </row>
     <row r="7" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="22"/>
+      <c r="A7" s="23"/>
       <c r="B7" s="4" t="s">
         <v>8</v>
       </c>
@@ -5661,7 +5664,7 @@
       </c>
     </row>
     <row r="8" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="22"/>
+      <c r="A8" s="23"/>
       <c r="B8" s="4" t="s">
         <v>9</v>
       </c>
@@ -5691,7 +5694,7 @@
       </c>
     </row>
     <row r="9" spans="1:26" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="21" t="s">
+      <c r="A9" s="22" t="s">
         <v>15</v>
       </c>
       <c r="B9" s="4" t="s">
@@ -5723,7 +5726,7 @@
       </c>
     </row>
     <row r="10" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="22"/>
+      <c r="A10" s="23"/>
       <c r="B10" s="4" t="s">
         <v>8</v>
       </c>
@@ -5753,7 +5756,7 @@
       </c>
     </row>
     <row r="11" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="22"/>
+      <c r="A11" s="23"/>
       <c r="B11" s="4" t="s">
         <v>9</v>
       </c>
@@ -5783,7 +5786,7 @@
       </c>
     </row>
     <row r="12" spans="1:26" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="21" t="s">
+      <c r="A12" s="22" t="s">
         <v>16</v>
       </c>
       <c r="B12" s="4" t="s">
@@ -5815,7 +5818,7 @@
       </c>
     </row>
     <row r="13" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="22"/>
+      <c r="A13" s="23"/>
       <c r="B13" s="4" t="s">
         <v>8</v>
       </c>
@@ -5845,7 +5848,7 @@
       </c>
     </row>
     <row r="14" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="22"/>
+      <c r="A14" s="23"/>
       <c r="B14" s="4" t="s">
         <v>9</v>
       </c>
@@ -5875,7 +5878,7 @@
       </c>
     </row>
     <row r="15" spans="1:26" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="21" t="s">
+      <c r="A15" s="22" t="s">
         <v>17</v>
       </c>
       <c r="B15" s="4" t="s">
@@ -5907,7 +5910,7 @@
       </c>
     </row>
     <row r="16" spans="1:26" ht="77.400000000000006" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="22"/>
+      <c r="A16" s="23"/>
       <c r="B16" s="4" t="s">
         <v>8</v>
       </c>
@@ -5937,7 +5940,7 @@
       </c>
     </row>
     <row r="17" spans="1:10" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="22"/>
+      <c r="A17" s="23"/>
       <c r="B17" s="4" t="s">
         <v>9</v>
       </c>
@@ -9923,8 +9926,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32A3AA99-F4D2-4A92-BF2C-95E1F810A93F}">
   <dimension ref="A1:I17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.44140625" defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.3"/>
@@ -9933,25 +9936,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="27" t="s">
+      <c r="B1" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="26" t="s">
+      <c r="C1" s="27" t="s">
         <v>42</v>
       </c>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
-      <c r="H1" s="26"/>
-      <c r="I1" s="26"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
+      <c r="H1" s="27"/>
+      <c r="I1" s="27"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" s="28"/>
-      <c r="B2" s="28"/>
+      <c r="A2" s="29"/>
+      <c r="B2" s="29"/>
       <c r="C2" s="14" t="s">
         <v>2</v>
       </c>
@@ -9975,7 +9978,7 @@
       </c>
     </row>
     <row r="3" spans="1:9" ht="87" x14ac:dyDescent="0.3">
-      <c r="A3" s="24" t="s">
+      <c r="A3" s="25" t="s">
         <v>13</v>
       </c>
       <c r="B3" s="15" t="s">
@@ -9996,9 +9999,15 @@
       <c r="G3" s="17" t="s">
         <v>62</v>
       </c>
+      <c r="H3" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="I3" s="18" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="4" spans="1:9" ht="104.4" x14ac:dyDescent="0.3">
-      <c r="A4" s="25"/>
+      <c r="A4" s="26"/>
       <c r="B4" s="15" t="s">
         <v>12</v>
       </c>
@@ -10017,9 +10026,15 @@
       <c r="G4" s="17" t="s">
         <v>55</v>
       </c>
+      <c r="H4" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="I4" s="18" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="5" spans="1:9" ht="52.2" x14ac:dyDescent="0.3">
-      <c r="A5" s="25"/>
+      <c r="A5" s="26"/>
       <c r="B5" s="15" t="s">
         <v>9</v>
       </c>
@@ -10038,9 +10053,15 @@
       <c r="G5" s="12" t="s">
         <v>44</v>
       </c>
+      <c r="H5" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="I5" s="18" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="6" spans="1:9" ht="156.6" x14ac:dyDescent="0.3">
-      <c r="A6" s="24" t="s">
+      <c r="A6" s="25" t="s">
         <v>14</v>
       </c>
       <c r="B6" s="15" t="s">
@@ -10061,9 +10082,15 @@
       <c r="G6" s="17" t="s">
         <v>64</v>
       </c>
+      <c r="H6" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="I6" s="18" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="7" spans="1:9" ht="156.6" x14ac:dyDescent="0.3">
-      <c r="A7" s="25"/>
+      <c r="A7" s="26"/>
       <c r="B7" s="15" t="s">
         <v>8</v>
       </c>
@@ -10082,9 +10109,15 @@
       <c r="G7" s="17" t="s">
         <v>55</v>
       </c>
+      <c r="H7" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="I7" s="18" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="8" spans="1:9" ht="69.599999999999994" x14ac:dyDescent="0.3">
-      <c r="A8" s="25"/>
+      <c r="A8" s="26"/>
       <c r="B8" s="15" t="s">
         <v>9</v>
       </c>
@@ -10103,9 +10136,15 @@
       <c r="G8" s="17" t="s">
         <v>44</v>
       </c>
+      <c r="H8" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="I8" s="18" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="9" spans="1:9" ht="139.19999999999999" x14ac:dyDescent="0.3">
-      <c r="A9" s="24" t="s">
+      <c r="A9" s="25" t="s">
         <v>15</v>
       </c>
       <c r="B9" s="15" t="s">
@@ -10126,9 +10165,15 @@
       <c r="G9" s="17" t="s">
         <v>64</v>
       </c>
+      <c r="H9" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="I9" s="18" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="10" spans="1:9" ht="156.6" x14ac:dyDescent="0.3">
-      <c r="A10" s="25"/>
+      <c r="A10" s="26"/>
       <c r="B10" s="15" t="s">
         <v>8</v>
       </c>
@@ -10147,9 +10192,15 @@
       <c r="G10" s="17" t="s">
         <v>55</v>
       </c>
+      <c r="H10" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="I10" s="18" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="11" spans="1:9" ht="69.599999999999994" x14ac:dyDescent="0.3">
-      <c r="A11" s="25"/>
+      <c r="A11" s="26"/>
       <c r="B11" s="15" t="s">
         <v>9</v>
       </c>
@@ -10168,9 +10219,15 @@
       <c r="G11" s="17" t="s">
         <v>44</v>
       </c>
+      <c r="H11" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="I11" s="18" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="12" spans="1:9" ht="156.6" x14ac:dyDescent="0.3">
-      <c r="A12" s="24" t="s">
+      <c r="A12" s="25" t="s">
         <v>16</v>
       </c>
       <c r="B12" s="15" t="s">
@@ -10191,9 +10248,15 @@
       <c r="G12" s="17" t="s">
         <v>62</v>
       </c>
+      <c r="H12" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="I12" s="18" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="13" spans="1:9" ht="156.6" x14ac:dyDescent="0.3">
-      <c r="A13" s="25"/>
+      <c r="A13" s="26"/>
       <c r="B13" s="15" t="s">
         <v>8</v>
       </c>
@@ -10212,9 +10275,15 @@
       <c r="G13" s="17" t="s">
         <v>55</v>
       </c>
+      <c r="H13" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="I13" s="18" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="14" spans="1:9" ht="174" x14ac:dyDescent="0.3">
-      <c r="A14" s="25"/>
+      <c r="A14" s="26"/>
       <c r="B14" s="15" t="s">
         <v>9</v>
       </c>
@@ -10233,9 +10302,15 @@
       <c r="G14" s="12" t="s">
         <v>44</v>
       </c>
+      <c r="H14" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="I14" s="18" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="15" spans="1:9" ht="104.4" x14ac:dyDescent="0.3">
-      <c r="A15" s="24" t="s">
+      <c r="A15" s="25" t="s">
         <v>17</v>
       </c>
       <c r="B15" s="15" t="s">
@@ -10256,9 +10331,15 @@
       <c r="G15" s="17" t="s">
         <v>62</v>
       </c>
+      <c r="H15" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="I15" s="18" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="16" spans="1:9" ht="156.6" x14ac:dyDescent="0.3">
-      <c r="A16" s="25"/>
+      <c r="A16" s="26"/>
       <c r="B16" s="15" t="s">
         <v>8</v>
       </c>
@@ -10277,9 +10358,15 @@
       <c r="G16" s="17" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" ht="69.599999999999994" x14ac:dyDescent="0.3">
-      <c r="A17" s="25"/>
+      <c r="H16" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="I16" s="18" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="69.599999999999994" x14ac:dyDescent="0.3">
+      <c r="A17" s="26"/>
       <c r="B17" s="15" t="s">
         <v>9</v>
       </c>
@@ -10296,6 +10383,12 @@
         <v>61</v>
       </c>
       <c r="G17" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="H17" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="I17" s="18" t="s">
         <v>44</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updated du (week9 Fri)
</commit_message>
<xml_diff>
--- a/metrics/du.xlsx
+++ b/metrics/du.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\project-g4t6\metrics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAE8412B-FD3B-40EC-9920-3CA24042FF42}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{806B8C6D-7CAA-42D2-AE1F-500B333F5EF6}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="721" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="736" uniqueCount="89">
   <si>
     <t>Question</t>
   </si>
@@ -388,7 +388,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -480,19 +480,22 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -820,36 +823,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="33" t="s">
+      <c r="B1" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="38" t="s">
+      <c r="C1" s="36" t="s">
         <v>18</v>
       </c>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="38"/>
-      <c r="G1" s="38"/>
-      <c r="H1" s="38"/>
-      <c r="I1" s="38"/>
-      <c r="J1" s="35" t="s">
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
+      <c r="I1" s="36"/>
+      <c r="J1" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="K1" s="33" t="s">
+      <c r="K1" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="L1" s="38" t="s">
+      <c r="L1" s="36" t="s">
         <v>40</v>
       </c>
-      <c r="M1" s="38"/>
-      <c r="N1" s="38"/>
-      <c r="O1" s="38"/>
-      <c r="P1" s="38"/>
-      <c r="Q1" s="38"/>
-      <c r="R1" s="38"/>
+      <c r="M1" s="36"/>
+      <c r="N1" s="36"/>
+      <c r="O1" s="36"/>
+      <c r="P1" s="36"/>
+      <c r="Q1" s="36"/>
+      <c r="R1" s="36"/>
       <c r="S1" s="1"/>
       <c r="T1" s="1"/>
       <c r="U1" s="1"/>
@@ -860,8 +863,8 @@
       <c r="Z1" s="1"/>
     </row>
     <row r="2" spans="1:26" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="34"/>
-      <c r="B2" s="34"/>
+      <c r="A2" s="35"/>
+      <c r="B2" s="35"/>
       <c r="C2" s="3" t="s">
         <v>2</v>
       </c>
@@ -883,8 +886,8 @@
       <c r="I2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="J2" s="34"/>
-      <c r="K2" s="34"/>
+      <c r="J2" s="35"/>
+      <c r="K2" s="35"/>
       <c r="L2" s="3" t="s">
         <v>2</v>
       </c>
@@ -916,7 +919,7 @@
       <c r="Z2" s="1"/>
     </row>
     <row r="3" spans="1:26" ht="47.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="36" t="s">
+      <c r="A3" s="37" t="s">
         <v>13</v>
       </c>
       <c r="B3" s="4" t="s">
@@ -935,7 +938,7 @@
       <c r="I3" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="J3" s="36" t="s">
+      <c r="J3" s="37" t="s">
         <v>13</v>
       </c>
       <c r="K3" s="4" t="s">
@@ -964,7 +967,7 @@
       </c>
     </row>
     <row r="4" spans="1:26" ht="63" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="37"/>
+      <c r="A4" s="38"/>
       <c r="B4" s="4" t="s">
         <v>12</v>
       </c>
@@ -981,7 +984,7 @@
       <c r="I4" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="J4" s="37"/>
+      <c r="J4" s="38"/>
       <c r="K4" s="4" t="s">
         <v>12</v>
       </c>
@@ -1008,7 +1011,7 @@
       </c>
     </row>
     <row r="5" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="37"/>
+      <c r="A5" s="38"/>
       <c r="B5" s="4" t="s">
         <v>9</v>
       </c>
@@ -1025,7 +1028,7 @@
       <c r="I5" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="J5" s="37"/>
+      <c r="J5" s="38"/>
       <c r="K5" s="4" t="s">
         <v>9</v>
       </c>
@@ -1052,7 +1055,7 @@
       </c>
     </row>
     <row r="6" spans="1:26" ht="62.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="36" t="s">
+      <c r="A6" s="37" t="s">
         <v>14</v>
       </c>
       <c r="B6" s="4" t="s">
@@ -1071,7 +1074,7 @@
       <c r="I6" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="J6" s="36" t="s">
+      <c r="J6" s="37" t="s">
         <v>14</v>
       </c>
       <c r="K6" s="4" t="s">
@@ -1100,7 +1103,7 @@
       </c>
     </row>
     <row r="7" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="37"/>
+      <c r="A7" s="38"/>
       <c r="B7" s="4" t="s">
         <v>8</v>
       </c>
@@ -1117,7 +1120,7 @@
       <c r="I7" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="J7" s="37"/>
+      <c r="J7" s="38"/>
       <c r="K7" s="4" t="s">
         <v>8</v>
       </c>
@@ -1144,7 +1147,7 @@
       </c>
     </row>
     <row r="8" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="37"/>
+      <c r="A8" s="38"/>
       <c r="B8" s="4" t="s">
         <v>9</v>
       </c>
@@ -1161,7 +1164,7 @@
       <c r="I8" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="J8" s="37"/>
+      <c r="J8" s="38"/>
       <c r="K8" s="4" t="s">
         <v>9</v>
       </c>
@@ -1188,7 +1191,7 @@
       </c>
     </row>
     <row r="9" spans="1:26" ht="64.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="36" t="s">
+      <c r="A9" s="37" t="s">
         <v>15</v>
       </c>
       <c r="B9" s="4" t="s">
@@ -1207,7 +1210,7 @@
       <c r="I9" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="J9" s="36" t="s">
+      <c r="J9" s="37" t="s">
         <v>15</v>
       </c>
       <c r="K9" s="4" t="s">
@@ -1236,7 +1239,7 @@
       </c>
     </row>
     <row r="10" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="37"/>
+      <c r="A10" s="38"/>
       <c r="B10" s="4" t="s">
         <v>8</v>
       </c>
@@ -1253,7 +1256,7 @@
       <c r="I10" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="J10" s="37"/>
+      <c r="J10" s="38"/>
       <c r="K10" s="4" t="s">
         <v>8</v>
       </c>
@@ -1280,7 +1283,7 @@
       </c>
     </row>
     <row r="11" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="37"/>
+      <c r="A11" s="38"/>
       <c r="B11" s="4" t="s">
         <v>9</v>
       </c>
@@ -1297,7 +1300,7 @@
       <c r="I11" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="J11" s="37"/>
+      <c r="J11" s="38"/>
       <c r="K11" s="4" t="s">
         <v>9</v>
       </c>
@@ -1324,7 +1327,7 @@
       </c>
     </row>
     <row r="12" spans="1:26" ht="64.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="36" t="s">
+      <c r="A12" s="37" t="s">
         <v>16</v>
       </c>
       <c r="B12" s="4" t="s">
@@ -1343,7 +1346,7 @@
       <c r="I12" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="J12" s="36" t="s">
+      <c r="J12" s="37" t="s">
         <v>16</v>
       </c>
       <c r="K12" s="4" t="s">
@@ -1372,7 +1375,7 @@
       </c>
     </row>
     <row r="13" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="37"/>
+      <c r="A13" s="38"/>
       <c r="B13" s="4" t="s">
         <v>8</v>
       </c>
@@ -1389,7 +1392,7 @@
       <c r="I13" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="J13" s="37"/>
+      <c r="J13" s="38"/>
       <c r="K13" s="4" t="s">
         <v>8</v>
       </c>
@@ -1416,7 +1419,7 @@
       </c>
     </row>
     <row r="14" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="37"/>
+      <c r="A14" s="38"/>
       <c r="B14" s="4" t="s">
         <v>9</v>
       </c>
@@ -1433,7 +1436,7 @@
       <c r="I14" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="J14" s="37"/>
+      <c r="J14" s="38"/>
       <c r="K14" s="4" t="s">
         <v>9</v>
       </c>
@@ -1460,7 +1463,7 @@
       </c>
     </row>
     <row r="15" spans="1:26" ht="64.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="36" t="s">
+      <c r="A15" s="37" t="s">
         <v>17</v>
       </c>
       <c r="B15" s="4" t="s">
@@ -1479,7 +1482,7 @@
       <c r="I15" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="J15" s="36" t="s">
+      <c r="J15" s="37" t="s">
         <v>17</v>
       </c>
       <c r="K15" s="4" t="s">
@@ -1508,7 +1511,7 @@
       </c>
     </row>
     <row r="16" spans="1:26" ht="77.400000000000006" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="37"/>
+      <c r="A16" s="38"/>
       <c r="B16" s="4" t="s">
         <v>8</v>
       </c>
@@ -1525,7 +1528,7 @@
       <c r="I16" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="J16" s="37"/>
+      <c r="J16" s="38"/>
       <c r="K16" s="4" t="s">
         <v>8</v>
       </c>
@@ -1552,7 +1555,7 @@
       </c>
     </row>
     <row r="17" spans="1:18" ht="63.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="37"/>
+      <c r="A17" s="38"/>
       <c r="B17" s="4" t="s">
         <v>9</v>
       </c>
@@ -1569,7 +1572,7 @@
       <c r="I17" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="J17" s="37"/>
+      <c r="J17" s="38"/>
       <c r="K17" s="4" t="s">
         <v>9</v>
       </c>
@@ -5533,11 +5536,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="K1:K2"/>
-    <mergeCell ref="L1:R1"/>
-    <mergeCell ref="J3:J5"/>
-    <mergeCell ref="J6:J8"/>
-    <mergeCell ref="C1:I1"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="J15:J17"/>
@@ -5549,6 +5547,11 @@
     <mergeCell ref="A3:A5"/>
     <mergeCell ref="A6:A8"/>
     <mergeCell ref="A9:A11"/>
+    <mergeCell ref="K1:K2"/>
+    <mergeCell ref="L1:R1"/>
+    <mergeCell ref="J3:J5"/>
+    <mergeCell ref="J6:J8"/>
+    <mergeCell ref="C1:I1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -5582,24 +5585,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="33" t="s">
+      <c r="B1" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="33" t="s">
+      <c r="C1" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="38" t="s">
+      <c r="D1" s="36" t="s">
         <v>41</v>
       </c>
-      <c r="E1" s="38"/>
-      <c r="F1" s="38"/>
-      <c r="G1" s="38"/>
-      <c r="H1" s="38"/>
-      <c r="I1" s="38"/>
-      <c r="J1" s="38"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
+      <c r="I1" s="36"/>
+      <c r="J1" s="36"/>
       <c r="S1" s="1"/>
       <c r="T1" s="1"/>
       <c r="U1" s="1"/>
@@ -5610,9 +5613,9 @@
       <c r="Z1" s="1"/>
     </row>
     <row r="2" spans="1:26" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="34"/>
-      <c r="B2" s="34"/>
-      <c r="C2" s="34"/>
+      <c r="A2" s="35"/>
+      <c r="B2" s="35"/>
+      <c r="C2" s="35"/>
       <c r="D2" s="3" t="s">
         <v>2</v>
       </c>
@@ -5644,7 +5647,7 @@
       <c r="Z2" s="1"/>
     </row>
     <row r="3" spans="1:26" ht="47.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="36" t="s">
+      <c r="A3" s="37" t="s">
         <v>13</v>
       </c>
       <c r="B3" s="4" t="s">
@@ -5676,7 +5679,7 @@
       </c>
     </row>
     <row r="4" spans="1:26" ht="63" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="37"/>
+      <c r="A4" s="38"/>
       <c r="B4" s="4" t="s">
         <v>12</v>
       </c>
@@ -5706,7 +5709,7 @@
       </c>
     </row>
     <row r="5" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="37"/>
+      <c r="A5" s="38"/>
       <c r="B5" s="4" t="s">
         <v>9</v>
       </c>
@@ -5736,7 +5739,7 @@
       </c>
     </row>
     <row r="6" spans="1:26" ht="62.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="36" t="s">
+      <c r="A6" s="37" t="s">
         <v>14</v>
       </c>
       <c r="B6" s="4" t="s">
@@ -5768,7 +5771,7 @@
       </c>
     </row>
     <row r="7" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="37"/>
+      <c r="A7" s="38"/>
       <c r="B7" s="4" t="s">
         <v>8</v>
       </c>
@@ -5798,7 +5801,7 @@
       </c>
     </row>
     <row r="8" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="37"/>
+      <c r="A8" s="38"/>
       <c r="B8" s="4" t="s">
         <v>9</v>
       </c>
@@ -5828,7 +5831,7 @@
       </c>
     </row>
     <row r="9" spans="1:26" ht="64.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="36" t="s">
+      <c r="A9" s="37" t="s">
         <v>15</v>
       </c>
       <c r="B9" s="4" t="s">
@@ -5860,7 +5863,7 @@
       </c>
     </row>
     <row r="10" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="37"/>
+      <c r="A10" s="38"/>
       <c r="B10" s="4" t="s">
         <v>8</v>
       </c>
@@ -5890,7 +5893,7 @@
       </c>
     </row>
     <row r="11" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="37"/>
+      <c r="A11" s="38"/>
       <c r="B11" s="4" t="s">
         <v>9</v>
       </c>
@@ -5920,7 +5923,7 @@
       </c>
     </row>
     <row r="12" spans="1:26" ht="64.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="36" t="s">
+      <c r="A12" s="37" t="s">
         <v>16</v>
       </c>
       <c r="B12" s="4" t="s">
@@ -5952,7 +5955,7 @@
       </c>
     </row>
     <row r="13" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="37"/>
+      <c r="A13" s="38"/>
       <c r="B13" s="4" t="s">
         <v>8</v>
       </c>
@@ -5982,7 +5985,7 @@
       </c>
     </row>
     <row r="14" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="37"/>
+      <c r="A14" s="38"/>
       <c r="B14" s="4" t="s">
         <v>9</v>
       </c>
@@ -6012,7 +6015,7 @@
       </c>
     </row>
     <row r="15" spans="1:26" ht="64.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="36" t="s">
+      <c r="A15" s="37" t="s">
         <v>17</v>
       </c>
       <c r="B15" s="4" t="s">
@@ -6044,7 +6047,7 @@
       </c>
     </row>
     <row r="16" spans="1:26" ht="77.400000000000006" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="37"/>
+      <c r="A16" s="38"/>
       <c r="B16" s="4" t="s">
         <v>8</v>
       </c>
@@ -6074,7 +6077,7 @@
       </c>
     </row>
     <row r="17" spans="1:10" ht="63.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="37"/>
+      <c r="A17" s="38"/>
       <c r="B17" s="4" t="s">
         <v>9</v>
       </c>
@@ -10070,25 +10073,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="18" x14ac:dyDescent="0.4">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="42" t="s">
+      <c r="B1" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="41" t="s">
+      <c r="C1" s="42" t="s">
         <v>42</v>
       </c>
-      <c r="D1" s="41"/>
-      <c r="E1" s="41"/>
-      <c r="F1" s="41"/>
-      <c r="G1" s="41"/>
-      <c r="H1" s="41"/>
-      <c r="I1" s="41"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="42"/>
+      <c r="F1" s="42"/>
+      <c r="G1" s="42"/>
+      <c r="H1" s="42"/>
+      <c r="I1" s="42"/>
     </row>
     <row r="2" spans="1:9" ht="18" x14ac:dyDescent="0.4">
-      <c r="A2" s="43"/>
-      <c r="B2" s="43"/>
+      <c r="A2" s="44"/>
+      <c r="B2" s="44"/>
       <c r="C2" s="14" t="s">
         <v>2</v>
       </c>
@@ -10112,7 +10115,7 @@
       </c>
     </row>
     <row r="3" spans="1:9" ht="87.5" x14ac:dyDescent="0.35">
-      <c r="A3" s="39" t="s">
+      <c r="A3" s="40" t="s">
         <v>13</v>
       </c>
       <c r="B3" s="15" t="s">
@@ -10141,7 +10144,7 @@
       </c>
     </row>
     <row r="4" spans="1:9" ht="105" x14ac:dyDescent="0.35">
-      <c r="A4" s="40"/>
+      <c r="A4" s="41"/>
       <c r="B4" s="15" t="s">
         <v>12</v>
       </c>
@@ -10168,7 +10171,7 @@
       </c>
     </row>
     <row r="5" spans="1:9" ht="52.5" x14ac:dyDescent="0.35">
-      <c r="A5" s="40"/>
+      <c r="A5" s="41"/>
       <c r="B5" s="15" t="s">
         <v>9</v>
       </c>
@@ -10195,7 +10198,7 @@
       </c>
     </row>
     <row r="6" spans="1:9" ht="157.5" x14ac:dyDescent="0.35">
-      <c r="A6" s="39" t="s">
+      <c r="A6" s="40" t="s">
         <v>14</v>
       </c>
       <c r="B6" s="15" t="s">
@@ -10224,7 +10227,7 @@
       </c>
     </row>
     <row r="7" spans="1:9" ht="157.5" x14ac:dyDescent="0.35">
-      <c r="A7" s="40"/>
+      <c r="A7" s="41"/>
       <c r="B7" s="15" t="s">
         <v>8</v>
       </c>
@@ -10251,7 +10254,7 @@
       </c>
     </row>
     <row r="8" spans="1:9" ht="70" x14ac:dyDescent="0.35">
-      <c r="A8" s="40"/>
+      <c r="A8" s="41"/>
       <c r="B8" s="15" t="s">
         <v>9</v>
       </c>
@@ -10278,7 +10281,7 @@
       </c>
     </row>
     <row r="9" spans="1:9" ht="140" x14ac:dyDescent="0.35">
-      <c r="A9" s="39" t="s">
+      <c r="A9" s="40" t="s">
         <v>15</v>
       </c>
       <c r="B9" s="15" t="s">
@@ -10307,7 +10310,7 @@
       </c>
     </row>
     <row r="10" spans="1:9" ht="157.5" x14ac:dyDescent="0.35">
-      <c r="A10" s="40"/>
+      <c r="A10" s="41"/>
       <c r="B10" s="15" t="s">
         <v>8</v>
       </c>
@@ -10334,7 +10337,7 @@
       </c>
     </row>
     <row r="11" spans="1:9" ht="70" x14ac:dyDescent="0.35">
-      <c r="A11" s="40"/>
+      <c r="A11" s="41"/>
       <c r="B11" s="15" t="s">
         <v>9</v>
       </c>
@@ -10361,7 +10364,7 @@
       </c>
     </row>
     <row r="12" spans="1:9" ht="157.5" x14ac:dyDescent="0.35">
-      <c r="A12" s="39" t="s">
+      <c r="A12" s="40" t="s">
         <v>16</v>
       </c>
       <c r="B12" s="15" t="s">
@@ -10390,7 +10393,7 @@
       </c>
     </row>
     <row r="13" spans="1:9" ht="157.5" x14ac:dyDescent="0.35">
-      <c r="A13" s="40"/>
+      <c r="A13" s="41"/>
       <c r="B13" s="15" t="s">
         <v>8</v>
       </c>
@@ -10417,7 +10420,7 @@
       </c>
     </row>
     <row r="14" spans="1:9" ht="175" x14ac:dyDescent="0.35">
-      <c r="A14" s="40"/>
+      <c r="A14" s="41"/>
       <c r="B14" s="15" t="s">
         <v>9</v>
       </c>
@@ -10444,7 +10447,7 @@
       </c>
     </row>
     <row r="15" spans="1:9" ht="105" x14ac:dyDescent="0.35">
-      <c r="A15" s="39" t="s">
+      <c r="A15" s="40" t="s">
         <v>17</v>
       </c>
       <c r="B15" s="15" t="s">
@@ -10473,7 +10476,7 @@
       </c>
     </row>
     <row r="16" spans="1:9" ht="157.5" x14ac:dyDescent="0.35">
-      <c r="A16" s="40"/>
+      <c r="A16" s="41"/>
       <c r="B16" s="15" t="s">
         <v>8</v>
       </c>
@@ -10500,7 +10503,7 @@
       </c>
     </row>
     <row r="17" spans="1:9" ht="70" x14ac:dyDescent="0.35">
-      <c r="A17" s="40"/>
+      <c r="A17" s="41"/>
       <c r="B17" s="15" t="s">
         <v>9</v>
       </c>
@@ -10561,25 +10564,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="18" x14ac:dyDescent="0.4">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="42" t="s">
+      <c r="B1" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="41" t="s">
+      <c r="C1" s="42" t="s">
         <v>64</v>
       </c>
-      <c r="D1" s="41"/>
-      <c r="E1" s="41"/>
-      <c r="F1" s="41"/>
-      <c r="G1" s="41"/>
-      <c r="H1" s="41"/>
-      <c r="I1" s="41"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="42"/>
+      <c r="F1" s="42"/>
+      <c r="G1" s="42"/>
+      <c r="H1" s="42"/>
+      <c r="I1" s="42"/>
     </row>
     <row r="2" spans="1:9" ht="18" x14ac:dyDescent="0.4">
-      <c r="A2" s="43"/>
-      <c r="B2" s="43"/>
+      <c r="A2" s="44"/>
+      <c r="B2" s="44"/>
       <c r="C2" s="14" t="s">
         <v>2</v>
       </c>
@@ -10603,7 +10606,7 @@
       </c>
     </row>
     <row r="3" spans="1:9" ht="105" x14ac:dyDescent="0.35">
-      <c r="A3" s="39" t="s">
+      <c r="A3" s="40" t="s">
         <v>13</v>
       </c>
       <c r="B3" s="21" t="s">
@@ -10632,7 +10635,7 @@
       </c>
     </row>
     <row r="4" spans="1:9" ht="105" x14ac:dyDescent="0.35">
-      <c r="A4" s="40"/>
+      <c r="A4" s="41"/>
       <c r="B4" s="21" t="s">
         <v>12</v>
       </c>
@@ -10659,7 +10662,7 @@
       </c>
     </row>
     <row r="5" spans="1:9" ht="87.5" x14ac:dyDescent="0.35">
-      <c r="A5" s="40"/>
+      <c r="A5" s="41"/>
       <c r="B5" s="21" t="s">
         <v>9</v>
       </c>
@@ -10686,7 +10689,7 @@
       </c>
     </row>
     <row r="6" spans="1:9" ht="122.5" x14ac:dyDescent="0.35">
-      <c r="A6" s="39" t="s">
+      <c r="A6" s="40" t="s">
         <v>14</v>
       </c>
       <c r="B6" s="21" t="s">
@@ -10715,7 +10718,7 @@
       </c>
     </row>
     <row r="7" spans="1:9" ht="105" x14ac:dyDescent="0.35">
-      <c r="A7" s="40"/>
+      <c r="A7" s="41"/>
       <c r="B7" s="21" t="s">
         <v>8</v>
       </c>
@@ -10742,7 +10745,7 @@
       </c>
     </row>
     <row r="8" spans="1:9" ht="105" x14ac:dyDescent="0.35">
-      <c r="A8" s="40"/>
+      <c r="A8" s="41"/>
       <c r="B8" s="21" t="s">
         <v>9</v>
       </c>
@@ -10769,7 +10772,7 @@
       </c>
     </row>
     <row r="9" spans="1:9" ht="70" x14ac:dyDescent="0.35">
-      <c r="A9" s="39" t="s">
+      <c r="A9" s="40" t="s">
         <v>15</v>
       </c>
       <c r="B9" s="21" t="s">
@@ -10798,7 +10801,7 @@
       </c>
     </row>
     <row r="10" spans="1:9" ht="52.5" x14ac:dyDescent="0.35">
-      <c r="A10" s="40"/>
+      <c r="A10" s="41"/>
       <c r="B10" s="21" t="s">
         <v>8</v>
       </c>
@@ -10825,7 +10828,7 @@
       </c>
     </row>
     <row r="11" spans="1:9" ht="157.5" x14ac:dyDescent="0.35">
-      <c r="A11" s="40"/>
+      <c r="A11" s="41"/>
       <c r="B11" s="21" t="s">
         <v>9</v>
       </c>
@@ -10852,7 +10855,7 @@
       </c>
     </row>
     <row r="12" spans="1:9" ht="192.5" x14ac:dyDescent="0.35">
-      <c r="A12" s="39" t="s">
+      <c r="A12" s="40" t="s">
         <v>16</v>
       </c>
       <c r="B12" s="21" t="s">
@@ -10881,7 +10884,7 @@
       </c>
     </row>
     <row r="13" spans="1:9" ht="192.5" x14ac:dyDescent="0.35">
-      <c r="A13" s="40"/>
+      <c r="A13" s="41"/>
       <c r="B13" s="21" t="s">
         <v>8</v>
       </c>
@@ -10908,7 +10911,7 @@
       </c>
     </row>
     <row r="14" spans="1:9" ht="87.5" x14ac:dyDescent="0.35">
-      <c r="A14" s="40"/>
+      <c r="A14" s="41"/>
       <c r="B14" s="21" t="s">
         <v>9</v>
       </c>
@@ -10935,7 +10938,7 @@
       </c>
     </row>
     <row r="15" spans="1:9" ht="70" x14ac:dyDescent="0.35">
-      <c r="A15" s="39" t="s">
+      <c r="A15" s="40" t="s">
         <v>17</v>
       </c>
       <c r="B15" s="21" t="s">
@@ -10964,7 +10967,7 @@
       </c>
     </row>
     <row r="16" spans="1:9" ht="52.5" x14ac:dyDescent="0.35">
-      <c r="A16" s="40"/>
+      <c r="A16" s="41"/>
       <c r="B16" s="21" t="s">
         <v>8</v>
       </c>
@@ -10991,7 +10994,7 @@
       </c>
     </row>
     <row r="17" spans="1:9" ht="157.5" x14ac:dyDescent="0.35">
-      <c r="A17" s="40"/>
+      <c r="A17" s="41"/>
       <c r="B17" s="21" t="s">
         <v>9</v>
       </c>
@@ -11037,8 +11040,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B762D8C-72F3-45B7-9544-A442629D54B9}">
   <dimension ref="A1:I17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.453125" defaultRowHeight="17.5" x14ac:dyDescent="0.35"/>
@@ -11054,25 +11057,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="18" x14ac:dyDescent="0.4">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="42" t="s">
+      <c r="B1" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="41" t="s">
+      <c r="C1" s="42" t="s">
         <v>64</v>
       </c>
-      <c r="D1" s="41"/>
-      <c r="E1" s="41"/>
-      <c r="F1" s="41"/>
-      <c r="G1" s="41"/>
-      <c r="H1" s="41"/>
-      <c r="I1" s="41"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="42"/>
+      <c r="F1" s="42"/>
+      <c r="G1" s="42"/>
+      <c r="H1" s="42"/>
+      <c r="I1" s="42"/>
     </row>
     <row r="2" spans="1:9" ht="18" x14ac:dyDescent="0.4">
-      <c r="A2" s="43"/>
-      <c r="B2" s="43"/>
+      <c r="A2" s="44"/>
+      <c r="B2" s="44"/>
       <c r="C2" s="14" t="s">
         <v>2</v>
       </c>
@@ -11096,7 +11099,7 @@
       </c>
     </row>
     <row r="3" spans="1:9" ht="192.5" x14ac:dyDescent="0.35">
-      <c r="A3" s="39" t="s">
+      <c r="A3" s="40" t="s">
         <v>13</v>
       </c>
       <c r="B3" s="23" t="s">
@@ -11114,12 +11117,14 @@
       <c r="F3" s="25" t="s">
         <v>81</v>
       </c>
-      <c r="G3" s="25"/>
+      <c r="G3" s="25" t="s">
+        <v>84</v>
+      </c>
       <c r="H3" s="25"/>
       <c r="I3" s="26"/>
     </row>
     <row r="4" spans="1:9" ht="140" x14ac:dyDescent="0.35">
-      <c r="A4" s="40"/>
+      <c r="A4" s="41"/>
       <c r="B4" s="23" t="s">
         <v>12</v>
       </c>
@@ -11135,12 +11140,14 @@
       <c r="F4" s="25" t="s">
         <v>84</v>
       </c>
-      <c r="G4" s="25"/>
+      <c r="G4" s="25" t="s">
+        <v>55</v>
+      </c>
       <c r="H4" s="26"/>
       <c r="I4" s="25"/>
     </row>
     <row r="5" spans="1:9" ht="52.5" x14ac:dyDescent="0.35">
-      <c r="A5" s="40"/>
+      <c r="A5" s="41"/>
       <c r="B5" s="23" t="s">
         <v>9</v>
       </c>
@@ -11156,11 +11163,13 @@
       <c r="F5" s="31" t="s">
         <v>30</v>
       </c>
-      <c r="G5" s="25"/>
+      <c r="G5" s="31" t="s">
+        <v>30</v>
+      </c>
       <c r="H5" s="25"/>
     </row>
     <row r="6" spans="1:9" ht="192.5" x14ac:dyDescent="0.35">
-      <c r="A6" s="39" t="s">
+      <c r="A6" s="40" t="s">
         <v>14</v>
       </c>
       <c r="B6" s="23" t="s">
@@ -11178,12 +11187,14 @@
       <c r="F6" s="25" t="s">
         <v>81</v>
       </c>
-      <c r="G6" s="25"/>
+      <c r="G6" s="25" t="s">
+        <v>85</v>
+      </c>
       <c r="H6" s="25"/>
       <c r="I6" s="26"/>
     </row>
     <row r="7" spans="1:9" ht="140" x14ac:dyDescent="0.35">
-      <c r="A7" s="40"/>
+      <c r="A7" s="41"/>
       <c r="B7" s="23" t="s">
         <v>8</v>
       </c>
@@ -11199,12 +11210,14 @@
       <c r="F7" s="25" t="s">
         <v>85</v>
       </c>
-      <c r="G7" s="25"/>
+      <c r="G7" s="25" t="s">
+        <v>55</v>
+      </c>
       <c r="H7" s="26"/>
       <c r="I7" s="25"/>
     </row>
     <row r="8" spans="1:9" ht="52.5" x14ac:dyDescent="0.35">
-      <c r="A8" s="40"/>
+      <c r="A8" s="41"/>
       <c r="B8" s="23" t="s">
         <v>9</v>
       </c>
@@ -11220,11 +11233,13 @@
       <c r="F8" s="31" t="s">
         <v>30</v>
       </c>
-      <c r="G8" s="25"/>
+      <c r="G8" s="31" t="s">
+        <v>30</v>
+      </c>
       <c r="H8" s="25"/>
     </row>
-    <row r="9" spans="1:9" ht="35" x14ac:dyDescent="0.35">
-      <c r="A9" s="39" t="s">
+    <row r="9" spans="1:9" ht="157.5" x14ac:dyDescent="0.35">
+      <c r="A9" s="40" t="s">
         <v>15</v>
       </c>
       <c r="B9" s="23" t="s">
@@ -11242,11 +11257,14 @@
       <c r="F9" s="25" t="s">
         <v>81</v>
       </c>
+      <c r="G9" s="33" t="s">
+        <v>88</v>
+      </c>
       <c r="H9" s="25"/>
       <c r="I9" s="25"/>
     </row>
     <row r="10" spans="1:9" ht="140" x14ac:dyDescent="0.35">
-      <c r="A10" s="40"/>
+      <c r="A10" s="41"/>
       <c r="B10" s="23" t="s">
         <v>8</v>
       </c>
@@ -11262,12 +11280,14 @@
       <c r="F10" s="32" t="s">
         <v>88</v>
       </c>
-      <c r="G10" s="25"/>
+      <c r="G10" s="25" t="s">
+        <v>55</v>
+      </c>
       <c r="H10" s="25"/>
       <c r="I10" s="25"/>
     </row>
     <row r="11" spans="1:9" ht="52.5" x14ac:dyDescent="0.35">
-      <c r="A11" s="40"/>
+      <c r="A11" s="41"/>
       <c r="B11" s="23" t="s">
         <v>9</v>
       </c>
@@ -11283,12 +11303,14 @@
       <c r="F11" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="G11" s="25"/>
+      <c r="G11" s="25" t="s">
+        <v>30</v>
+      </c>
       <c r="H11" s="25"/>
       <c r="I11" s="25"/>
     </row>
     <row r="12" spans="1:9" ht="192.5" x14ac:dyDescent="0.35">
-      <c r="A12" s="39" t="s">
+      <c r="A12" s="40" t="s">
         <v>16</v>
       </c>
       <c r="B12" s="23" t="s">
@@ -11306,12 +11328,14 @@
       <c r="F12" s="25" t="s">
         <v>83</v>
       </c>
-      <c r="G12" s="25"/>
+      <c r="G12" s="25" t="s">
+        <v>86</v>
+      </c>
       <c r="H12" s="25"/>
       <c r="I12" s="26"/>
     </row>
     <row r="13" spans="1:9" ht="140" x14ac:dyDescent="0.35">
-      <c r="A13" s="40"/>
+      <c r="A13" s="41"/>
       <c r="B13" s="23" t="s">
         <v>8</v>
       </c>
@@ -11327,12 +11351,14 @@
       <c r="F13" s="25" t="s">
         <v>86</v>
       </c>
-      <c r="G13" s="25"/>
+      <c r="G13" s="25" t="s">
+        <v>55</v>
+      </c>
       <c r="H13" s="26"/>
       <c r="I13" s="25"/>
     </row>
     <row r="14" spans="1:9" ht="52.5" x14ac:dyDescent="0.35">
-      <c r="A14" s="40"/>
+      <c r="A14" s="41"/>
       <c r="B14" s="23" t="s">
         <v>9</v>
       </c>
@@ -11348,10 +11374,13 @@
       <c r="F14" s="24" t="s">
         <v>30</v>
       </c>
+      <c r="G14" s="33" t="s">
+        <v>30</v>
+      </c>
       <c r="H14" s="25"/>
     </row>
-    <row r="15" spans="1:9" ht="35" x14ac:dyDescent="0.35">
-      <c r="A15" s="39" t="s">
+    <row r="15" spans="1:9" ht="192.5" x14ac:dyDescent="0.35">
+      <c r="A15" s="40" t="s">
         <v>17</v>
       </c>
       <c r="B15" s="23" t="s">
@@ -11369,11 +11398,14 @@
       <c r="F15" s="25" t="s">
         <v>81</v>
       </c>
+      <c r="G15" s="33" t="s">
+        <v>87</v>
+      </c>
       <c r="H15" s="25"/>
       <c r="I15" s="25"/>
     </row>
     <row r="16" spans="1:9" ht="157.5" x14ac:dyDescent="0.35">
-      <c r="A16" s="40"/>
+      <c r="A16" s="41"/>
       <c r="B16" s="23" t="s">
         <v>8</v>
       </c>
@@ -11389,12 +11421,14 @@
       <c r="F16" s="24" t="s">
         <v>87</v>
       </c>
-      <c r="G16" s="25"/>
+      <c r="G16" s="25" t="s">
+        <v>55</v>
+      </c>
       <c r="H16" s="25"/>
       <c r="I16" s="25"/>
     </row>
     <row r="17" spans="1:9" ht="52.5" x14ac:dyDescent="0.35">
-      <c r="A17" s="40"/>
+      <c r="A17" s="41"/>
       <c r="B17" s="23" t="s">
         <v>9</v>
       </c>
@@ -11410,7 +11444,9 @@
       <c r="F17" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="G17" s="25"/>
+      <c r="G17" s="25" t="s">
+        <v>30</v>
+      </c>
       <c r="H17" s="25"/>
       <c r="I17" s="25"/>
     </row>

</xml_diff>

<commit_message>
updated ud (week9 sat)
</commit_message>
<xml_diff>
--- a/metrics/du.xlsx
+++ b/metrics/du.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\project-g4t6\metrics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{806B8C6D-7CAA-42D2-AE1F-500B333F5EF6}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D168C13-83F3-4961-AAAB-3B65CF7ABE57}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="736" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="751" uniqueCount="89">
   <si>
     <t>Question</t>
   </si>
@@ -388,7 +388,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -483,19 +483,22 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -823,36 +826,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="39" t="s">
+      <c r="A1" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="34" t="s">
+      <c r="B1" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="36" t="s">
+      <c r="C1" s="40" t="s">
         <v>18</v>
       </c>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
-      <c r="F1" s="36"/>
-      <c r="G1" s="36"/>
-      <c r="H1" s="36"/>
-      <c r="I1" s="36"/>
-      <c r="J1" s="39" t="s">
+      <c r="D1" s="40"/>
+      <c r="E1" s="40"/>
+      <c r="F1" s="40"/>
+      <c r="G1" s="40"/>
+      <c r="H1" s="40"/>
+      <c r="I1" s="40"/>
+      <c r="J1" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="K1" s="34" t="s">
+      <c r="K1" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="L1" s="36" t="s">
+      <c r="L1" s="40" t="s">
         <v>40</v>
       </c>
-      <c r="M1" s="36"/>
-      <c r="N1" s="36"/>
-      <c r="O1" s="36"/>
-      <c r="P1" s="36"/>
-      <c r="Q1" s="36"/>
-      <c r="R1" s="36"/>
+      <c r="M1" s="40"/>
+      <c r="N1" s="40"/>
+      <c r="O1" s="40"/>
+      <c r="P1" s="40"/>
+      <c r="Q1" s="40"/>
+      <c r="R1" s="40"/>
       <c r="S1" s="1"/>
       <c r="T1" s="1"/>
       <c r="U1" s="1"/>
@@ -863,8 +866,8 @@
       <c r="Z1" s="1"/>
     </row>
     <row r="2" spans="1:26" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="35"/>
-      <c r="B2" s="35"/>
+      <c r="A2" s="36"/>
+      <c r="B2" s="36"/>
       <c r="C2" s="3" t="s">
         <v>2</v>
       </c>
@@ -886,8 +889,8 @@
       <c r="I2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="J2" s="35"/>
-      <c r="K2" s="35"/>
+      <c r="J2" s="36"/>
+      <c r="K2" s="36"/>
       <c r="L2" s="3" t="s">
         <v>2</v>
       </c>
@@ -919,7 +922,7 @@
       <c r="Z2" s="1"/>
     </row>
     <row r="3" spans="1:26" ht="47.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="37" t="s">
+      <c r="A3" s="38" t="s">
         <v>13</v>
       </c>
       <c r="B3" s="4" t="s">
@@ -938,7 +941,7 @@
       <c r="I3" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="J3" s="37" t="s">
+      <c r="J3" s="38" t="s">
         <v>13</v>
       </c>
       <c r="K3" s="4" t="s">
@@ -967,7 +970,7 @@
       </c>
     </row>
     <row r="4" spans="1:26" ht="63" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="38"/>
+      <c r="A4" s="39"/>
       <c r="B4" s="4" t="s">
         <v>12</v>
       </c>
@@ -984,7 +987,7 @@
       <c r="I4" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="J4" s="38"/>
+      <c r="J4" s="39"/>
       <c r="K4" s="4" t="s">
         <v>12</v>
       </c>
@@ -1011,7 +1014,7 @@
       </c>
     </row>
     <row r="5" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="38"/>
+      <c r="A5" s="39"/>
       <c r="B5" s="4" t="s">
         <v>9</v>
       </c>
@@ -1028,7 +1031,7 @@
       <c r="I5" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="J5" s="38"/>
+      <c r="J5" s="39"/>
       <c r="K5" s="4" t="s">
         <v>9</v>
       </c>
@@ -1055,7 +1058,7 @@
       </c>
     </row>
     <row r="6" spans="1:26" ht="62.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="37" t="s">
+      <c r="A6" s="38" t="s">
         <v>14</v>
       </c>
       <c r="B6" s="4" t="s">
@@ -1074,7 +1077,7 @@
       <c r="I6" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="J6" s="37" t="s">
+      <c r="J6" s="38" t="s">
         <v>14</v>
       </c>
       <c r="K6" s="4" t="s">
@@ -1103,7 +1106,7 @@
       </c>
     </row>
     <row r="7" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="38"/>
+      <c r="A7" s="39"/>
       <c r="B7" s="4" t="s">
         <v>8</v>
       </c>
@@ -1120,7 +1123,7 @@
       <c r="I7" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="J7" s="38"/>
+      <c r="J7" s="39"/>
       <c r="K7" s="4" t="s">
         <v>8</v>
       </c>
@@ -1147,7 +1150,7 @@
       </c>
     </row>
     <row r="8" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="38"/>
+      <c r="A8" s="39"/>
       <c r="B8" s="4" t="s">
         <v>9</v>
       </c>
@@ -1164,7 +1167,7 @@
       <c r="I8" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="J8" s="38"/>
+      <c r="J8" s="39"/>
       <c r="K8" s="4" t="s">
         <v>9</v>
       </c>
@@ -1191,7 +1194,7 @@
       </c>
     </row>
     <row r="9" spans="1:26" ht="64.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="37" t="s">
+      <c r="A9" s="38" t="s">
         <v>15</v>
       </c>
       <c r="B9" s="4" t="s">
@@ -1210,7 +1213,7 @@
       <c r="I9" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="J9" s="37" t="s">
+      <c r="J9" s="38" t="s">
         <v>15</v>
       </c>
       <c r="K9" s="4" t="s">
@@ -1239,7 +1242,7 @@
       </c>
     </row>
     <row r="10" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="38"/>
+      <c r="A10" s="39"/>
       <c r="B10" s="4" t="s">
         <v>8</v>
       </c>
@@ -1256,7 +1259,7 @@
       <c r="I10" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="J10" s="38"/>
+      <c r="J10" s="39"/>
       <c r="K10" s="4" t="s">
         <v>8</v>
       </c>
@@ -1283,7 +1286,7 @@
       </c>
     </row>
     <row r="11" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="38"/>
+      <c r="A11" s="39"/>
       <c r="B11" s="4" t="s">
         <v>9</v>
       </c>
@@ -1300,7 +1303,7 @@
       <c r="I11" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="J11" s="38"/>
+      <c r="J11" s="39"/>
       <c r="K11" s="4" t="s">
         <v>9</v>
       </c>
@@ -1327,7 +1330,7 @@
       </c>
     </row>
     <row r="12" spans="1:26" ht="64.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="37" t="s">
+      <c r="A12" s="38" t="s">
         <v>16</v>
       </c>
       <c r="B12" s="4" t="s">
@@ -1346,7 +1349,7 @@
       <c r="I12" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="J12" s="37" t="s">
+      <c r="J12" s="38" t="s">
         <v>16</v>
       </c>
       <c r="K12" s="4" t="s">
@@ -1375,7 +1378,7 @@
       </c>
     </row>
     <row r="13" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="38"/>
+      <c r="A13" s="39"/>
       <c r="B13" s="4" t="s">
         <v>8</v>
       </c>
@@ -1392,7 +1395,7 @@
       <c r="I13" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="J13" s="38"/>
+      <c r="J13" s="39"/>
       <c r="K13" s="4" t="s">
         <v>8</v>
       </c>
@@ -1419,7 +1422,7 @@
       </c>
     </row>
     <row r="14" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="38"/>
+      <c r="A14" s="39"/>
       <c r="B14" s="4" t="s">
         <v>9</v>
       </c>
@@ -1436,7 +1439,7 @@
       <c r="I14" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="J14" s="38"/>
+      <c r="J14" s="39"/>
       <c r="K14" s="4" t="s">
         <v>9</v>
       </c>
@@ -1463,7 +1466,7 @@
       </c>
     </row>
     <row r="15" spans="1:26" ht="64.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="37" t="s">
+      <c r="A15" s="38" t="s">
         <v>17</v>
       </c>
       <c r="B15" s="4" t="s">
@@ -1482,7 +1485,7 @@
       <c r="I15" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="J15" s="37" t="s">
+      <c r="J15" s="38" t="s">
         <v>17</v>
       </c>
       <c r="K15" s="4" t="s">
@@ -1511,7 +1514,7 @@
       </c>
     </row>
     <row r="16" spans="1:26" ht="77.400000000000006" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="38"/>
+      <c r="A16" s="39"/>
       <c r="B16" s="4" t="s">
         <v>8</v>
       </c>
@@ -1528,7 +1531,7 @@
       <c r="I16" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="J16" s="38"/>
+      <c r="J16" s="39"/>
       <c r="K16" s="4" t="s">
         <v>8</v>
       </c>
@@ -1555,7 +1558,7 @@
       </c>
     </row>
     <row r="17" spans="1:18" ht="63.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="38"/>
+      <c r="A17" s="39"/>
       <c r="B17" s="4" t="s">
         <v>9</v>
       </c>
@@ -1572,7 +1575,7 @@
       <c r="I17" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="J17" s="38"/>
+      <c r="J17" s="39"/>
       <c r="K17" s="4" t="s">
         <v>9</v>
       </c>
@@ -5536,6 +5539,11 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="K1:K2"/>
+    <mergeCell ref="L1:R1"/>
+    <mergeCell ref="J3:J5"/>
+    <mergeCell ref="J6:J8"/>
+    <mergeCell ref="C1:I1"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="J15:J17"/>
@@ -5547,11 +5555,6 @@
     <mergeCell ref="A3:A5"/>
     <mergeCell ref="A6:A8"/>
     <mergeCell ref="A9:A11"/>
-    <mergeCell ref="K1:K2"/>
-    <mergeCell ref="L1:R1"/>
-    <mergeCell ref="J3:J5"/>
-    <mergeCell ref="J6:J8"/>
-    <mergeCell ref="C1:I1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -5585,24 +5588,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="39" t="s">
+      <c r="A1" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="34" t="s">
+      <c r="B1" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="34" t="s">
+      <c r="C1" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="36" t="s">
+      <c r="D1" s="40" t="s">
         <v>41</v>
       </c>
-      <c r="E1" s="36"/>
-      <c r="F1" s="36"/>
-      <c r="G1" s="36"/>
-      <c r="H1" s="36"/>
-      <c r="I1" s="36"/>
-      <c r="J1" s="36"/>
+      <c r="E1" s="40"/>
+      <c r="F1" s="40"/>
+      <c r="G1" s="40"/>
+      <c r="H1" s="40"/>
+      <c r="I1" s="40"/>
+      <c r="J1" s="40"/>
       <c r="S1" s="1"/>
       <c r="T1" s="1"/>
       <c r="U1" s="1"/>
@@ -5613,9 +5616,9 @@
       <c r="Z1" s="1"/>
     </row>
     <row r="2" spans="1:26" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="35"/>
-      <c r="B2" s="35"/>
-      <c r="C2" s="35"/>
+      <c r="A2" s="36"/>
+      <c r="B2" s="36"/>
+      <c r="C2" s="36"/>
       <c r="D2" s="3" t="s">
         <v>2</v>
       </c>
@@ -5647,7 +5650,7 @@
       <c r="Z2" s="1"/>
     </row>
     <row r="3" spans="1:26" ht="47.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="37" t="s">
+      <c r="A3" s="38" t="s">
         <v>13</v>
       </c>
       <c r="B3" s="4" t="s">
@@ -5679,7 +5682,7 @@
       </c>
     </row>
     <row r="4" spans="1:26" ht="63" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="38"/>
+      <c r="A4" s="39"/>
       <c r="B4" s="4" t="s">
         <v>12</v>
       </c>
@@ -5709,7 +5712,7 @@
       </c>
     </row>
     <row r="5" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="38"/>
+      <c r="A5" s="39"/>
       <c r="B5" s="4" t="s">
         <v>9</v>
       </c>
@@ -5739,7 +5742,7 @@
       </c>
     </row>
     <row r="6" spans="1:26" ht="62.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="37" t="s">
+      <c r="A6" s="38" t="s">
         <v>14</v>
       </c>
       <c r="B6" s="4" t="s">
@@ -5771,7 +5774,7 @@
       </c>
     </row>
     <row r="7" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="38"/>
+      <c r="A7" s="39"/>
       <c r="B7" s="4" t="s">
         <v>8</v>
       </c>
@@ -5801,7 +5804,7 @@
       </c>
     </row>
     <row r="8" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="38"/>
+      <c r="A8" s="39"/>
       <c r="B8" s="4" t="s">
         <v>9</v>
       </c>
@@ -5831,7 +5834,7 @@
       </c>
     </row>
     <row r="9" spans="1:26" ht="64.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="37" t="s">
+      <c r="A9" s="38" t="s">
         <v>15</v>
       </c>
       <c r="B9" s="4" t="s">
@@ -5863,7 +5866,7 @@
       </c>
     </row>
     <row r="10" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="38"/>
+      <c r="A10" s="39"/>
       <c r="B10" s="4" t="s">
         <v>8</v>
       </c>
@@ -5893,7 +5896,7 @@
       </c>
     </row>
     <row r="11" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="38"/>
+      <c r="A11" s="39"/>
       <c r="B11" s="4" t="s">
         <v>9</v>
       </c>
@@ -5923,7 +5926,7 @@
       </c>
     </row>
     <row r="12" spans="1:26" ht="64.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="37" t="s">
+      <c r="A12" s="38" t="s">
         <v>16</v>
       </c>
       <c r="B12" s="4" t="s">
@@ -5955,7 +5958,7 @@
       </c>
     </row>
     <row r="13" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="38"/>
+      <c r="A13" s="39"/>
       <c r="B13" s="4" t="s">
         <v>8</v>
       </c>
@@ -5985,7 +5988,7 @@
       </c>
     </row>
     <row r="14" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="38"/>
+      <c r="A14" s="39"/>
       <c r="B14" s="4" t="s">
         <v>9</v>
       </c>
@@ -6015,7 +6018,7 @@
       </c>
     </row>
     <row r="15" spans="1:26" ht="64.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="37" t="s">
+      <c r="A15" s="38" t="s">
         <v>17</v>
       </c>
       <c r="B15" s="4" t="s">
@@ -6047,7 +6050,7 @@
       </c>
     </row>
     <row r="16" spans="1:26" ht="77.400000000000006" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="38"/>
+      <c r="A16" s="39"/>
       <c r="B16" s="4" t="s">
         <v>8</v>
       </c>
@@ -6077,7 +6080,7 @@
       </c>
     </row>
     <row r="17" spans="1:10" ht="63.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="38"/>
+      <c r="A17" s="39"/>
       <c r="B17" s="4" t="s">
         <v>9</v>
       </c>
@@ -10073,25 +10076,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="18" x14ac:dyDescent="0.4">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="44" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="43" t="s">
+      <c r="B1" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="42" t="s">
+      <c r="C1" s="43" t="s">
         <v>42</v>
       </c>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42"/>
-      <c r="G1" s="42"/>
-      <c r="H1" s="42"/>
-      <c r="I1" s="42"/>
+      <c r="D1" s="43"/>
+      <c r="E1" s="43"/>
+      <c r="F1" s="43"/>
+      <c r="G1" s="43"/>
+      <c r="H1" s="43"/>
+      <c r="I1" s="43"/>
     </row>
     <row r="2" spans="1:9" ht="18" x14ac:dyDescent="0.4">
-      <c r="A2" s="44"/>
-      <c r="B2" s="44"/>
+      <c r="A2" s="45"/>
+      <c r="B2" s="45"/>
       <c r="C2" s="14" t="s">
         <v>2</v>
       </c>
@@ -10115,7 +10118,7 @@
       </c>
     </row>
     <row r="3" spans="1:9" ht="87.5" x14ac:dyDescent="0.35">
-      <c r="A3" s="40" t="s">
+      <c r="A3" s="41" t="s">
         <v>13</v>
       </c>
       <c r="B3" s="15" t="s">
@@ -10144,7 +10147,7 @@
       </c>
     </row>
     <row r="4" spans="1:9" ht="105" x14ac:dyDescent="0.35">
-      <c r="A4" s="41"/>
+      <c r="A4" s="42"/>
       <c r="B4" s="15" t="s">
         <v>12</v>
       </c>
@@ -10171,7 +10174,7 @@
       </c>
     </row>
     <row r="5" spans="1:9" ht="52.5" x14ac:dyDescent="0.35">
-      <c r="A5" s="41"/>
+      <c r="A5" s="42"/>
       <c r="B5" s="15" t="s">
         <v>9</v>
       </c>
@@ -10198,7 +10201,7 @@
       </c>
     </row>
     <row r="6" spans="1:9" ht="157.5" x14ac:dyDescent="0.35">
-      <c r="A6" s="40" t="s">
+      <c r="A6" s="41" t="s">
         <v>14</v>
       </c>
       <c r="B6" s="15" t="s">
@@ -10227,7 +10230,7 @@
       </c>
     </row>
     <row r="7" spans="1:9" ht="157.5" x14ac:dyDescent="0.35">
-      <c r="A7" s="41"/>
+      <c r="A7" s="42"/>
       <c r="B7" s="15" t="s">
         <v>8</v>
       </c>
@@ -10254,7 +10257,7 @@
       </c>
     </row>
     <row r="8" spans="1:9" ht="70" x14ac:dyDescent="0.35">
-      <c r="A8" s="41"/>
+      <c r="A8" s="42"/>
       <c r="B8" s="15" t="s">
         <v>9</v>
       </c>
@@ -10281,7 +10284,7 @@
       </c>
     </row>
     <row r="9" spans="1:9" ht="140" x14ac:dyDescent="0.35">
-      <c r="A9" s="40" t="s">
+      <c r="A9" s="41" t="s">
         <v>15</v>
       </c>
       <c r="B9" s="15" t="s">
@@ -10310,7 +10313,7 @@
       </c>
     </row>
     <row r="10" spans="1:9" ht="157.5" x14ac:dyDescent="0.35">
-      <c r="A10" s="41"/>
+      <c r="A10" s="42"/>
       <c r="B10" s="15" t="s">
         <v>8</v>
       </c>
@@ -10337,7 +10340,7 @@
       </c>
     </row>
     <row r="11" spans="1:9" ht="70" x14ac:dyDescent="0.35">
-      <c r="A11" s="41"/>
+      <c r="A11" s="42"/>
       <c r="B11" s="15" t="s">
         <v>9</v>
       </c>
@@ -10364,7 +10367,7 @@
       </c>
     </row>
     <row r="12" spans="1:9" ht="157.5" x14ac:dyDescent="0.35">
-      <c r="A12" s="40" t="s">
+      <c r="A12" s="41" t="s">
         <v>16</v>
       </c>
       <c r="B12" s="15" t="s">
@@ -10393,7 +10396,7 @@
       </c>
     </row>
     <row r="13" spans="1:9" ht="157.5" x14ac:dyDescent="0.35">
-      <c r="A13" s="41"/>
+      <c r="A13" s="42"/>
       <c r="B13" s="15" t="s">
         <v>8</v>
       </c>
@@ -10420,7 +10423,7 @@
       </c>
     </row>
     <row r="14" spans="1:9" ht="175" x14ac:dyDescent="0.35">
-      <c r="A14" s="41"/>
+      <c r="A14" s="42"/>
       <c r="B14" s="15" t="s">
         <v>9</v>
       </c>
@@ -10447,7 +10450,7 @@
       </c>
     </row>
     <row r="15" spans="1:9" ht="105" x14ac:dyDescent="0.35">
-      <c r="A15" s="40" t="s">
+      <c r="A15" s="41" t="s">
         <v>17</v>
       </c>
       <c r="B15" s="15" t="s">
@@ -10476,7 +10479,7 @@
       </c>
     </row>
     <row r="16" spans="1:9" ht="157.5" x14ac:dyDescent="0.35">
-      <c r="A16" s="41"/>
+      <c r="A16" s="42"/>
       <c r="B16" s="15" t="s">
         <v>8</v>
       </c>
@@ -10503,7 +10506,7 @@
       </c>
     </row>
     <row r="17" spans="1:9" ht="70" x14ac:dyDescent="0.35">
-      <c r="A17" s="41"/>
+      <c r="A17" s="42"/>
       <c r="B17" s="15" t="s">
         <v>9</v>
       </c>
@@ -10564,25 +10567,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="18" x14ac:dyDescent="0.4">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="44" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="43" t="s">
+      <c r="B1" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="42" t="s">
+      <c r="C1" s="43" t="s">
         <v>64</v>
       </c>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42"/>
-      <c r="G1" s="42"/>
-      <c r="H1" s="42"/>
-      <c r="I1" s="42"/>
+      <c r="D1" s="43"/>
+      <c r="E1" s="43"/>
+      <c r="F1" s="43"/>
+      <c r="G1" s="43"/>
+      <c r="H1" s="43"/>
+      <c r="I1" s="43"/>
     </row>
     <row r="2" spans="1:9" ht="18" x14ac:dyDescent="0.4">
-      <c r="A2" s="44"/>
-      <c r="B2" s="44"/>
+      <c r="A2" s="45"/>
+      <c r="B2" s="45"/>
       <c r="C2" s="14" t="s">
         <v>2</v>
       </c>
@@ -10606,7 +10609,7 @@
       </c>
     </row>
     <row r="3" spans="1:9" ht="105" x14ac:dyDescent="0.35">
-      <c r="A3" s="40" t="s">
+      <c r="A3" s="41" t="s">
         <v>13</v>
       </c>
       <c r="B3" s="21" t="s">
@@ -10635,7 +10638,7 @@
       </c>
     </row>
     <row r="4" spans="1:9" ht="105" x14ac:dyDescent="0.35">
-      <c r="A4" s="41"/>
+      <c r="A4" s="42"/>
       <c r="B4" s="21" t="s">
         <v>12</v>
       </c>
@@ -10662,7 +10665,7 @@
       </c>
     </row>
     <row r="5" spans="1:9" ht="87.5" x14ac:dyDescent="0.35">
-      <c r="A5" s="41"/>
+      <c r="A5" s="42"/>
       <c r="B5" s="21" t="s">
         <v>9</v>
       </c>
@@ -10689,7 +10692,7 @@
       </c>
     </row>
     <row r="6" spans="1:9" ht="122.5" x14ac:dyDescent="0.35">
-      <c r="A6" s="40" t="s">
+      <c r="A6" s="41" t="s">
         <v>14</v>
       </c>
       <c r="B6" s="21" t="s">
@@ -10718,7 +10721,7 @@
       </c>
     </row>
     <row r="7" spans="1:9" ht="105" x14ac:dyDescent="0.35">
-      <c r="A7" s="41"/>
+      <c r="A7" s="42"/>
       <c r="B7" s="21" t="s">
         <v>8</v>
       </c>
@@ -10745,7 +10748,7 @@
       </c>
     </row>
     <row r="8" spans="1:9" ht="105" x14ac:dyDescent="0.35">
-      <c r="A8" s="41"/>
+      <c r="A8" s="42"/>
       <c r="B8" s="21" t="s">
         <v>9</v>
       </c>
@@ -10772,7 +10775,7 @@
       </c>
     </row>
     <row r="9" spans="1:9" ht="70" x14ac:dyDescent="0.35">
-      <c r="A9" s="40" t="s">
+      <c r="A9" s="41" t="s">
         <v>15</v>
       </c>
       <c r="B9" s="21" t="s">
@@ -10801,7 +10804,7 @@
       </c>
     </row>
     <row r="10" spans="1:9" ht="52.5" x14ac:dyDescent="0.35">
-      <c r="A10" s="41"/>
+      <c r="A10" s="42"/>
       <c r="B10" s="21" t="s">
         <v>8</v>
       </c>
@@ -10828,7 +10831,7 @@
       </c>
     </row>
     <row r="11" spans="1:9" ht="157.5" x14ac:dyDescent="0.35">
-      <c r="A11" s="41"/>
+      <c r="A11" s="42"/>
       <c r="B11" s="21" t="s">
         <v>9</v>
       </c>
@@ -10855,7 +10858,7 @@
       </c>
     </row>
     <row r="12" spans="1:9" ht="192.5" x14ac:dyDescent="0.35">
-      <c r="A12" s="40" t="s">
+      <c r="A12" s="41" t="s">
         <v>16</v>
       </c>
       <c r="B12" s="21" t="s">
@@ -10884,7 +10887,7 @@
       </c>
     </row>
     <row r="13" spans="1:9" ht="192.5" x14ac:dyDescent="0.35">
-      <c r="A13" s="41"/>
+      <c r="A13" s="42"/>
       <c r="B13" s="21" t="s">
         <v>8</v>
       </c>
@@ -10911,7 +10914,7 @@
       </c>
     </row>
     <row r="14" spans="1:9" ht="87.5" x14ac:dyDescent="0.35">
-      <c r="A14" s="41"/>
+      <c r="A14" s="42"/>
       <c r="B14" s="21" t="s">
         <v>9</v>
       </c>
@@ -10938,7 +10941,7 @@
       </c>
     </row>
     <row r="15" spans="1:9" ht="70" x14ac:dyDescent="0.35">
-      <c r="A15" s="40" t="s">
+      <c r="A15" s="41" t="s">
         <v>17</v>
       </c>
       <c r="B15" s="21" t="s">
@@ -10967,7 +10970,7 @@
       </c>
     </row>
     <row r="16" spans="1:9" ht="52.5" x14ac:dyDescent="0.35">
-      <c r="A16" s="41"/>
+      <c r="A16" s="42"/>
       <c r="B16" s="21" t="s">
         <v>8</v>
       </c>
@@ -10994,7 +10997,7 @@
       </c>
     </row>
     <row r="17" spans="1:9" ht="157.5" x14ac:dyDescent="0.35">
-      <c r="A17" s="41"/>
+      <c r="A17" s="42"/>
       <c r="B17" s="21" t="s">
         <v>9</v>
       </c>
@@ -11040,8 +11043,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B762D8C-72F3-45B7-9544-A442629D54B9}">
   <dimension ref="A1:I17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.453125" defaultRowHeight="17.5" x14ac:dyDescent="0.35"/>
@@ -11057,25 +11060,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="18" x14ac:dyDescent="0.4">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="44" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="43" t="s">
+      <c r="B1" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="42" t="s">
+      <c r="C1" s="43" t="s">
         <v>64</v>
       </c>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42"/>
-      <c r="G1" s="42"/>
-      <c r="H1" s="42"/>
-      <c r="I1" s="42"/>
+      <c r="D1" s="43"/>
+      <c r="E1" s="43"/>
+      <c r="F1" s="43"/>
+      <c r="G1" s="43"/>
+      <c r="H1" s="43"/>
+      <c r="I1" s="43"/>
     </row>
     <row r="2" spans="1:9" ht="18" x14ac:dyDescent="0.4">
-      <c r="A2" s="44"/>
-      <c r="B2" s="44"/>
+      <c r="A2" s="45"/>
+      <c r="B2" s="45"/>
       <c r="C2" s="14" t="s">
         <v>2</v>
       </c>
@@ -11099,7 +11102,7 @@
       </c>
     </row>
     <row r="3" spans="1:9" ht="192.5" x14ac:dyDescent="0.35">
-      <c r="A3" s="40" t="s">
+      <c r="A3" s="41" t="s">
         <v>13</v>
       </c>
       <c r="B3" s="23" t="s">
@@ -11120,11 +11123,13 @@
       <c r="G3" s="25" t="s">
         <v>84</v>
       </c>
-      <c r="H3" s="25"/>
+      <c r="H3" s="25" t="s">
+        <v>55</v>
+      </c>
       <c r="I3" s="26"/>
     </row>
     <row r="4" spans="1:9" ht="140" x14ac:dyDescent="0.35">
-      <c r="A4" s="41"/>
+      <c r="A4" s="42"/>
       <c r="B4" s="23" t="s">
         <v>12</v>
       </c>
@@ -11143,11 +11148,13 @@
       <c r="G4" s="25" t="s">
         <v>55</v>
       </c>
-      <c r="H4" s="26"/>
+      <c r="H4" s="25" t="s">
+        <v>55</v>
+      </c>
       <c r="I4" s="25"/>
     </row>
     <row r="5" spans="1:9" ht="52.5" x14ac:dyDescent="0.35">
-      <c r="A5" s="41"/>
+      <c r="A5" s="42"/>
       <c r="B5" s="23" t="s">
         <v>9</v>
       </c>
@@ -11166,10 +11173,12 @@
       <c r="G5" s="31" t="s">
         <v>30</v>
       </c>
-      <c r="H5" s="25"/>
+      <c r="H5" s="25" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="6" spans="1:9" ht="192.5" x14ac:dyDescent="0.35">
-      <c r="A6" s="40" t="s">
+      <c r="A6" s="41" t="s">
         <v>14</v>
       </c>
       <c r="B6" s="23" t="s">
@@ -11190,11 +11199,13 @@
       <c r="G6" s="25" t="s">
         <v>85</v>
       </c>
-      <c r="H6" s="25"/>
+      <c r="H6" s="25" t="s">
+        <v>55</v>
+      </c>
       <c r="I6" s="26"/>
     </row>
     <row r="7" spans="1:9" ht="140" x14ac:dyDescent="0.35">
-      <c r="A7" s="41"/>
+      <c r="A7" s="42"/>
       <c r="B7" s="23" t="s">
         <v>8</v>
       </c>
@@ -11213,11 +11224,13 @@
       <c r="G7" s="25" t="s">
         <v>55</v>
       </c>
-      <c r="H7" s="26"/>
+      <c r="H7" s="25" t="s">
+        <v>55</v>
+      </c>
       <c r="I7" s="25"/>
     </row>
     <row r="8" spans="1:9" ht="52.5" x14ac:dyDescent="0.35">
-      <c r="A8" s="41"/>
+      <c r="A8" s="42"/>
       <c r="B8" s="23" t="s">
         <v>9</v>
       </c>
@@ -11236,10 +11249,12 @@
       <c r="G8" s="31" t="s">
         <v>30</v>
       </c>
-      <c r="H8" s="25"/>
+      <c r="H8" s="25" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="9" spans="1:9" ht="157.5" x14ac:dyDescent="0.35">
-      <c r="A9" s="40" t="s">
+      <c r="A9" s="41" t="s">
         <v>15</v>
       </c>
       <c r="B9" s="23" t="s">
@@ -11260,11 +11275,13 @@
       <c r="G9" s="33" t="s">
         <v>88</v>
       </c>
-      <c r="H9" s="25"/>
+      <c r="H9" s="25" t="s">
+        <v>55</v>
+      </c>
       <c r="I9" s="25"/>
     </row>
     <row r="10" spans="1:9" ht="140" x14ac:dyDescent="0.35">
-      <c r="A10" s="41"/>
+      <c r="A10" s="42"/>
       <c r="B10" s="23" t="s">
         <v>8</v>
       </c>
@@ -11283,11 +11300,13 @@
       <c r="G10" s="25" t="s">
         <v>55</v>
       </c>
-      <c r="H10" s="25"/>
+      <c r="H10" s="25" t="s">
+        <v>55</v>
+      </c>
       <c r="I10" s="25"/>
     </row>
     <row r="11" spans="1:9" ht="52.5" x14ac:dyDescent="0.35">
-      <c r="A11" s="41"/>
+      <c r="A11" s="42"/>
       <c r="B11" s="23" t="s">
         <v>9</v>
       </c>
@@ -11306,11 +11325,13 @@
       <c r="G11" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="H11" s="25"/>
+      <c r="H11" s="25" t="s">
+        <v>30</v>
+      </c>
       <c r="I11" s="25"/>
     </row>
     <row r="12" spans="1:9" ht="192.5" x14ac:dyDescent="0.35">
-      <c r="A12" s="40" t="s">
+      <c r="A12" s="41" t="s">
         <v>16</v>
       </c>
       <c r="B12" s="23" t="s">
@@ -11331,11 +11352,13 @@
       <c r="G12" s="25" t="s">
         <v>86</v>
       </c>
-      <c r="H12" s="25"/>
+      <c r="H12" s="25" t="s">
+        <v>55</v>
+      </c>
       <c r="I12" s="26"/>
     </row>
     <row r="13" spans="1:9" ht="140" x14ac:dyDescent="0.35">
-      <c r="A13" s="41"/>
+      <c r="A13" s="42"/>
       <c r="B13" s="23" t="s">
         <v>8</v>
       </c>
@@ -11354,11 +11377,13 @@
       <c r="G13" s="25" t="s">
         <v>55</v>
       </c>
-      <c r="H13" s="26"/>
+      <c r="H13" s="25" t="s">
+        <v>55</v>
+      </c>
       <c r="I13" s="25"/>
     </row>
     <row r="14" spans="1:9" ht="52.5" x14ac:dyDescent="0.35">
-      <c r="A14" s="41"/>
+      <c r="A14" s="42"/>
       <c r="B14" s="23" t="s">
         <v>9</v>
       </c>
@@ -11377,10 +11402,12 @@
       <c r="G14" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="H14" s="25"/>
+      <c r="H14" s="34" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="15" spans="1:9" ht="192.5" x14ac:dyDescent="0.35">
-      <c r="A15" s="40" t="s">
+      <c r="A15" s="41" t="s">
         <v>17</v>
       </c>
       <c r="B15" s="23" t="s">
@@ -11401,11 +11428,13 @@
       <c r="G15" s="33" t="s">
         <v>87</v>
       </c>
-      <c r="H15" s="25"/>
+      <c r="H15" s="25" t="s">
+        <v>55</v>
+      </c>
       <c r="I15" s="25"/>
     </row>
     <row r="16" spans="1:9" ht="157.5" x14ac:dyDescent="0.35">
-      <c r="A16" s="41"/>
+      <c r="A16" s="42"/>
       <c r="B16" s="23" t="s">
         <v>8</v>
       </c>
@@ -11424,11 +11453,13 @@
       <c r="G16" s="25" t="s">
         <v>55</v>
       </c>
-      <c r="H16" s="25"/>
+      <c r="H16" s="25" t="s">
+        <v>55</v>
+      </c>
       <c r="I16" s="25"/>
     </row>
     <row r="17" spans="1:9" ht="52.5" x14ac:dyDescent="0.35">
-      <c r="A17" s="41"/>
+      <c r="A17" s="42"/>
       <c r="B17" s="23" t="s">
         <v>9</v>
       </c>
@@ -11447,7 +11478,9 @@
       <c r="G17" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="H17" s="25"/>
+      <c r="H17" s="25" t="s">
+        <v>30</v>
+      </c>
       <c r="I17" s="25"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated du (week9 sun)
</commit_message>
<xml_diff>
--- a/metrics/du.xlsx
+++ b/metrics/du.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\project-g4t6\metrics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D168C13-83F3-4961-AAAB-3B65CF7ABE57}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39F041C1-E36C-449D-95E7-964463720E97}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9850" yWindow="590" windowWidth="9280" windowHeight="7360" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Week 5" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="751" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="769" uniqueCount="92">
   <si>
     <t>Question</t>
   </si>
@@ -310,6 +310,17 @@
 (2) Discovered redundant testcases and came up with improved testcases for Prerequisite.csv
 </t>
   </si>
+  <si>
+    <t>Cleared Round 1 logic</t>
+  </si>
+  <si>
+    <t>(1) did JSON dump and start
+(2)  Did half of Round 2 clearing</t>
+  </si>
+  <si>
+    <t>(1) Updated schedule
+(2) Finished running testcases for bid.csv</t>
+  </si>
 </sst>
 </file>
 
@@ -388,7 +399,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -486,19 +497,22 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -826,36 +840,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="41" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="35" t="s">
+      <c r="B1" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="40" t="s">
+      <c r="C1" s="38" t="s">
         <v>18</v>
       </c>
-      <c r="D1" s="40"/>
-      <c r="E1" s="40"/>
-      <c r="F1" s="40"/>
-      <c r="G1" s="40"/>
-      <c r="H1" s="40"/>
-      <c r="I1" s="40"/>
-      <c r="J1" s="37" t="s">
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
+      <c r="G1" s="38"/>
+      <c r="H1" s="38"/>
+      <c r="I1" s="38"/>
+      <c r="J1" s="41" t="s">
         <v>1</v>
       </c>
-      <c r="K1" s="35" t="s">
+      <c r="K1" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="L1" s="40" t="s">
+      <c r="L1" s="38" t="s">
         <v>40</v>
       </c>
-      <c r="M1" s="40"/>
-      <c r="N1" s="40"/>
-      <c r="O1" s="40"/>
-      <c r="P1" s="40"/>
-      <c r="Q1" s="40"/>
-      <c r="R1" s="40"/>
+      <c r="M1" s="38"/>
+      <c r="N1" s="38"/>
+      <c r="O1" s="38"/>
+      <c r="P1" s="38"/>
+      <c r="Q1" s="38"/>
+      <c r="R1" s="38"/>
       <c r="S1" s="1"/>
       <c r="T1" s="1"/>
       <c r="U1" s="1"/>
@@ -866,8 +880,8 @@
       <c r="Z1" s="1"/>
     </row>
     <row r="2" spans="1:26" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="36"/>
-      <c r="B2" s="36"/>
+      <c r="A2" s="37"/>
+      <c r="B2" s="37"/>
       <c r="C2" s="3" t="s">
         <v>2</v>
       </c>
@@ -889,8 +903,8 @@
       <c r="I2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="J2" s="36"/>
-      <c r="K2" s="36"/>
+      <c r="J2" s="37"/>
+      <c r="K2" s="37"/>
       <c r="L2" s="3" t="s">
         <v>2</v>
       </c>
@@ -922,7 +936,7 @@
       <c r="Z2" s="1"/>
     </row>
     <row r="3" spans="1:26" ht="47.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="38" t="s">
+      <c r="A3" s="39" t="s">
         <v>13</v>
       </c>
       <c r="B3" s="4" t="s">
@@ -941,7 +955,7 @@
       <c r="I3" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="J3" s="38" t="s">
+      <c r="J3" s="39" t="s">
         <v>13</v>
       </c>
       <c r="K3" s="4" t="s">
@@ -970,7 +984,7 @@
       </c>
     </row>
     <row r="4" spans="1:26" ht="63" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="39"/>
+      <c r="A4" s="40"/>
       <c r="B4" s="4" t="s">
         <v>12</v>
       </c>
@@ -987,7 +1001,7 @@
       <c r="I4" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="J4" s="39"/>
+      <c r="J4" s="40"/>
       <c r="K4" s="4" t="s">
         <v>12</v>
       </c>
@@ -1014,7 +1028,7 @@
       </c>
     </row>
     <row r="5" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="39"/>
+      <c r="A5" s="40"/>
       <c r="B5" s="4" t="s">
         <v>9</v>
       </c>
@@ -1031,7 +1045,7 @@
       <c r="I5" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="J5" s="39"/>
+      <c r="J5" s="40"/>
       <c r="K5" s="4" t="s">
         <v>9</v>
       </c>
@@ -1058,7 +1072,7 @@
       </c>
     </row>
     <row r="6" spans="1:26" ht="62.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="38" t="s">
+      <c r="A6" s="39" t="s">
         <v>14</v>
       </c>
       <c r="B6" s="4" t="s">
@@ -1077,7 +1091,7 @@
       <c r="I6" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="J6" s="38" t="s">
+      <c r="J6" s="39" t="s">
         <v>14</v>
       </c>
       <c r="K6" s="4" t="s">
@@ -1106,7 +1120,7 @@
       </c>
     </row>
     <row r="7" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="39"/>
+      <c r="A7" s="40"/>
       <c r="B7" s="4" t="s">
         <v>8</v>
       </c>
@@ -1123,7 +1137,7 @@
       <c r="I7" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="J7" s="39"/>
+      <c r="J7" s="40"/>
       <c r="K7" s="4" t="s">
         <v>8</v>
       </c>
@@ -1150,7 +1164,7 @@
       </c>
     </row>
     <row r="8" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="39"/>
+      <c r="A8" s="40"/>
       <c r="B8" s="4" t="s">
         <v>9</v>
       </c>
@@ -1167,7 +1181,7 @@
       <c r="I8" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="J8" s="39"/>
+      <c r="J8" s="40"/>
       <c r="K8" s="4" t="s">
         <v>9</v>
       </c>
@@ -1194,7 +1208,7 @@
       </c>
     </row>
     <row r="9" spans="1:26" ht="64.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="38" t="s">
+      <c r="A9" s="39" t="s">
         <v>15</v>
       </c>
       <c r="B9" s="4" t="s">
@@ -1213,7 +1227,7 @@
       <c r="I9" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="J9" s="38" t="s">
+      <c r="J9" s="39" t="s">
         <v>15</v>
       </c>
       <c r="K9" s="4" t="s">
@@ -1242,7 +1256,7 @@
       </c>
     </row>
     <row r="10" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="39"/>
+      <c r="A10" s="40"/>
       <c r="B10" s="4" t="s">
         <v>8</v>
       </c>
@@ -1259,7 +1273,7 @@
       <c r="I10" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="J10" s="39"/>
+      <c r="J10" s="40"/>
       <c r="K10" s="4" t="s">
         <v>8</v>
       </c>
@@ -1286,7 +1300,7 @@
       </c>
     </row>
     <row r="11" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="39"/>
+      <c r="A11" s="40"/>
       <c r="B11" s="4" t="s">
         <v>9</v>
       </c>
@@ -1303,7 +1317,7 @@
       <c r="I11" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="J11" s="39"/>
+      <c r="J11" s="40"/>
       <c r="K11" s="4" t="s">
         <v>9</v>
       </c>
@@ -1330,7 +1344,7 @@
       </c>
     </row>
     <row r="12" spans="1:26" ht="64.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="38" t="s">
+      <c r="A12" s="39" t="s">
         <v>16</v>
       </c>
       <c r="B12" s="4" t="s">
@@ -1349,7 +1363,7 @@
       <c r="I12" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="J12" s="38" t="s">
+      <c r="J12" s="39" t="s">
         <v>16</v>
       </c>
       <c r="K12" s="4" t="s">
@@ -1378,7 +1392,7 @@
       </c>
     </row>
     <row r="13" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="39"/>
+      <c r="A13" s="40"/>
       <c r="B13" s="4" t="s">
         <v>8</v>
       </c>
@@ -1395,7 +1409,7 @@
       <c r="I13" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="J13" s="39"/>
+      <c r="J13" s="40"/>
       <c r="K13" s="4" t="s">
         <v>8</v>
       </c>
@@ -1422,7 +1436,7 @@
       </c>
     </row>
     <row r="14" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="39"/>
+      <c r="A14" s="40"/>
       <c r="B14" s="4" t="s">
         <v>9</v>
       </c>
@@ -1439,7 +1453,7 @@
       <c r="I14" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="J14" s="39"/>
+      <c r="J14" s="40"/>
       <c r="K14" s="4" t="s">
         <v>9</v>
       </c>
@@ -1466,7 +1480,7 @@
       </c>
     </row>
     <row r="15" spans="1:26" ht="64.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="38" t="s">
+      <c r="A15" s="39" t="s">
         <v>17</v>
       </c>
       <c r="B15" s="4" t="s">
@@ -1485,7 +1499,7 @@
       <c r="I15" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="J15" s="38" t="s">
+      <c r="J15" s="39" t="s">
         <v>17</v>
       </c>
       <c r="K15" s="4" t="s">
@@ -1514,7 +1528,7 @@
       </c>
     </row>
     <row r="16" spans="1:26" ht="77.400000000000006" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="39"/>
+      <c r="A16" s="40"/>
       <c r="B16" s="4" t="s">
         <v>8</v>
       </c>
@@ -1531,7 +1545,7 @@
       <c r="I16" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="J16" s="39"/>
+      <c r="J16" s="40"/>
       <c r="K16" s="4" t="s">
         <v>8</v>
       </c>
@@ -1558,7 +1572,7 @@
       </c>
     </row>
     <row r="17" spans="1:18" ht="63.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="39"/>
+      <c r="A17" s="40"/>
       <c r="B17" s="4" t="s">
         <v>9</v>
       </c>
@@ -1575,7 +1589,7 @@
       <c r="I17" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="J17" s="39"/>
+      <c r="J17" s="40"/>
       <c r="K17" s="4" t="s">
         <v>9</v>
       </c>
@@ -5539,11 +5553,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="K1:K2"/>
-    <mergeCell ref="L1:R1"/>
-    <mergeCell ref="J3:J5"/>
-    <mergeCell ref="J6:J8"/>
-    <mergeCell ref="C1:I1"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="J15:J17"/>
@@ -5555,6 +5564,11 @@
     <mergeCell ref="A3:A5"/>
     <mergeCell ref="A6:A8"/>
     <mergeCell ref="A9:A11"/>
+    <mergeCell ref="K1:K2"/>
+    <mergeCell ref="L1:R1"/>
+    <mergeCell ref="J3:J5"/>
+    <mergeCell ref="J6:J8"/>
+    <mergeCell ref="C1:I1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -5588,24 +5602,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="41" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="35" t="s">
+      <c r="B1" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="35" t="s">
+      <c r="C1" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="40" t="s">
+      <c r="D1" s="38" t="s">
         <v>41</v>
       </c>
-      <c r="E1" s="40"/>
-      <c r="F1" s="40"/>
-      <c r="G1" s="40"/>
-      <c r="H1" s="40"/>
-      <c r="I1" s="40"/>
-      <c r="J1" s="40"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
+      <c r="G1" s="38"/>
+      <c r="H1" s="38"/>
+      <c r="I1" s="38"/>
+      <c r="J1" s="38"/>
       <c r="S1" s="1"/>
       <c r="T1" s="1"/>
       <c r="U1" s="1"/>
@@ -5616,9 +5630,9 @@
       <c r="Z1" s="1"/>
     </row>
     <row r="2" spans="1:26" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="36"/>
-      <c r="B2" s="36"/>
-      <c r="C2" s="36"/>
+      <c r="A2" s="37"/>
+      <c r="B2" s="37"/>
+      <c r="C2" s="37"/>
       <c r="D2" s="3" t="s">
         <v>2</v>
       </c>
@@ -5650,7 +5664,7 @@
       <c r="Z2" s="1"/>
     </row>
     <row r="3" spans="1:26" ht="47.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="38" t="s">
+      <c r="A3" s="39" t="s">
         <v>13</v>
       </c>
       <c r="B3" s="4" t="s">
@@ -5682,7 +5696,7 @@
       </c>
     </row>
     <row r="4" spans="1:26" ht="63" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="39"/>
+      <c r="A4" s="40"/>
       <c r="B4" s="4" t="s">
         <v>12</v>
       </c>
@@ -5712,7 +5726,7 @@
       </c>
     </row>
     <row r="5" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="39"/>
+      <c r="A5" s="40"/>
       <c r="B5" s="4" t="s">
         <v>9</v>
       </c>
@@ -5742,7 +5756,7 @@
       </c>
     </row>
     <row r="6" spans="1:26" ht="62.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="38" t="s">
+      <c r="A6" s="39" t="s">
         <v>14</v>
       </c>
       <c r="B6" s="4" t="s">
@@ -5774,7 +5788,7 @@
       </c>
     </row>
     <row r="7" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="39"/>
+      <c r="A7" s="40"/>
       <c r="B7" s="4" t="s">
         <v>8</v>
       </c>
@@ -5804,7 +5818,7 @@
       </c>
     </row>
     <row r="8" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="39"/>
+      <c r="A8" s="40"/>
       <c r="B8" s="4" t="s">
         <v>9</v>
       </c>
@@ -5834,7 +5848,7 @@
       </c>
     </row>
     <row r="9" spans="1:26" ht="64.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="38" t="s">
+      <c r="A9" s="39" t="s">
         <v>15</v>
       </c>
       <c r="B9" s="4" t="s">
@@ -5866,7 +5880,7 @@
       </c>
     </row>
     <row r="10" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="39"/>
+      <c r="A10" s="40"/>
       <c r="B10" s="4" t="s">
         <v>8</v>
       </c>
@@ -5896,7 +5910,7 @@
       </c>
     </row>
     <row r="11" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="39"/>
+      <c r="A11" s="40"/>
       <c r="B11" s="4" t="s">
         <v>9</v>
       </c>
@@ -5926,7 +5940,7 @@
       </c>
     </row>
     <row r="12" spans="1:26" ht="64.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="38" t="s">
+      <c r="A12" s="39" t="s">
         <v>16</v>
       </c>
       <c r="B12" s="4" t="s">
@@ -5958,7 +5972,7 @@
       </c>
     </row>
     <row r="13" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="39"/>
+      <c r="A13" s="40"/>
       <c r="B13" s="4" t="s">
         <v>8</v>
       </c>
@@ -5988,7 +6002,7 @@
       </c>
     </row>
     <row r="14" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="39"/>
+      <c r="A14" s="40"/>
       <c r="B14" s="4" t="s">
         <v>9</v>
       </c>
@@ -6018,7 +6032,7 @@
       </c>
     </row>
     <row r="15" spans="1:26" ht="64.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="38" t="s">
+      <c r="A15" s="39" t="s">
         <v>17</v>
       </c>
       <c r="B15" s="4" t="s">
@@ -6050,7 +6064,7 @@
       </c>
     </row>
     <row r="16" spans="1:26" ht="77.400000000000006" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="39"/>
+      <c r="A16" s="40"/>
       <c r="B16" s="4" t="s">
         <v>8</v>
       </c>
@@ -6080,7 +6094,7 @@
       </c>
     </row>
     <row r="17" spans="1:10" ht="63.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="39"/>
+      <c r="A17" s="40"/>
       <c r="B17" s="4" t="s">
         <v>9</v>
       </c>
@@ -10076,25 +10090,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="18" x14ac:dyDescent="0.4">
-      <c r="A1" s="44" t="s">
+      <c r="A1" s="45" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="44" t="s">
+      <c r="B1" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="43" t="s">
+      <c r="C1" s="44" t="s">
         <v>42</v>
       </c>
-      <c r="D1" s="43"/>
-      <c r="E1" s="43"/>
-      <c r="F1" s="43"/>
-      <c r="G1" s="43"/>
-      <c r="H1" s="43"/>
-      <c r="I1" s="43"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
+      <c r="F1" s="44"/>
+      <c r="G1" s="44"/>
+      <c r="H1" s="44"/>
+      <c r="I1" s="44"/>
     </row>
     <row r="2" spans="1:9" ht="18" x14ac:dyDescent="0.4">
-      <c r="A2" s="45"/>
-      <c r="B2" s="45"/>
+      <c r="A2" s="46"/>
+      <c r="B2" s="46"/>
       <c r="C2" s="14" t="s">
         <v>2</v>
       </c>
@@ -10118,7 +10132,7 @@
       </c>
     </row>
     <row r="3" spans="1:9" ht="87.5" x14ac:dyDescent="0.35">
-      <c r="A3" s="41" t="s">
+      <c r="A3" s="42" t="s">
         <v>13</v>
       </c>
       <c r="B3" s="15" t="s">
@@ -10147,7 +10161,7 @@
       </c>
     </row>
     <row r="4" spans="1:9" ht="105" x14ac:dyDescent="0.35">
-      <c r="A4" s="42"/>
+      <c r="A4" s="43"/>
       <c r="B4" s="15" t="s">
         <v>12</v>
       </c>
@@ -10174,7 +10188,7 @@
       </c>
     </row>
     <row r="5" spans="1:9" ht="52.5" x14ac:dyDescent="0.35">
-      <c r="A5" s="42"/>
+      <c r="A5" s="43"/>
       <c r="B5" s="15" t="s">
         <v>9</v>
       </c>
@@ -10201,7 +10215,7 @@
       </c>
     </row>
     <row r="6" spans="1:9" ht="157.5" x14ac:dyDescent="0.35">
-      <c r="A6" s="41" t="s">
+      <c r="A6" s="42" t="s">
         <v>14</v>
       </c>
       <c r="B6" s="15" t="s">
@@ -10230,7 +10244,7 @@
       </c>
     </row>
     <row r="7" spans="1:9" ht="157.5" x14ac:dyDescent="0.35">
-      <c r="A7" s="42"/>
+      <c r="A7" s="43"/>
       <c r="B7" s="15" t="s">
         <v>8</v>
       </c>
@@ -10257,7 +10271,7 @@
       </c>
     </row>
     <row r="8" spans="1:9" ht="70" x14ac:dyDescent="0.35">
-      <c r="A8" s="42"/>
+      <c r="A8" s="43"/>
       <c r="B8" s="15" t="s">
         <v>9</v>
       </c>
@@ -10284,7 +10298,7 @@
       </c>
     </row>
     <row r="9" spans="1:9" ht="140" x14ac:dyDescent="0.35">
-      <c r="A9" s="41" t="s">
+      <c r="A9" s="42" t="s">
         <v>15</v>
       </c>
       <c r="B9" s="15" t="s">
@@ -10313,7 +10327,7 @@
       </c>
     </row>
     <row r="10" spans="1:9" ht="157.5" x14ac:dyDescent="0.35">
-      <c r="A10" s="42"/>
+      <c r="A10" s="43"/>
       <c r="B10" s="15" t="s">
         <v>8</v>
       </c>
@@ -10340,7 +10354,7 @@
       </c>
     </row>
     <row r="11" spans="1:9" ht="70" x14ac:dyDescent="0.35">
-      <c r="A11" s="42"/>
+      <c r="A11" s="43"/>
       <c r="B11" s="15" t="s">
         <v>9</v>
       </c>
@@ -10367,7 +10381,7 @@
       </c>
     </row>
     <row r="12" spans="1:9" ht="157.5" x14ac:dyDescent="0.35">
-      <c r="A12" s="41" t="s">
+      <c r="A12" s="42" t="s">
         <v>16</v>
       </c>
       <c r="B12" s="15" t="s">
@@ -10396,7 +10410,7 @@
       </c>
     </row>
     <row r="13" spans="1:9" ht="157.5" x14ac:dyDescent="0.35">
-      <c r="A13" s="42"/>
+      <c r="A13" s="43"/>
       <c r="B13" s="15" t="s">
         <v>8</v>
       </c>
@@ -10423,7 +10437,7 @@
       </c>
     </row>
     <row r="14" spans="1:9" ht="175" x14ac:dyDescent="0.35">
-      <c r="A14" s="42"/>
+      <c r="A14" s="43"/>
       <c r="B14" s="15" t="s">
         <v>9</v>
       </c>
@@ -10450,7 +10464,7 @@
       </c>
     </row>
     <row r="15" spans="1:9" ht="105" x14ac:dyDescent="0.35">
-      <c r="A15" s="41" t="s">
+      <c r="A15" s="42" t="s">
         <v>17</v>
       </c>
       <c r="B15" s="15" t="s">
@@ -10479,7 +10493,7 @@
       </c>
     </row>
     <row r="16" spans="1:9" ht="157.5" x14ac:dyDescent="0.35">
-      <c r="A16" s="42"/>
+      <c r="A16" s="43"/>
       <c r="B16" s="15" t="s">
         <v>8</v>
       </c>
@@ -10506,7 +10520,7 @@
       </c>
     </row>
     <row r="17" spans="1:9" ht="70" x14ac:dyDescent="0.35">
-      <c r="A17" s="42"/>
+      <c r="A17" s="43"/>
       <c r="B17" s="15" t="s">
         <v>9</v>
       </c>
@@ -10567,25 +10581,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="18" x14ac:dyDescent="0.4">
-      <c r="A1" s="44" t="s">
+      <c r="A1" s="45" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="44" t="s">
+      <c r="B1" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="43" t="s">
+      <c r="C1" s="44" t="s">
         <v>64</v>
       </c>
-      <c r="D1" s="43"/>
-      <c r="E1" s="43"/>
-      <c r="F1" s="43"/>
-      <c r="G1" s="43"/>
-      <c r="H1" s="43"/>
-      <c r="I1" s="43"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
+      <c r="F1" s="44"/>
+      <c r="G1" s="44"/>
+      <c r="H1" s="44"/>
+      <c r="I1" s="44"/>
     </row>
     <row r="2" spans="1:9" ht="18" x14ac:dyDescent="0.4">
-      <c r="A2" s="45"/>
-      <c r="B2" s="45"/>
+      <c r="A2" s="46"/>
+      <c r="B2" s="46"/>
       <c r="C2" s="14" t="s">
         <v>2</v>
       </c>
@@ -10609,7 +10623,7 @@
       </c>
     </row>
     <row r="3" spans="1:9" ht="105" x14ac:dyDescent="0.35">
-      <c r="A3" s="41" t="s">
+      <c r="A3" s="42" t="s">
         <v>13</v>
       </c>
       <c r="B3" s="21" t="s">
@@ -10638,7 +10652,7 @@
       </c>
     </row>
     <row r="4" spans="1:9" ht="105" x14ac:dyDescent="0.35">
-      <c r="A4" s="42"/>
+      <c r="A4" s="43"/>
       <c r="B4" s="21" t="s">
         <v>12</v>
       </c>
@@ -10665,7 +10679,7 @@
       </c>
     </row>
     <row r="5" spans="1:9" ht="87.5" x14ac:dyDescent="0.35">
-      <c r="A5" s="42"/>
+      <c r="A5" s="43"/>
       <c r="B5" s="21" t="s">
         <v>9</v>
       </c>
@@ -10692,7 +10706,7 @@
       </c>
     </row>
     <row r="6" spans="1:9" ht="122.5" x14ac:dyDescent="0.35">
-      <c r="A6" s="41" t="s">
+      <c r="A6" s="42" t="s">
         <v>14</v>
       </c>
       <c r="B6" s="21" t="s">
@@ -10721,7 +10735,7 @@
       </c>
     </row>
     <row r="7" spans="1:9" ht="105" x14ac:dyDescent="0.35">
-      <c r="A7" s="42"/>
+      <c r="A7" s="43"/>
       <c r="B7" s="21" t="s">
         <v>8</v>
       </c>
@@ -10748,7 +10762,7 @@
       </c>
     </row>
     <row r="8" spans="1:9" ht="105" x14ac:dyDescent="0.35">
-      <c r="A8" s="42"/>
+      <c r="A8" s="43"/>
       <c r="B8" s="21" t="s">
         <v>9</v>
       </c>
@@ -10775,7 +10789,7 @@
       </c>
     </row>
     <row r="9" spans="1:9" ht="70" x14ac:dyDescent="0.35">
-      <c r="A9" s="41" t="s">
+      <c r="A9" s="42" t="s">
         <v>15</v>
       </c>
       <c r="B9" s="21" t="s">
@@ -10804,7 +10818,7 @@
       </c>
     </row>
     <row r="10" spans="1:9" ht="52.5" x14ac:dyDescent="0.35">
-      <c r="A10" s="42"/>
+      <c r="A10" s="43"/>
       <c r="B10" s="21" t="s">
         <v>8</v>
       </c>
@@ -10831,7 +10845,7 @@
       </c>
     </row>
     <row r="11" spans="1:9" ht="157.5" x14ac:dyDescent="0.35">
-      <c r="A11" s="42"/>
+      <c r="A11" s="43"/>
       <c r="B11" s="21" t="s">
         <v>9</v>
       </c>
@@ -10858,7 +10872,7 @@
       </c>
     </row>
     <row r="12" spans="1:9" ht="192.5" x14ac:dyDescent="0.35">
-      <c r="A12" s="41" t="s">
+      <c r="A12" s="42" t="s">
         <v>16</v>
       </c>
       <c r="B12" s="21" t="s">
@@ -10887,7 +10901,7 @@
       </c>
     </row>
     <row r="13" spans="1:9" ht="192.5" x14ac:dyDescent="0.35">
-      <c r="A13" s="42"/>
+      <c r="A13" s="43"/>
       <c r="B13" s="21" t="s">
         <v>8</v>
       </c>
@@ -10914,7 +10928,7 @@
       </c>
     </row>
     <row r="14" spans="1:9" ht="87.5" x14ac:dyDescent="0.35">
-      <c r="A14" s="42"/>
+      <c r="A14" s="43"/>
       <c r="B14" s="21" t="s">
         <v>9</v>
       </c>
@@ -10941,7 +10955,7 @@
       </c>
     </row>
     <row r="15" spans="1:9" ht="70" x14ac:dyDescent="0.35">
-      <c r="A15" s="41" t="s">
+      <c r="A15" s="42" t="s">
         <v>17</v>
       </c>
       <c r="B15" s="21" t="s">
@@ -10970,7 +10984,7 @@
       </c>
     </row>
     <row r="16" spans="1:9" ht="52.5" x14ac:dyDescent="0.35">
-      <c r="A16" s="42"/>
+      <c r="A16" s="43"/>
       <c r="B16" s="21" t="s">
         <v>8</v>
       </c>
@@ -10997,7 +11011,7 @@
       </c>
     </row>
     <row r="17" spans="1:9" ht="157.5" x14ac:dyDescent="0.35">
-      <c r="A17" s="42"/>
+      <c r="A17" s="43"/>
       <c r="B17" s="21" t="s">
         <v>9</v>
       </c>
@@ -11041,10 +11055,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B762D8C-72F3-45B7-9544-A442629D54B9}">
-  <dimension ref="A1:I17"/>
+  <dimension ref="A1:J17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:I1"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.453125" defaultRowHeight="17.5" x14ac:dyDescent="0.35"/>
@@ -11059,26 +11073,26 @@
     <col min="9" max="16384" width="17.453125" style="24"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="18" x14ac:dyDescent="0.4">
-      <c r="A1" s="44" t="s">
+    <row r="1" spans="1:10" ht="18" x14ac:dyDescent="0.4">
+      <c r="A1" s="45" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="44" t="s">
+      <c r="B1" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="43" t="s">
+      <c r="C1" s="44" t="s">
         <v>64</v>
       </c>
-      <c r="D1" s="43"/>
-      <c r="E1" s="43"/>
-      <c r="F1" s="43"/>
-      <c r="G1" s="43"/>
-      <c r="H1" s="43"/>
-      <c r="I1" s="43"/>
-    </row>
-    <row r="2" spans="1:9" ht="18" x14ac:dyDescent="0.4">
-      <c r="A2" s="45"/>
-      <c r="B2" s="45"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
+      <c r="F1" s="44"/>
+      <c r="G1" s="44"/>
+      <c r="H1" s="44"/>
+      <c r="I1" s="44"/>
+    </row>
+    <row r="2" spans="1:10" ht="18" x14ac:dyDescent="0.4">
+      <c r="A2" s="46"/>
+      <c r="B2" s="46"/>
       <c r="C2" s="14" t="s">
         <v>2</v>
       </c>
@@ -11101,8 +11115,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="192.5" x14ac:dyDescent="0.35">
-      <c r="A3" s="41" t="s">
+    <row r="3" spans="1:10" ht="192.5" x14ac:dyDescent="0.35">
+      <c r="A3" s="42" t="s">
         <v>13</v>
       </c>
       <c r="B3" s="23" t="s">
@@ -11126,10 +11140,12 @@
       <c r="H3" s="25" t="s">
         <v>55</v>
       </c>
-      <c r="I3" s="26"/>
-    </row>
-    <row r="4" spans="1:9" ht="140" x14ac:dyDescent="0.35">
-      <c r="A4" s="42"/>
+      <c r="I3" s="25" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="140" x14ac:dyDescent="0.35">
+      <c r="A4" s="43"/>
       <c r="B4" s="23" t="s">
         <v>12</v>
       </c>
@@ -11151,10 +11167,12 @@
       <c r="H4" s="25" t="s">
         <v>55</v>
       </c>
-      <c r="I4" s="25"/>
-    </row>
-    <row r="5" spans="1:9" ht="52.5" x14ac:dyDescent="0.35">
-      <c r="A5" s="42"/>
+      <c r="I4" s="25" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="52.5" x14ac:dyDescent="0.35">
+      <c r="A5" s="43"/>
       <c r="B5" s="23" t="s">
         <v>9</v>
       </c>
@@ -11176,9 +11194,12 @@
       <c r="H5" s="25" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" ht="192.5" x14ac:dyDescent="0.35">
-      <c r="A6" s="41" t="s">
+      <c r="I5" s="25" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="192.5" x14ac:dyDescent="0.35">
+      <c r="A6" s="42" t="s">
         <v>14</v>
       </c>
       <c r="B6" s="23" t="s">
@@ -11202,10 +11223,12 @@
       <c r="H6" s="25" t="s">
         <v>55</v>
       </c>
-      <c r="I6" s="26"/>
-    </row>
-    <row r="7" spans="1:9" ht="140" x14ac:dyDescent="0.35">
-      <c r="A7" s="42"/>
+      <c r="I6" s="25" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="140" x14ac:dyDescent="0.35">
+      <c r="A7" s="43"/>
       <c r="B7" s="23" t="s">
         <v>8</v>
       </c>
@@ -11227,10 +11250,12 @@
       <c r="H7" s="25" t="s">
         <v>55</v>
       </c>
-      <c r="I7" s="25"/>
-    </row>
-    <row r="8" spans="1:9" ht="52.5" x14ac:dyDescent="0.35">
-      <c r="A8" s="42"/>
+      <c r="I7" s="25" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="52.5" x14ac:dyDescent="0.35">
+      <c r="A8" s="43"/>
       <c r="B8" s="23" t="s">
         <v>9</v>
       </c>
@@ -11252,9 +11277,12 @@
       <c r="H8" s="25" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" ht="157.5" x14ac:dyDescent="0.35">
-      <c r="A9" s="41" t="s">
+      <c r="I8" s="25" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="157.5" x14ac:dyDescent="0.35">
+      <c r="A9" s="42" t="s">
         <v>15</v>
       </c>
       <c r="B9" s="23" t="s">
@@ -11278,10 +11306,12 @@
       <c r="H9" s="25" t="s">
         <v>55</v>
       </c>
-      <c r="I9" s="25"/>
-    </row>
-    <row r="10" spans="1:9" ht="140" x14ac:dyDescent="0.35">
-      <c r="A10" s="42"/>
+      <c r="I9" s="25" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="140" x14ac:dyDescent="0.35">
+      <c r="A10" s="43"/>
       <c r="B10" s="23" t="s">
         <v>8</v>
       </c>
@@ -11303,10 +11333,12 @@
       <c r="H10" s="25" t="s">
         <v>55</v>
       </c>
-      <c r="I10" s="25"/>
-    </row>
-    <row r="11" spans="1:9" ht="52.5" x14ac:dyDescent="0.35">
-      <c r="A11" s="42"/>
+      <c r="I10" s="25" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="52.5" x14ac:dyDescent="0.35">
+      <c r="A11" s="43"/>
       <c r="B11" s="23" t="s">
         <v>9</v>
       </c>
@@ -11328,10 +11360,12 @@
       <c r="H11" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="I11" s="25"/>
-    </row>
-    <row r="12" spans="1:9" ht="192.5" x14ac:dyDescent="0.35">
-      <c r="A12" s="41" t="s">
+      <c r="I11" s="25" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="192.5" x14ac:dyDescent="0.35">
+      <c r="A12" s="42" t="s">
         <v>16</v>
       </c>
       <c r="B12" s="23" t="s">
@@ -11355,10 +11389,12 @@
       <c r="H12" s="25" t="s">
         <v>55</v>
       </c>
-      <c r="I12" s="26"/>
-    </row>
-    <row r="13" spans="1:9" ht="140" x14ac:dyDescent="0.35">
-      <c r="A13" s="42"/>
+      <c r="I12" s="25" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="140" x14ac:dyDescent="0.35">
+      <c r="A13" s="43"/>
       <c r="B13" s="23" t="s">
         <v>8</v>
       </c>
@@ -11380,10 +11416,12 @@
       <c r="H13" s="25" t="s">
         <v>55</v>
       </c>
-      <c r="I13" s="25"/>
-    </row>
-    <row r="14" spans="1:9" ht="52.5" x14ac:dyDescent="0.35">
-      <c r="A14" s="42"/>
+      <c r="I13" s="25" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="52.5" x14ac:dyDescent="0.35">
+      <c r="A14" s="43"/>
       <c r="B14" s="23" t="s">
         <v>9</v>
       </c>
@@ -11405,9 +11443,12 @@
       <c r="H14" s="34" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" ht="192.5" x14ac:dyDescent="0.35">
-      <c r="A15" s="41" t="s">
+      <c r="I14" s="35" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="192.5" x14ac:dyDescent="0.35">
+      <c r="A15" s="42" t="s">
         <v>17</v>
       </c>
       <c r="B15" s="23" t="s">
@@ -11431,10 +11472,15 @@
       <c r="H15" s="25" t="s">
         <v>55</v>
       </c>
-      <c r="I15" s="25"/>
-    </row>
-    <row r="16" spans="1:9" ht="157.5" x14ac:dyDescent="0.35">
-      <c r="A16" s="42"/>
+      <c r="I15" s="25" t="s">
+        <v>55</v>
+      </c>
+      <c r="J15" s="25" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="157.5" x14ac:dyDescent="0.35">
+      <c r="A16" s="43"/>
       <c r="B16" s="23" t="s">
         <v>8</v>
       </c>
@@ -11456,10 +11502,15 @@
       <c r="H16" s="25" t="s">
         <v>55</v>
       </c>
-      <c r="I16" s="25"/>
-    </row>
-    <row r="17" spans="1:9" ht="52.5" x14ac:dyDescent="0.35">
-      <c r="A17" s="42"/>
+      <c r="I16" s="25" t="s">
+        <v>55</v>
+      </c>
+      <c r="J16" s="25" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="52.5" x14ac:dyDescent="0.35">
+      <c r="A17" s="43"/>
       <c r="B17" s="23" t="s">
         <v>9</v>
       </c>
@@ -11481,7 +11532,12 @@
       <c r="H17" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="I17" s="25"/>
+      <c r="I17" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="J17" s="25" t="s">
+        <v>30</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="8">

</xml_diff>

<commit_message>
updated du (week10 mon)
</commit_message>
<xml_diff>
--- a/metrics/du.xlsx
+++ b/metrics/du.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\project-g4t6\metrics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39F041C1-E36C-449D-95E7-964463720E97}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D53365CA-5502-4255-A3EF-EA607F1BF195}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9850" yWindow="590" windowWidth="9280" windowHeight="7360" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Week 5" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="Week 7" sheetId="4" r:id="rId3"/>
     <sheet name="Week 8" sheetId="5" r:id="rId4"/>
     <sheet name="Week 9" sheetId="6" r:id="rId5"/>
+    <sheet name="Week 10" sheetId="7" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="769" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="814" uniqueCount="93">
   <si>
     <t>Question</t>
   </si>
@@ -321,6 +322,9 @@
     <t>(1) Updated schedule
 (2) Finished running testcases for bid.csv</t>
   </si>
+  <si>
+    <t>Nade changes to testcases for bid.csv</t>
+  </si>
 </sst>
 </file>
 
@@ -399,7 +403,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -500,19 +504,25 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -840,36 +850,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="41" t="s">
+      <c r="A1" s="40" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="36" t="s">
+      <c r="B1" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="38" t="s">
+      <c r="C1" s="43" t="s">
         <v>18</v>
       </c>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="38"/>
-      <c r="G1" s="38"/>
-      <c r="H1" s="38"/>
-      <c r="I1" s="38"/>
-      <c r="J1" s="41" t="s">
+      <c r="D1" s="43"/>
+      <c r="E1" s="43"/>
+      <c r="F1" s="43"/>
+      <c r="G1" s="43"/>
+      <c r="H1" s="43"/>
+      <c r="I1" s="43"/>
+      <c r="J1" s="40" t="s">
         <v>1</v>
       </c>
-      <c r="K1" s="36" t="s">
+      <c r="K1" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="L1" s="38" t="s">
+      <c r="L1" s="43" t="s">
         <v>40</v>
       </c>
-      <c r="M1" s="38"/>
-      <c r="N1" s="38"/>
-      <c r="O1" s="38"/>
-      <c r="P1" s="38"/>
-      <c r="Q1" s="38"/>
-      <c r="R1" s="38"/>
+      <c r="M1" s="43"/>
+      <c r="N1" s="43"/>
+      <c r="O1" s="43"/>
+      <c r="P1" s="43"/>
+      <c r="Q1" s="43"/>
+      <c r="R1" s="43"/>
       <c r="S1" s="1"/>
       <c r="T1" s="1"/>
       <c r="U1" s="1"/>
@@ -880,8 +890,8 @@
       <c r="Z1" s="1"/>
     </row>
     <row r="2" spans="1:26" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="37"/>
-      <c r="B2" s="37"/>
+      <c r="A2" s="39"/>
+      <c r="B2" s="39"/>
       <c r="C2" s="3" t="s">
         <v>2</v>
       </c>
@@ -903,8 +913,8 @@
       <c r="I2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="J2" s="37"/>
-      <c r="K2" s="37"/>
+      <c r="J2" s="39"/>
+      <c r="K2" s="39"/>
       <c r="L2" s="3" t="s">
         <v>2</v>
       </c>
@@ -936,7 +946,7 @@
       <c r="Z2" s="1"/>
     </row>
     <row r="3" spans="1:26" ht="47.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="39" t="s">
+      <c r="A3" s="41" t="s">
         <v>13</v>
       </c>
       <c r="B3" s="4" t="s">
@@ -955,7 +965,7 @@
       <c r="I3" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="J3" s="39" t="s">
+      <c r="J3" s="41" t="s">
         <v>13</v>
       </c>
       <c r="K3" s="4" t="s">
@@ -984,7 +994,7 @@
       </c>
     </row>
     <row r="4" spans="1:26" ht="63" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="40"/>
+      <c r="A4" s="42"/>
       <c r="B4" s="4" t="s">
         <v>12</v>
       </c>
@@ -1001,7 +1011,7 @@
       <c r="I4" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="J4" s="40"/>
+      <c r="J4" s="42"/>
       <c r="K4" s="4" t="s">
         <v>12</v>
       </c>
@@ -1028,7 +1038,7 @@
       </c>
     </row>
     <row r="5" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="40"/>
+      <c r="A5" s="42"/>
       <c r="B5" s="4" t="s">
         <v>9</v>
       </c>
@@ -1045,7 +1055,7 @@
       <c r="I5" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="J5" s="40"/>
+      <c r="J5" s="42"/>
       <c r="K5" s="4" t="s">
         <v>9</v>
       </c>
@@ -1072,7 +1082,7 @@
       </c>
     </row>
     <row r="6" spans="1:26" ht="62.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="39" t="s">
+      <c r="A6" s="41" t="s">
         <v>14</v>
       </c>
       <c r="B6" s="4" t="s">
@@ -1091,7 +1101,7 @@
       <c r="I6" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="J6" s="39" t="s">
+      <c r="J6" s="41" t="s">
         <v>14</v>
       </c>
       <c r="K6" s="4" t="s">
@@ -1120,7 +1130,7 @@
       </c>
     </row>
     <row r="7" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="40"/>
+      <c r="A7" s="42"/>
       <c r="B7" s="4" t="s">
         <v>8</v>
       </c>
@@ -1137,7 +1147,7 @@
       <c r="I7" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="J7" s="40"/>
+      <c r="J7" s="42"/>
       <c r="K7" s="4" t="s">
         <v>8</v>
       </c>
@@ -1164,7 +1174,7 @@
       </c>
     </row>
     <row r="8" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="40"/>
+      <c r="A8" s="42"/>
       <c r="B8" s="4" t="s">
         <v>9</v>
       </c>
@@ -1181,7 +1191,7 @@
       <c r="I8" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="J8" s="40"/>
+      <c r="J8" s="42"/>
       <c r="K8" s="4" t="s">
         <v>9</v>
       </c>
@@ -1208,7 +1218,7 @@
       </c>
     </row>
     <row r="9" spans="1:26" ht="64.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="39" t="s">
+      <c r="A9" s="41" t="s">
         <v>15</v>
       </c>
       <c r="B9" s="4" t="s">
@@ -1227,7 +1237,7 @@
       <c r="I9" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="J9" s="39" t="s">
+      <c r="J9" s="41" t="s">
         <v>15</v>
       </c>
       <c r="K9" s="4" t="s">
@@ -1256,7 +1266,7 @@
       </c>
     </row>
     <row r="10" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="40"/>
+      <c r="A10" s="42"/>
       <c r="B10" s="4" t="s">
         <v>8</v>
       </c>
@@ -1273,7 +1283,7 @@
       <c r="I10" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="J10" s="40"/>
+      <c r="J10" s="42"/>
       <c r="K10" s="4" t="s">
         <v>8</v>
       </c>
@@ -1300,7 +1310,7 @@
       </c>
     </row>
     <row r="11" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="40"/>
+      <c r="A11" s="42"/>
       <c r="B11" s="4" t="s">
         <v>9</v>
       </c>
@@ -1317,7 +1327,7 @@
       <c r="I11" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="J11" s="40"/>
+      <c r="J11" s="42"/>
       <c r="K11" s="4" t="s">
         <v>9</v>
       </c>
@@ -1344,7 +1354,7 @@
       </c>
     </row>
     <row r="12" spans="1:26" ht="64.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="39" t="s">
+      <c r="A12" s="41" t="s">
         <v>16</v>
       </c>
       <c r="B12" s="4" t="s">
@@ -1363,7 +1373,7 @@
       <c r="I12" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="J12" s="39" t="s">
+      <c r="J12" s="41" t="s">
         <v>16</v>
       </c>
       <c r="K12" s="4" t="s">
@@ -1392,7 +1402,7 @@
       </c>
     </row>
     <row r="13" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="40"/>
+      <c r="A13" s="42"/>
       <c r="B13" s="4" t="s">
         <v>8</v>
       </c>
@@ -1409,7 +1419,7 @@
       <c r="I13" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="J13" s="40"/>
+      <c r="J13" s="42"/>
       <c r="K13" s="4" t="s">
         <v>8</v>
       </c>
@@ -1436,7 +1446,7 @@
       </c>
     </row>
     <row r="14" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="40"/>
+      <c r="A14" s="42"/>
       <c r="B14" s="4" t="s">
         <v>9</v>
       </c>
@@ -1453,7 +1463,7 @@
       <c r="I14" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="J14" s="40"/>
+      <c r="J14" s="42"/>
       <c r="K14" s="4" t="s">
         <v>9</v>
       </c>
@@ -1480,7 +1490,7 @@
       </c>
     </row>
     <row r="15" spans="1:26" ht="64.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="39" t="s">
+      <c r="A15" s="41" t="s">
         <v>17</v>
       </c>
       <c r="B15" s="4" t="s">
@@ -1499,7 +1509,7 @@
       <c r="I15" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="J15" s="39" t="s">
+      <c r="J15" s="41" t="s">
         <v>17</v>
       </c>
       <c r="K15" s="4" t="s">
@@ -1528,7 +1538,7 @@
       </c>
     </row>
     <row r="16" spans="1:26" ht="77.400000000000006" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="40"/>
+      <c r="A16" s="42"/>
       <c r="B16" s="4" t="s">
         <v>8</v>
       </c>
@@ -1545,7 +1555,7 @@
       <c r="I16" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="J16" s="40"/>
+      <c r="J16" s="42"/>
       <c r="K16" s="4" t="s">
         <v>8</v>
       </c>
@@ -1572,7 +1582,7 @@
       </c>
     </row>
     <row r="17" spans="1:18" ht="63.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="40"/>
+      <c r="A17" s="42"/>
       <c r="B17" s="4" t="s">
         <v>9</v>
       </c>
@@ -1589,7 +1599,7 @@
       <c r="I17" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="J17" s="40"/>
+      <c r="J17" s="42"/>
       <c r="K17" s="4" t="s">
         <v>9</v>
       </c>
@@ -5553,6 +5563,11 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="K1:K2"/>
+    <mergeCell ref="L1:R1"/>
+    <mergeCell ref="J3:J5"/>
+    <mergeCell ref="J6:J8"/>
+    <mergeCell ref="C1:I1"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="J15:J17"/>
@@ -5564,11 +5579,6 @@
     <mergeCell ref="A3:A5"/>
     <mergeCell ref="A6:A8"/>
     <mergeCell ref="A9:A11"/>
-    <mergeCell ref="K1:K2"/>
-    <mergeCell ref="L1:R1"/>
-    <mergeCell ref="J3:J5"/>
-    <mergeCell ref="J6:J8"/>
-    <mergeCell ref="C1:I1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -5602,24 +5612,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="41" t="s">
+      <c r="A1" s="40" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="36" t="s">
+      <c r="B1" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="36" t="s">
+      <c r="C1" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="38" t="s">
+      <c r="D1" s="43" t="s">
         <v>41</v>
       </c>
-      <c r="E1" s="38"/>
-      <c r="F1" s="38"/>
-      <c r="G1" s="38"/>
-      <c r="H1" s="38"/>
-      <c r="I1" s="38"/>
-      <c r="J1" s="38"/>
+      <c r="E1" s="43"/>
+      <c r="F1" s="43"/>
+      <c r="G1" s="43"/>
+      <c r="H1" s="43"/>
+      <c r="I1" s="43"/>
+      <c r="J1" s="43"/>
       <c r="S1" s="1"/>
       <c r="T1" s="1"/>
       <c r="U1" s="1"/>
@@ -5630,9 +5640,9 @@
       <c r="Z1" s="1"/>
     </row>
     <row r="2" spans="1:26" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="37"/>
-      <c r="B2" s="37"/>
-      <c r="C2" s="37"/>
+      <c r="A2" s="39"/>
+      <c r="B2" s="39"/>
+      <c r="C2" s="39"/>
       <c r="D2" s="3" t="s">
         <v>2</v>
       </c>
@@ -5664,7 +5674,7 @@
       <c r="Z2" s="1"/>
     </row>
     <row r="3" spans="1:26" ht="47.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="39" t="s">
+      <c r="A3" s="41" t="s">
         <v>13</v>
       </c>
       <c r="B3" s="4" t="s">
@@ -5696,7 +5706,7 @@
       </c>
     </row>
     <row r="4" spans="1:26" ht="63" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="40"/>
+      <c r="A4" s="42"/>
       <c r="B4" s="4" t="s">
         <v>12</v>
       </c>
@@ -5726,7 +5736,7 @@
       </c>
     </row>
     <row r="5" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="40"/>
+      <c r="A5" s="42"/>
       <c r="B5" s="4" t="s">
         <v>9</v>
       </c>
@@ -5756,7 +5766,7 @@
       </c>
     </row>
     <row r="6" spans="1:26" ht="62.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="39" t="s">
+      <c r="A6" s="41" t="s">
         <v>14</v>
       </c>
       <c r="B6" s="4" t="s">
@@ -5788,7 +5798,7 @@
       </c>
     </row>
     <row r="7" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="40"/>
+      <c r="A7" s="42"/>
       <c r="B7" s="4" t="s">
         <v>8</v>
       </c>
@@ -5818,7 +5828,7 @@
       </c>
     </row>
     <row r="8" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="40"/>
+      <c r="A8" s="42"/>
       <c r="B8" s="4" t="s">
         <v>9</v>
       </c>
@@ -5848,7 +5858,7 @@
       </c>
     </row>
     <row r="9" spans="1:26" ht="64.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="39" t="s">
+      <c r="A9" s="41" t="s">
         <v>15</v>
       </c>
       <c r="B9" s="4" t="s">
@@ -5880,7 +5890,7 @@
       </c>
     </row>
     <row r="10" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="40"/>
+      <c r="A10" s="42"/>
       <c r="B10" s="4" t="s">
         <v>8</v>
       </c>
@@ -5910,7 +5920,7 @@
       </c>
     </row>
     <row r="11" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="40"/>
+      <c r="A11" s="42"/>
       <c r="B11" s="4" t="s">
         <v>9</v>
       </c>
@@ -5940,7 +5950,7 @@
       </c>
     </row>
     <row r="12" spans="1:26" ht="64.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="39" t="s">
+      <c r="A12" s="41" t="s">
         <v>16</v>
       </c>
       <c r="B12" s="4" t="s">
@@ -5972,7 +5982,7 @@
       </c>
     </row>
     <row r="13" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="40"/>
+      <c r="A13" s="42"/>
       <c r="B13" s="4" t="s">
         <v>8</v>
       </c>
@@ -6002,7 +6012,7 @@
       </c>
     </row>
     <row r="14" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="40"/>
+      <c r="A14" s="42"/>
       <c r="B14" s="4" t="s">
         <v>9</v>
       </c>
@@ -6032,7 +6042,7 @@
       </c>
     </row>
     <row r="15" spans="1:26" ht="64.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="39" t="s">
+      <c r="A15" s="41" t="s">
         <v>17</v>
       </c>
       <c r="B15" s="4" t="s">
@@ -6064,7 +6074,7 @@
       </c>
     </row>
     <row r="16" spans="1:26" ht="77.400000000000006" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="40"/>
+      <c r="A16" s="42"/>
       <c r="B16" s="4" t="s">
         <v>8</v>
       </c>
@@ -6094,7 +6104,7 @@
       </c>
     </row>
     <row r="17" spans="1:10" ht="63.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="40"/>
+      <c r="A17" s="42"/>
       <c r="B17" s="4" t="s">
         <v>9</v>
       </c>
@@ -10090,25 +10100,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="18" x14ac:dyDescent="0.4">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="47" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="45" t="s">
+      <c r="B1" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="44" t="s">
+      <c r="C1" s="46" t="s">
         <v>42</v>
       </c>
-      <c r="D1" s="44"/>
-      <c r="E1" s="44"/>
-      <c r="F1" s="44"/>
-      <c r="G1" s="44"/>
-      <c r="H1" s="44"/>
-      <c r="I1" s="44"/>
+      <c r="D1" s="46"/>
+      <c r="E1" s="46"/>
+      <c r="F1" s="46"/>
+      <c r="G1" s="46"/>
+      <c r="H1" s="46"/>
+      <c r="I1" s="46"/>
     </row>
     <row r="2" spans="1:9" ht="18" x14ac:dyDescent="0.4">
-      <c r="A2" s="46"/>
-      <c r="B2" s="46"/>
+      <c r="A2" s="48"/>
+      <c r="B2" s="48"/>
       <c r="C2" s="14" t="s">
         <v>2</v>
       </c>
@@ -10132,7 +10142,7 @@
       </c>
     </row>
     <row r="3" spans="1:9" ht="87.5" x14ac:dyDescent="0.35">
-      <c r="A3" s="42" t="s">
+      <c r="A3" s="44" t="s">
         <v>13</v>
       </c>
       <c r="B3" s="15" t="s">
@@ -10161,7 +10171,7 @@
       </c>
     </row>
     <row r="4" spans="1:9" ht="105" x14ac:dyDescent="0.35">
-      <c r="A4" s="43"/>
+      <c r="A4" s="45"/>
       <c r="B4" s="15" t="s">
         <v>12</v>
       </c>
@@ -10188,7 +10198,7 @@
       </c>
     </row>
     <row r="5" spans="1:9" ht="52.5" x14ac:dyDescent="0.35">
-      <c r="A5" s="43"/>
+      <c r="A5" s="45"/>
       <c r="B5" s="15" t="s">
         <v>9</v>
       </c>
@@ -10215,7 +10225,7 @@
       </c>
     </row>
     <row r="6" spans="1:9" ht="157.5" x14ac:dyDescent="0.35">
-      <c r="A6" s="42" t="s">
+      <c r="A6" s="44" t="s">
         <v>14</v>
       </c>
       <c r="B6" s="15" t="s">
@@ -10244,7 +10254,7 @@
       </c>
     </row>
     <row r="7" spans="1:9" ht="157.5" x14ac:dyDescent="0.35">
-      <c r="A7" s="43"/>
+      <c r="A7" s="45"/>
       <c r="B7" s="15" t="s">
         <v>8</v>
       </c>
@@ -10271,7 +10281,7 @@
       </c>
     </row>
     <row r="8" spans="1:9" ht="70" x14ac:dyDescent="0.35">
-      <c r="A8" s="43"/>
+      <c r="A8" s="45"/>
       <c r="B8" s="15" t="s">
         <v>9</v>
       </c>
@@ -10298,7 +10308,7 @@
       </c>
     </row>
     <row r="9" spans="1:9" ht="140" x14ac:dyDescent="0.35">
-      <c r="A9" s="42" t="s">
+      <c r="A9" s="44" t="s">
         <v>15</v>
       </c>
       <c r="B9" s="15" t="s">
@@ -10327,7 +10337,7 @@
       </c>
     </row>
     <row r="10" spans="1:9" ht="157.5" x14ac:dyDescent="0.35">
-      <c r="A10" s="43"/>
+      <c r="A10" s="45"/>
       <c r="B10" s="15" t="s">
         <v>8</v>
       </c>
@@ -10354,7 +10364,7 @@
       </c>
     </row>
     <row r="11" spans="1:9" ht="70" x14ac:dyDescent="0.35">
-      <c r="A11" s="43"/>
+      <c r="A11" s="45"/>
       <c r="B11" s="15" t="s">
         <v>9</v>
       </c>
@@ -10381,7 +10391,7 @@
       </c>
     </row>
     <row r="12" spans="1:9" ht="157.5" x14ac:dyDescent="0.35">
-      <c r="A12" s="42" t="s">
+      <c r="A12" s="44" t="s">
         <v>16</v>
       </c>
       <c r="B12" s="15" t="s">
@@ -10410,7 +10420,7 @@
       </c>
     </row>
     <row r="13" spans="1:9" ht="157.5" x14ac:dyDescent="0.35">
-      <c r="A13" s="43"/>
+      <c r="A13" s="45"/>
       <c r="B13" s="15" t="s">
         <v>8</v>
       </c>
@@ -10437,7 +10447,7 @@
       </c>
     </row>
     <row r="14" spans="1:9" ht="175" x14ac:dyDescent="0.35">
-      <c r="A14" s="43"/>
+      <c r="A14" s="45"/>
       <c r="B14" s="15" t="s">
         <v>9</v>
       </c>
@@ -10464,7 +10474,7 @@
       </c>
     </row>
     <row r="15" spans="1:9" ht="105" x14ac:dyDescent="0.35">
-      <c r="A15" s="42" t="s">
+      <c r="A15" s="44" t="s">
         <v>17</v>
       </c>
       <c r="B15" s="15" t="s">
@@ -10493,7 +10503,7 @@
       </c>
     </row>
     <row r="16" spans="1:9" ht="157.5" x14ac:dyDescent="0.35">
-      <c r="A16" s="43"/>
+      <c r="A16" s="45"/>
       <c r="B16" s="15" t="s">
         <v>8</v>
       </c>
@@ -10520,7 +10530,7 @@
       </c>
     </row>
     <row r="17" spans="1:9" ht="70" x14ac:dyDescent="0.35">
-      <c r="A17" s="43"/>
+      <c r="A17" s="45"/>
       <c r="B17" s="15" t="s">
         <v>9</v>
       </c>
@@ -10581,25 +10591,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="18" x14ac:dyDescent="0.4">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="47" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="45" t="s">
+      <c r="B1" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="44" t="s">
+      <c r="C1" s="46" t="s">
         <v>64</v>
       </c>
-      <c r="D1" s="44"/>
-      <c r="E1" s="44"/>
-      <c r="F1" s="44"/>
-      <c r="G1" s="44"/>
-      <c r="H1" s="44"/>
-      <c r="I1" s="44"/>
+      <c r="D1" s="46"/>
+      <c r="E1" s="46"/>
+      <c r="F1" s="46"/>
+      <c r="G1" s="46"/>
+      <c r="H1" s="46"/>
+      <c r="I1" s="46"/>
     </row>
     <row r="2" spans="1:9" ht="18" x14ac:dyDescent="0.4">
-      <c r="A2" s="46"/>
-      <c r="B2" s="46"/>
+      <c r="A2" s="48"/>
+      <c r="B2" s="48"/>
       <c r="C2" s="14" t="s">
         <v>2</v>
       </c>
@@ -10623,7 +10633,7 @@
       </c>
     </row>
     <row r="3" spans="1:9" ht="105" x14ac:dyDescent="0.35">
-      <c r="A3" s="42" t="s">
+      <c r="A3" s="44" t="s">
         <v>13</v>
       </c>
       <c r="B3" s="21" t="s">
@@ -10652,7 +10662,7 @@
       </c>
     </row>
     <row r="4" spans="1:9" ht="105" x14ac:dyDescent="0.35">
-      <c r="A4" s="43"/>
+      <c r="A4" s="45"/>
       <c r="B4" s="21" t="s">
         <v>12</v>
       </c>
@@ -10679,7 +10689,7 @@
       </c>
     </row>
     <row r="5" spans="1:9" ht="87.5" x14ac:dyDescent="0.35">
-      <c r="A5" s="43"/>
+      <c r="A5" s="45"/>
       <c r="B5" s="21" t="s">
         <v>9</v>
       </c>
@@ -10706,7 +10716,7 @@
       </c>
     </row>
     <row r="6" spans="1:9" ht="122.5" x14ac:dyDescent="0.35">
-      <c r="A6" s="42" t="s">
+      <c r="A6" s="44" t="s">
         <v>14</v>
       </c>
       <c r="B6" s="21" t="s">
@@ -10735,7 +10745,7 @@
       </c>
     </row>
     <row r="7" spans="1:9" ht="105" x14ac:dyDescent="0.35">
-      <c r="A7" s="43"/>
+      <c r="A7" s="45"/>
       <c r="B7" s="21" t="s">
         <v>8</v>
       </c>
@@ -10762,7 +10772,7 @@
       </c>
     </row>
     <row r="8" spans="1:9" ht="105" x14ac:dyDescent="0.35">
-      <c r="A8" s="43"/>
+      <c r="A8" s="45"/>
       <c r="B8" s="21" t="s">
         <v>9</v>
       </c>
@@ -10789,7 +10799,7 @@
       </c>
     </row>
     <row r="9" spans="1:9" ht="70" x14ac:dyDescent="0.35">
-      <c r="A9" s="42" t="s">
+      <c r="A9" s="44" t="s">
         <v>15</v>
       </c>
       <c r="B9" s="21" t="s">
@@ -10818,7 +10828,7 @@
       </c>
     </row>
     <row r="10" spans="1:9" ht="52.5" x14ac:dyDescent="0.35">
-      <c r="A10" s="43"/>
+      <c r="A10" s="45"/>
       <c r="B10" s="21" t="s">
         <v>8</v>
       </c>
@@ -10845,7 +10855,7 @@
       </c>
     </row>
     <row r="11" spans="1:9" ht="157.5" x14ac:dyDescent="0.35">
-      <c r="A11" s="43"/>
+      <c r="A11" s="45"/>
       <c r="B11" s="21" t="s">
         <v>9</v>
       </c>
@@ -10872,7 +10882,7 @@
       </c>
     </row>
     <row r="12" spans="1:9" ht="192.5" x14ac:dyDescent="0.35">
-      <c r="A12" s="42" t="s">
+      <c r="A12" s="44" t="s">
         <v>16</v>
       </c>
       <c r="B12" s="21" t="s">
@@ -10901,7 +10911,7 @@
       </c>
     </row>
     <row r="13" spans="1:9" ht="192.5" x14ac:dyDescent="0.35">
-      <c r="A13" s="43"/>
+      <c r="A13" s="45"/>
       <c r="B13" s="21" t="s">
         <v>8</v>
       </c>
@@ -10928,7 +10938,7 @@
       </c>
     </row>
     <row r="14" spans="1:9" ht="87.5" x14ac:dyDescent="0.35">
-      <c r="A14" s="43"/>
+      <c r="A14" s="45"/>
       <c r="B14" s="21" t="s">
         <v>9</v>
       </c>
@@ -10955,7 +10965,7 @@
       </c>
     </row>
     <row r="15" spans="1:9" ht="70" x14ac:dyDescent="0.35">
-      <c r="A15" s="42" t="s">
+      <c r="A15" s="44" t="s">
         <v>17</v>
       </c>
       <c r="B15" s="21" t="s">
@@ -10984,7 +10994,7 @@
       </c>
     </row>
     <row r="16" spans="1:9" ht="52.5" x14ac:dyDescent="0.35">
-      <c r="A16" s="43"/>
+      <c r="A16" s="45"/>
       <c r="B16" s="21" t="s">
         <v>8</v>
       </c>
@@ -11011,7 +11021,7 @@
       </c>
     </row>
     <row r="17" spans="1:9" ht="157.5" x14ac:dyDescent="0.35">
-      <c r="A17" s="43"/>
+      <c r="A17" s="45"/>
       <c r="B17" s="21" t="s">
         <v>9</v>
       </c>
@@ -11057,8 +11067,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B762D8C-72F3-45B7-9544-A442629D54B9}">
   <dimension ref="A1:J17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1"/>
+    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection sqref="A1:A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.453125" defaultRowHeight="17.5" x14ac:dyDescent="0.35"/>
@@ -11074,25 +11084,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="18" x14ac:dyDescent="0.4">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="47" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="45" t="s">
+      <c r="B1" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="44" t="s">
+      <c r="C1" s="46" t="s">
         <v>64</v>
       </c>
-      <c r="D1" s="44"/>
-      <c r="E1" s="44"/>
-      <c r="F1" s="44"/>
-      <c r="G1" s="44"/>
-      <c r="H1" s="44"/>
-      <c r="I1" s="44"/>
+      <c r="D1" s="46"/>
+      <c r="E1" s="46"/>
+      <c r="F1" s="46"/>
+      <c r="G1" s="46"/>
+      <c r="H1" s="46"/>
+      <c r="I1" s="46"/>
     </row>
     <row r="2" spans="1:10" ht="18" x14ac:dyDescent="0.4">
-      <c r="A2" s="46"/>
-      <c r="B2" s="46"/>
+      <c r="A2" s="48"/>
+      <c r="B2" s="48"/>
       <c r="C2" s="14" t="s">
         <v>2</v>
       </c>
@@ -11116,7 +11126,7 @@
       </c>
     </row>
     <row r="3" spans="1:10" ht="192.5" x14ac:dyDescent="0.35">
-      <c r="A3" s="42" t="s">
+      <c r="A3" s="44" t="s">
         <v>13</v>
       </c>
       <c r="B3" s="23" t="s">
@@ -11145,7 +11155,7 @@
       </c>
     </row>
     <row r="4" spans="1:10" ht="140" x14ac:dyDescent="0.35">
-      <c r="A4" s="43"/>
+      <c r="A4" s="45"/>
       <c r="B4" s="23" t="s">
         <v>12</v>
       </c>
@@ -11172,7 +11182,7 @@
       </c>
     </row>
     <row r="5" spans="1:10" ht="52.5" x14ac:dyDescent="0.35">
-      <c r="A5" s="43"/>
+      <c r="A5" s="45"/>
       <c r="B5" s="23" t="s">
         <v>9</v>
       </c>
@@ -11199,7 +11209,7 @@
       </c>
     </row>
     <row r="6" spans="1:10" ht="192.5" x14ac:dyDescent="0.35">
-      <c r="A6" s="42" t="s">
+      <c r="A6" s="44" t="s">
         <v>14</v>
       </c>
       <c r="B6" s="23" t="s">
@@ -11228,7 +11238,7 @@
       </c>
     </row>
     <row r="7" spans="1:10" ht="140" x14ac:dyDescent="0.35">
-      <c r="A7" s="43"/>
+      <c r="A7" s="45"/>
       <c r="B7" s="23" t="s">
         <v>8</v>
       </c>
@@ -11255,7 +11265,7 @@
       </c>
     </row>
     <row r="8" spans="1:10" ht="52.5" x14ac:dyDescent="0.35">
-      <c r="A8" s="43"/>
+      <c r="A8" s="45"/>
       <c r="B8" s="23" t="s">
         <v>9</v>
       </c>
@@ -11282,7 +11292,7 @@
       </c>
     </row>
     <row r="9" spans="1:10" ht="157.5" x14ac:dyDescent="0.35">
-      <c r="A9" s="42" t="s">
+      <c r="A9" s="44" t="s">
         <v>15</v>
       </c>
       <c r="B9" s="23" t="s">
@@ -11311,7 +11321,7 @@
       </c>
     </row>
     <row r="10" spans="1:10" ht="140" x14ac:dyDescent="0.35">
-      <c r="A10" s="43"/>
+      <c r="A10" s="45"/>
       <c r="B10" s="23" t="s">
         <v>8</v>
       </c>
@@ -11338,7 +11348,7 @@
       </c>
     </row>
     <row r="11" spans="1:10" ht="52.5" x14ac:dyDescent="0.35">
-      <c r="A11" s="43"/>
+      <c r="A11" s="45"/>
       <c r="B11" s="23" t="s">
         <v>9</v>
       </c>
@@ -11365,7 +11375,7 @@
       </c>
     </row>
     <row r="12" spans="1:10" ht="192.5" x14ac:dyDescent="0.35">
-      <c r="A12" s="42" t="s">
+      <c r="A12" s="44" t="s">
         <v>16</v>
       </c>
       <c r="B12" s="23" t="s">
@@ -11394,7 +11404,7 @@
       </c>
     </row>
     <row r="13" spans="1:10" ht="140" x14ac:dyDescent="0.35">
-      <c r="A13" s="43"/>
+      <c r="A13" s="45"/>
       <c r="B13" s="23" t="s">
         <v>8</v>
       </c>
@@ -11421,7 +11431,7 @@
       </c>
     </row>
     <row r="14" spans="1:10" ht="52.5" x14ac:dyDescent="0.35">
-      <c r="A14" s="43"/>
+      <c r="A14" s="45"/>
       <c r="B14" s="23" t="s">
         <v>9</v>
       </c>
@@ -11448,7 +11458,7 @@
       </c>
     </row>
     <row r="15" spans="1:10" ht="192.5" x14ac:dyDescent="0.35">
-      <c r="A15" s="42" t="s">
+      <c r="A15" s="44" t="s">
         <v>17</v>
       </c>
       <c r="B15" s="23" t="s">
@@ -11480,7 +11490,7 @@
       </c>
     </row>
     <row r="16" spans="1:10" ht="157.5" x14ac:dyDescent="0.35">
-      <c r="A16" s="43"/>
+      <c r="A16" s="45"/>
       <c r="B16" s="23" t="s">
         <v>8</v>
       </c>
@@ -11510,7 +11520,7 @@
       </c>
     </row>
     <row r="17" spans="1:10" ht="52.5" x14ac:dyDescent="0.35">
-      <c r="A17" s="43"/>
+      <c r="A17" s="45"/>
       <c r="B17" s="23" t="s">
         <v>9</v>
       </c>
@@ -11538,6 +11548,314 @@
       <c r="J17" s="25" t="s">
         <v>30</v>
       </c>
+    </row>
+  </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="A12:A14"/>
+    <mergeCell ref="A15:A17"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:I1"/>
+    <mergeCell ref="A3:A5"/>
+    <mergeCell ref="A6:A8"/>
+    <mergeCell ref="A9:A11"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B35242D0-2AD6-442D-ABA4-BF0550EDBCE1}">
+  <dimension ref="A1:J17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="I17" sqref="I17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="17.453125" defaultRowHeight="17.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="2" width="17.453125" style="37"/>
+    <col min="3" max="3" width="20.54296875" style="37" customWidth="1"/>
+    <col min="4" max="4" width="36.90625" style="37" customWidth="1"/>
+    <col min="5" max="5" width="26.6328125" style="37" customWidth="1"/>
+    <col min="6" max="6" width="26.36328125" style="37" customWidth="1"/>
+    <col min="7" max="7" width="23.54296875" style="37" customWidth="1"/>
+    <col min="8" max="8" width="20.81640625" style="37" customWidth="1"/>
+    <col min="9" max="16384" width="17.453125" style="37"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="18" x14ac:dyDescent="0.4">
+      <c r="A1" s="47" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="47" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="46" t="s">
+        <v>64</v>
+      </c>
+      <c r="D1" s="46"/>
+      <c r="E1" s="46"/>
+      <c r="F1" s="46"/>
+      <c r="G1" s="46"/>
+      <c r="H1" s="46"/>
+      <c r="I1" s="46"/>
+    </row>
+    <row r="2" spans="1:10" ht="18" x14ac:dyDescent="0.4">
+      <c r="A2" s="48"/>
+      <c r="B2" s="48"/>
+      <c r="C2" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="I2" s="14" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="35" x14ac:dyDescent="0.35">
+      <c r="A3" s="44" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="36" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="25" t="s">
+        <v>89</v>
+      </c>
+      <c r="D3" s="25"/>
+      <c r="E3" s="25"/>
+      <c r="F3" s="25"/>
+      <c r="G3" s="25"/>
+      <c r="H3" s="25"/>
+      <c r="I3" s="25"/>
+    </row>
+    <row r="4" spans="1:10" ht="35" x14ac:dyDescent="0.35">
+      <c r="A4" s="45"/>
+      <c r="B4" s="36" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="25" t="s">
+        <v>55</v>
+      </c>
+      <c r="D4" s="25"/>
+      <c r="E4" s="25"/>
+      <c r="F4" s="25"/>
+      <c r="G4" s="25"/>
+      <c r="H4" s="25"/>
+      <c r="I4" s="25"/>
+    </row>
+    <row r="5" spans="1:10" ht="52.5" x14ac:dyDescent="0.35">
+      <c r="A5" s="45"/>
+      <c r="B5" s="36" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="25" t="s">
+        <v>77</v>
+      </c>
+      <c r="D5" s="25"/>
+      <c r="E5" s="25"/>
+      <c r="F5" s="31"/>
+      <c r="G5" s="31"/>
+      <c r="H5" s="25"/>
+      <c r="I5" s="25"/>
+    </row>
+    <row r="6" spans="1:10" ht="87.5" x14ac:dyDescent="0.35">
+      <c r="A6" s="44" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="36" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="25" t="s">
+        <v>90</v>
+      </c>
+      <c r="D6" s="25"/>
+      <c r="E6" s="25"/>
+      <c r="F6" s="25"/>
+      <c r="G6" s="25"/>
+      <c r="H6" s="25"/>
+      <c r="I6" s="25"/>
+    </row>
+    <row r="7" spans="1:10" ht="52.5" x14ac:dyDescent="0.35">
+      <c r="A7" s="45"/>
+      <c r="B7" s="36" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="25" t="s">
+        <v>55</v>
+      </c>
+      <c r="D7" s="25"/>
+      <c r="E7" s="25"/>
+      <c r="F7" s="25"/>
+      <c r="G7" s="25"/>
+      <c r="H7" s="25"/>
+      <c r="I7" s="25"/>
+    </row>
+    <row r="8" spans="1:10" ht="52.5" x14ac:dyDescent="0.35">
+      <c r="A8" s="45"/>
+      <c r="B8" s="36" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="25" t="s">
+        <v>77</v>
+      </c>
+      <c r="D8" s="25"/>
+      <c r="E8" s="25"/>
+      <c r="F8" s="31"/>
+      <c r="G8" s="31"/>
+      <c r="H8" s="25"/>
+      <c r="I8" s="25"/>
+    </row>
+    <row r="9" spans="1:10" ht="105" x14ac:dyDescent="0.35">
+      <c r="A9" s="44" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="36" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="25" t="s">
+        <v>91</v>
+      </c>
+      <c r="D9" s="25"/>
+      <c r="E9" s="25"/>
+      <c r="F9" s="25"/>
+      <c r="H9" s="25"/>
+      <c r="I9" s="25"/>
+    </row>
+    <row r="10" spans="1:10" ht="52.5" x14ac:dyDescent="0.35">
+      <c r="A10" s="45"/>
+      <c r="B10" s="36" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="25" t="s">
+        <v>92</v>
+      </c>
+      <c r="D10" s="25"/>
+      <c r="E10" s="25"/>
+      <c r="G10" s="25"/>
+      <c r="H10" s="25"/>
+      <c r="I10" s="25"/>
+    </row>
+    <row r="11" spans="1:10" ht="52.5" x14ac:dyDescent="0.35">
+      <c r="A11" s="45"/>
+      <c r="B11" s="36" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="D11" s="25"/>
+      <c r="E11" s="25"/>
+      <c r="F11" s="25"/>
+      <c r="G11" s="25"/>
+      <c r="H11" s="25"/>
+      <c r="I11" s="25"/>
+    </row>
+    <row r="12" spans="1:10" ht="35" x14ac:dyDescent="0.35">
+      <c r="A12" s="44" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" s="36" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" s="25" t="s">
+        <v>89</v>
+      </c>
+      <c r="D12" s="25"/>
+      <c r="E12" s="25"/>
+      <c r="F12" s="25"/>
+      <c r="G12" s="25"/>
+      <c r="H12" s="25"/>
+      <c r="I12" s="25"/>
+    </row>
+    <row r="13" spans="1:10" ht="52.5" x14ac:dyDescent="0.35">
+      <c r="A13" s="45"/>
+      <c r="B13" s="36" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" s="25" t="s">
+        <v>55</v>
+      </c>
+      <c r="D13" s="25"/>
+      <c r="E13" s="25"/>
+      <c r="F13" s="25"/>
+      <c r="G13" s="25"/>
+      <c r="H13" s="25"/>
+      <c r="I13" s="25"/>
+    </row>
+    <row r="14" spans="1:10" ht="52.5" x14ac:dyDescent="0.35">
+      <c r="A14" s="45"/>
+      <c r="B14" s="36" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" s="25" t="s">
+        <v>77</v>
+      </c>
+      <c r="D14" s="25"/>
+      <c r="E14" s="25"/>
+    </row>
+    <row r="15" spans="1:10" ht="87.5" x14ac:dyDescent="0.35">
+      <c r="A15" s="44" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15" s="36" t="s">
+        <v>7</v>
+      </c>
+      <c r="C15" s="25" t="s">
+        <v>90</v>
+      </c>
+      <c r="D15" s="25"/>
+      <c r="E15" s="25"/>
+      <c r="F15" s="25"/>
+      <c r="H15" s="25"/>
+      <c r="I15" s="25"/>
+      <c r="J15" s="25"/>
+    </row>
+    <row r="16" spans="1:10" ht="52.5" x14ac:dyDescent="0.35">
+      <c r="A16" s="45"/>
+      <c r="B16" s="36" t="s">
+        <v>8</v>
+      </c>
+      <c r="C16" s="25" t="s">
+        <v>55</v>
+      </c>
+      <c r="D16" s="25"/>
+      <c r="E16" s="25"/>
+      <c r="G16" s="25"/>
+      <c r="H16" s="25"/>
+      <c r="I16" s="25"/>
+      <c r="J16" s="25"/>
+    </row>
+    <row r="17" spans="1:10" ht="52.5" x14ac:dyDescent="0.35">
+      <c r="A17" s="45"/>
+      <c r="B17" s="36" t="s">
+        <v>9</v>
+      </c>
+      <c r="C17" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="D17" s="25"/>
+      <c r="E17" s="25"/>
+      <c r="F17" s="25"/>
+      <c r="G17" s="25"/>
+      <c r="H17" s="25"/>
+      <c r="I17" s="25"/>
+      <c r="J17" s="25"/>
     </row>
   </sheetData>
   <mergeCells count="8">

</xml_diff>

<commit_message>
updated du (week10 tues)
</commit_message>
<xml_diff>
--- a/metrics/du.xlsx
+++ b/metrics/du.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\project-g4t6\metrics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D53365CA-5502-4255-A3EF-EA607F1BF195}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3AC6DE3-2E39-45D7-AFFD-502089EA54B2}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="814" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="829" uniqueCount="93">
   <si>
     <t>Question</t>
   </si>
@@ -514,15 +514,15 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -850,36 +850,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="43" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="43" t="s">
+      <c r="C1" s="40" t="s">
         <v>18</v>
       </c>
-      <c r="D1" s="43"/>
-      <c r="E1" s="43"/>
-      <c r="F1" s="43"/>
-      <c r="G1" s="43"/>
-      <c r="H1" s="43"/>
-      <c r="I1" s="43"/>
-      <c r="J1" s="40" t="s">
+      <c r="D1" s="40"/>
+      <c r="E1" s="40"/>
+      <c r="F1" s="40"/>
+      <c r="G1" s="40"/>
+      <c r="H1" s="40"/>
+      <c r="I1" s="40"/>
+      <c r="J1" s="43" t="s">
         <v>1</v>
       </c>
       <c r="K1" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="L1" s="43" t="s">
+      <c r="L1" s="40" t="s">
         <v>40</v>
       </c>
-      <c r="M1" s="43"/>
-      <c r="N1" s="43"/>
-      <c r="O1" s="43"/>
-      <c r="P1" s="43"/>
-      <c r="Q1" s="43"/>
-      <c r="R1" s="43"/>
+      <c r="M1" s="40"/>
+      <c r="N1" s="40"/>
+      <c r="O1" s="40"/>
+      <c r="P1" s="40"/>
+      <c r="Q1" s="40"/>
+      <c r="R1" s="40"/>
       <c r="S1" s="1"/>
       <c r="T1" s="1"/>
       <c r="U1" s="1"/>
@@ -5563,11 +5563,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="K1:K2"/>
-    <mergeCell ref="L1:R1"/>
-    <mergeCell ref="J3:J5"/>
-    <mergeCell ref="J6:J8"/>
-    <mergeCell ref="C1:I1"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="J15:J17"/>
@@ -5579,6 +5574,11 @@
     <mergeCell ref="A3:A5"/>
     <mergeCell ref="A6:A8"/>
     <mergeCell ref="A9:A11"/>
+    <mergeCell ref="K1:K2"/>
+    <mergeCell ref="L1:R1"/>
+    <mergeCell ref="J3:J5"/>
+    <mergeCell ref="J6:J8"/>
+    <mergeCell ref="C1:I1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -5612,7 +5612,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="43" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="38" t="s">
@@ -5621,15 +5621,15 @@
       <c r="C1" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="43" t="s">
+      <c r="D1" s="40" t="s">
         <v>41</v>
       </c>
-      <c r="E1" s="43"/>
-      <c r="F1" s="43"/>
-      <c r="G1" s="43"/>
-      <c r="H1" s="43"/>
-      <c r="I1" s="43"/>
-      <c r="J1" s="43"/>
+      <c r="E1" s="40"/>
+      <c r="F1" s="40"/>
+      <c r="G1" s="40"/>
+      <c r="H1" s="40"/>
+      <c r="I1" s="40"/>
+      <c r="J1" s="40"/>
       <c r="S1" s="1"/>
       <c r="T1" s="1"/>
       <c r="U1" s="1"/>
@@ -10688,7 +10688,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="87.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" ht="105" x14ac:dyDescent="0.35">
       <c r="A5" s="45"/>
       <c r="B5" s="21" t="s">
         <v>9</v>
@@ -11569,8 +11569,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B35242D0-2AD6-442D-ABA4-BF0550EDBCE1}">
   <dimension ref="A1:J17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.453125" defaultRowHeight="17.5" x14ac:dyDescent="0.35"/>
@@ -11637,7 +11637,9 @@
       <c r="C3" s="25" t="s">
         <v>89</v>
       </c>
-      <c r="D3" s="25"/>
+      <c r="D3" s="25" t="s">
+        <v>55</v>
+      </c>
       <c r="E3" s="25"/>
       <c r="F3" s="25"/>
       <c r="G3" s="25"/>
@@ -11652,7 +11654,9 @@
       <c r="C4" s="25" t="s">
         <v>55</v>
       </c>
-      <c r="D4" s="25"/>
+      <c r="D4" s="25" t="s">
+        <v>55</v>
+      </c>
       <c r="E4" s="25"/>
       <c r="F4" s="25"/>
       <c r="G4" s="25"/>
@@ -11667,7 +11671,9 @@
       <c r="C5" s="25" t="s">
         <v>77</v>
       </c>
-      <c r="D5" s="25"/>
+      <c r="D5" s="25" t="s">
+        <v>77</v>
+      </c>
       <c r="E5" s="25"/>
       <c r="F5" s="31"/>
       <c r="G5" s="31"/>
@@ -11684,7 +11690,9 @@
       <c r="C6" s="25" t="s">
         <v>90</v>
       </c>
-      <c r="D6" s="25"/>
+      <c r="D6" s="25" t="s">
+        <v>55</v>
+      </c>
       <c r="E6" s="25"/>
       <c r="F6" s="25"/>
       <c r="G6" s="25"/>
@@ -11699,7 +11707,9 @@
       <c r="C7" s="25" t="s">
         <v>55</v>
       </c>
-      <c r="D7" s="25"/>
+      <c r="D7" s="25" t="s">
+        <v>55</v>
+      </c>
       <c r="E7" s="25"/>
       <c r="F7" s="25"/>
       <c r="G7" s="25"/>
@@ -11714,7 +11724,9 @@
       <c r="C8" s="25" t="s">
         <v>77</v>
       </c>
-      <c r="D8" s="25"/>
+      <c r="D8" s="25" t="s">
+        <v>77</v>
+      </c>
       <c r="E8" s="25"/>
       <c r="F8" s="31"/>
       <c r="G8" s="31"/>
@@ -11731,7 +11743,9 @@
       <c r="C9" s="25" t="s">
         <v>91</v>
       </c>
-      <c r="D9" s="25"/>
+      <c r="D9" s="25" t="s">
+        <v>92</v>
+      </c>
       <c r="E9" s="25"/>
       <c r="F9" s="25"/>
       <c r="H9" s="25"/>
@@ -11745,7 +11759,9 @@
       <c r="C10" s="25" t="s">
         <v>92</v>
       </c>
-      <c r="D10" s="25"/>
+      <c r="D10" s="25" t="s">
+        <v>55</v>
+      </c>
       <c r="E10" s="25"/>
       <c r="G10" s="25"/>
       <c r="H10" s="25"/>
@@ -11759,7 +11775,9 @@
       <c r="C11" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="D11" s="25"/>
+      <c r="D11" s="25" t="s">
+        <v>30</v>
+      </c>
       <c r="E11" s="25"/>
       <c r="F11" s="25"/>
       <c r="G11" s="25"/>
@@ -11776,7 +11794,9 @@
       <c r="C12" s="25" t="s">
         <v>89</v>
       </c>
-      <c r="D12" s="25"/>
+      <c r="D12" s="25" t="s">
+        <v>55</v>
+      </c>
       <c r="E12" s="25"/>
       <c r="F12" s="25"/>
       <c r="G12" s="25"/>
@@ -11791,7 +11811,9 @@
       <c r="C13" s="25" t="s">
         <v>55</v>
       </c>
-      <c r="D13" s="25"/>
+      <c r="D13" s="25" t="s">
+        <v>55</v>
+      </c>
       <c r="E13" s="25"/>
       <c r="F13" s="25"/>
       <c r="G13" s="25"/>
@@ -11806,7 +11828,9 @@
       <c r="C14" s="25" t="s">
         <v>77</v>
       </c>
-      <c r="D14" s="25"/>
+      <c r="D14" s="25" t="s">
+        <v>77</v>
+      </c>
       <c r="E14" s="25"/>
     </row>
     <row r="15" spans="1:10" ht="87.5" x14ac:dyDescent="0.35">
@@ -11819,7 +11843,9 @@
       <c r="C15" s="25" t="s">
         <v>90</v>
       </c>
-      <c r="D15" s="25"/>
+      <c r="D15" s="25" t="s">
+        <v>55</v>
+      </c>
       <c r="E15" s="25"/>
       <c r="F15" s="25"/>
       <c r="H15" s="25"/>
@@ -11834,7 +11860,9 @@
       <c r="C16" s="25" t="s">
         <v>55</v>
       </c>
-      <c r="D16" s="25"/>
+      <c r="D16" s="25" t="s">
+        <v>55</v>
+      </c>
       <c r="E16" s="25"/>
       <c r="G16" s="25"/>
       <c r="H16" s="25"/>
@@ -11849,7 +11877,9 @@
       <c r="C17" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="D17" s="25"/>
+      <c r="D17" s="25" t="s">
+        <v>30</v>
+      </c>
       <c r="E17" s="25"/>
       <c r="F17" s="25"/>
       <c r="G17" s="25"/>

</xml_diff>

<commit_message>
update du (week10 wed)
</commit_message>
<xml_diff>
--- a/metrics/du.xlsx
+++ b/metrics/du.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\project-g4t6\metrics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3AC6DE3-2E39-45D7-AFFD-502089EA54B2}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{038B6CD9-648A-47A9-9553-3B9295AEC39F}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="829" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="844" uniqueCount="93">
   <si>
     <t>Question</t>
   </si>
@@ -514,15 +514,15 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -850,36 +850,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="40" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="40" t="s">
+      <c r="C1" s="43" t="s">
         <v>18</v>
       </c>
-      <c r="D1" s="40"/>
-      <c r="E1" s="40"/>
-      <c r="F1" s="40"/>
-      <c r="G1" s="40"/>
-      <c r="H1" s="40"/>
-      <c r="I1" s="40"/>
-      <c r="J1" s="43" t="s">
+      <c r="D1" s="43"/>
+      <c r="E1" s="43"/>
+      <c r="F1" s="43"/>
+      <c r="G1" s="43"/>
+      <c r="H1" s="43"/>
+      <c r="I1" s="43"/>
+      <c r="J1" s="40" t="s">
         <v>1</v>
       </c>
       <c r="K1" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="L1" s="40" t="s">
+      <c r="L1" s="43" t="s">
         <v>40</v>
       </c>
-      <c r="M1" s="40"/>
-      <c r="N1" s="40"/>
-      <c r="O1" s="40"/>
-      <c r="P1" s="40"/>
-      <c r="Q1" s="40"/>
-      <c r="R1" s="40"/>
+      <c r="M1" s="43"/>
+      <c r="N1" s="43"/>
+      <c r="O1" s="43"/>
+      <c r="P1" s="43"/>
+      <c r="Q1" s="43"/>
+      <c r="R1" s="43"/>
       <c r="S1" s="1"/>
       <c r="T1" s="1"/>
       <c r="U1" s="1"/>
@@ -5563,6 +5563,11 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="K1:K2"/>
+    <mergeCell ref="L1:R1"/>
+    <mergeCell ref="J3:J5"/>
+    <mergeCell ref="J6:J8"/>
+    <mergeCell ref="C1:I1"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="J15:J17"/>
@@ -5574,11 +5579,6 @@
     <mergeCell ref="A3:A5"/>
     <mergeCell ref="A6:A8"/>
     <mergeCell ref="A9:A11"/>
-    <mergeCell ref="K1:K2"/>
-    <mergeCell ref="L1:R1"/>
-    <mergeCell ref="J3:J5"/>
-    <mergeCell ref="J6:J8"/>
-    <mergeCell ref="C1:I1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -5612,7 +5612,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="40" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="38" t="s">
@@ -5621,15 +5621,15 @@
       <c r="C1" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="40" t="s">
+      <c r="D1" s="43" t="s">
         <v>41</v>
       </c>
-      <c r="E1" s="40"/>
-      <c r="F1" s="40"/>
-      <c r="G1" s="40"/>
-      <c r="H1" s="40"/>
-      <c r="I1" s="40"/>
-      <c r="J1" s="40"/>
+      <c r="E1" s="43"/>
+      <c r="F1" s="43"/>
+      <c r="G1" s="43"/>
+      <c r="H1" s="43"/>
+      <c r="I1" s="43"/>
+      <c r="J1" s="43"/>
       <c r="S1" s="1"/>
       <c r="T1" s="1"/>
       <c r="U1" s="1"/>
@@ -10688,7 +10688,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="105" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" ht="87.5" x14ac:dyDescent="0.35">
       <c r="A5" s="45"/>
       <c r="B5" s="21" t="s">
         <v>9</v>
@@ -11569,8 +11569,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B35242D0-2AD6-442D-ABA4-BF0550EDBCE1}">
   <dimension ref="A1:J17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.453125" defaultRowHeight="17.5" x14ac:dyDescent="0.35"/>
@@ -11640,7 +11640,9 @@
       <c r="D3" s="25" t="s">
         <v>55</v>
       </c>
-      <c r="E3" s="25"/>
+      <c r="E3" s="25" t="s">
+        <v>55</v>
+      </c>
       <c r="F3" s="25"/>
       <c r="G3" s="25"/>
       <c r="H3" s="25"/>
@@ -11657,7 +11659,9 @@
       <c r="D4" s="25" t="s">
         <v>55</v>
       </c>
-      <c r="E4" s="25"/>
+      <c r="E4" s="25" t="s">
+        <v>55</v>
+      </c>
       <c r="F4" s="25"/>
       <c r="G4" s="25"/>
       <c r="H4" s="25"/>
@@ -11674,7 +11678,9 @@
       <c r="D5" s="25" t="s">
         <v>77</v>
       </c>
-      <c r="E5" s="25"/>
+      <c r="E5" s="25" t="s">
+        <v>77</v>
+      </c>
       <c r="F5" s="31"/>
       <c r="G5" s="31"/>
       <c r="H5" s="25"/>
@@ -11693,7 +11699,9 @@
       <c r="D6" s="25" t="s">
         <v>55</v>
       </c>
-      <c r="E6" s="25"/>
+      <c r="E6" s="25" t="s">
+        <v>55</v>
+      </c>
       <c r="F6" s="25"/>
       <c r="G6" s="25"/>
       <c r="H6" s="25"/>
@@ -11710,7 +11718,9 @@
       <c r="D7" s="25" t="s">
         <v>55</v>
       </c>
-      <c r="E7" s="25"/>
+      <c r="E7" s="25" t="s">
+        <v>55</v>
+      </c>
       <c r="F7" s="25"/>
       <c r="G7" s="25"/>
       <c r="H7" s="25"/>
@@ -11727,7 +11737,9 @@
       <c r="D8" s="25" t="s">
         <v>77</v>
       </c>
-      <c r="E8" s="25"/>
+      <c r="E8" s="25" t="s">
+        <v>77</v>
+      </c>
       <c r="F8" s="31"/>
       <c r="G8" s="31"/>
       <c r="H8" s="25"/>
@@ -11746,7 +11758,9 @@
       <c r="D9" s="25" t="s">
         <v>92</v>
       </c>
-      <c r="E9" s="25"/>
+      <c r="E9" s="25" t="s">
+        <v>55</v>
+      </c>
       <c r="F9" s="25"/>
       <c r="H9" s="25"/>
       <c r="I9" s="25"/>
@@ -11762,7 +11776,9 @@
       <c r="D10" s="25" t="s">
         <v>55</v>
       </c>
-      <c r="E10" s="25"/>
+      <c r="E10" s="25" t="s">
+        <v>55</v>
+      </c>
       <c r="G10" s="25"/>
       <c r="H10" s="25"/>
       <c r="I10" s="25"/>
@@ -11778,7 +11794,9 @@
       <c r="D11" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="E11" s="25"/>
+      <c r="E11" s="25" t="s">
+        <v>30</v>
+      </c>
       <c r="F11" s="25"/>
       <c r="G11" s="25"/>
       <c r="H11" s="25"/>
@@ -11797,7 +11815,9 @@
       <c r="D12" s="25" t="s">
         <v>55</v>
       </c>
-      <c r="E12" s="25"/>
+      <c r="E12" s="25" t="s">
+        <v>55</v>
+      </c>
       <c r="F12" s="25"/>
       <c r="G12" s="25"/>
       <c r="H12" s="25"/>
@@ -11814,7 +11834,9 @@
       <c r="D13" s="25" t="s">
         <v>55</v>
       </c>
-      <c r="E13" s="25"/>
+      <c r="E13" s="25" t="s">
+        <v>55</v>
+      </c>
       <c r="F13" s="25"/>
       <c r="G13" s="25"/>
       <c r="H13" s="25"/>
@@ -11831,7 +11853,9 @@
       <c r="D14" s="25" t="s">
         <v>77</v>
       </c>
-      <c r="E14" s="25"/>
+      <c r="E14" s="25" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="15" spans="1:10" ht="87.5" x14ac:dyDescent="0.35">
       <c r="A15" s="44" t="s">
@@ -11846,7 +11870,9 @@
       <c r="D15" s="25" t="s">
         <v>55</v>
       </c>
-      <c r="E15" s="25"/>
+      <c r="E15" s="25" t="s">
+        <v>55</v>
+      </c>
       <c r="F15" s="25"/>
       <c r="H15" s="25"/>
       <c r="I15" s="25"/>
@@ -11863,7 +11889,9 @@
       <c r="D16" s="25" t="s">
         <v>55</v>
       </c>
-      <c r="E16" s="25"/>
+      <c r="E16" s="25" t="s">
+        <v>55</v>
+      </c>
       <c r="G16" s="25"/>
       <c r="H16" s="25"/>
       <c r="I16" s="25"/>
@@ -11880,7 +11908,9 @@
       <c r="D17" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="E17" s="25"/>
+      <c r="E17" s="25" t="s">
+        <v>30</v>
+      </c>
       <c r="F17" s="25"/>
       <c r="G17" s="25"/>
       <c r="H17" s="25"/>

</xml_diff>

<commit_message>
update du (week10 thurs)
</commit_message>
<xml_diff>
--- a/metrics/du.xlsx
+++ b/metrics/du.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\project-g4t6\metrics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{038B6CD9-648A-47A9-9553-3B9295AEC39F}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C33732E2-82DA-486C-904E-B4B971FED7F6}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="844" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="859" uniqueCount="101">
   <si>
     <t>Question</t>
   </si>
@@ -325,6 +325,32 @@
   <si>
     <t>Nade changes to testcases for bid.csv</t>
   </si>
+  <si>
+    <t>Made changes to testcases for bid.csv</t>
+  </si>
+  <si>
+    <t>Did the dropsection.csv</t>
+  </si>
+  <si>
+    <t>did JSON -update-bid.php</t>
+  </si>
+  <si>
+    <t>Boostrap vaidate not modular - cannot be reused for update-bid</t>
+  </si>
+  <si>
+    <t>1. Scheduling updates on googledrive
+2. neaten manual testcases</t>
+  </si>
+  <si>
+    <t>Did Round 2 clearing logic</t>
+  </si>
+  <si>
+    <t>1. Scheduling updates on googledrive
+2. Did dropsection.csv</t>
+  </si>
+  <si>
+    <t>coming up woth sound and consistent logic for the naming conventionf or task ID</t>
+  </si>
 </sst>
 </file>
 
@@ -514,15 +540,15 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -850,36 +876,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="43" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="43" t="s">
+      <c r="C1" s="40" t="s">
         <v>18</v>
       </c>
-      <c r="D1" s="43"/>
-      <c r="E1" s="43"/>
-      <c r="F1" s="43"/>
-      <c r="G1" s="43"/>
-      <c r="H1" s="43"/>
-      <c r="I1" s="43"/>
-      <c r="J1" s="40" t="s">
+      <c r="D1" s="40"/>
+      <c r="E1" s="40"/>
+      <c r="F1" s="40"/>
+      <c r="G1" s="40"/>
+      <c r="H1" s="40"/>
+      <c r="I1" s="40"/>
+      <c r="J1" s="43" t="s">
         <v>1</v>
       </c>
       <c r="K1" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="L1" s="43" t="s">
+      <c r="L1" s="40" t="s">
         <v>40</v>
       </c>
-      <c r="M1" s="43"/>
-      <c r="N1" s="43"/>
-      <c r="O1" s="43"/>
-      <c r="P1" s="43"/>
-      <c r="Q1" s="43"/>
-      <c r="R1" s="43"/>
+      <c r="M1" s="40"/>
+      <c r="N1" s="40"/>
+      <c r="O1" s="40"/>
+      <c r="P1" s="40"/>
+      <c r="Q1" s="40"/>
+      <c r="R1" s="40"/>
       <c r="S1" s="1"/>
       <c r="T1" s="1"/>
       <c r="U1" s="1"/>
@@ -5563,11 +5589,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="K1:K2"/>
-    <mergeCell ref="L1:R1"/>
-    <mergeCell ref="J3:J5"/>
-    <mergeCell ref="J6:J8"/>
-    <mergeCell ref="C1:I1"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="J15:J17"/>
@@ -5579,6 +5600,11 @@
     <mergeCell ref="A3:A5"/>
     <mergeCell ref="A6:A8"/>
     <mergeCell ref="A9:A11"/>
+    <mergeCell ref="K1:K2"/>
+    <mergeCell ref="L1:R1"/>
+    <mergeCell ref="J3:J5"/>
+    <mergeCell ref="J6:J8"/>
+    <mergeCell ref="C1:I1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -5612,7 +5638,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="43" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="38" t="s">
@@ -5621,15 +5647,15 @@
       <c r="C1" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="43" t="s">
+      <c r="D1" s="40" t="s">
         <v>41</v>
       </c>
-      <c r="E1" s="43"/>
-      <c r="F1" s="43"/>
-      <c r="G1" s="43"/>
-      <c r="H1" s="43"/>
-      <c r="I1" s="43"/>
-      <c r="J1" s="43"/>
+      <c r="E1" s="40"/>
+      <c r="F1" s="40"/>
+      <c r="G1" s="40"/>
+      <c r="H1" s="40"/>
+      <c r="I1" s="40"/>
+      <c r="J1" s="40"/>
       <c r="S1" s="1"/>
       <c r="T1" s="1"/>
       <c r="U1" s="1"/>
@@ -11569,8 +11595,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B35242D0-2AD6-442D-ABA4-BF0550EDBCE1}">
   <dimension ref="A1:J17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.453125" defaultRowHeight="17.5" x14ac:dyDescent="0.35"/>
@@ -11643,7 +11669,9 @@
       <c r="E3" s="25" t="s">
         <v>55</v>
       </c>
-      <c r="F3" s="25"/>
+      <c r="F3" s="25" t="s">
+        <v>55</v>
+      </c>
       <c r="G3" s="25"/>
       <c r="H3" s="25"/>
       <c r="I3" s="25"/>
@@ -11662,7 +11690,9 @@
       <c r="E4" s="25" t="s">
         <v>55</v>
       </c>
-      <c r="F4" s="25"/>
+      <c r="F4" s="25" t="s">
+        <v>94</v>
+      </c>
       <c r="G4" s="25"/>
       <c r="H4" s="25"/>
       <c r="I4" s="25"/>
@@ -11681,7 +11711,9 @@
       <c r="E5" s="25" t="s">
         <v>77</v>
       </c>
-      <c r="F5" s="31"/>
+      <c r="F5" s="25" t="s">
+        <v>77</v>
+      </c>
       <c r="G5" s="31"/>
       <c r="H5" s="25"/>
       <c r="I5" s="25"/>
@@ -11702,7 +11734,9 @@
       <c r="E6" s="25" t="s">
         <v>55</v>
       </c>
-      <c r="F6" s="25"/>
+      <c r="F6" s="25" t="s">
+        <v>55</v>
+      </c>
       <c r="G6" s="25"/>
       <c r="H6" s="25"/>
       <c r="I6" s="25"/>
@@ -11721,7 +11755,9 @@
       <c r="E7" s="25" t="s">
         <v>55</v>
       </c>
-      <c r="F7" s="25"/>
+      <c r="F7" s="25" t="s">
+        <v>95</v>
+      </c>
       <c r="G7" s="25"/>
       <c r="H7" s="25"/>
       <c r="I7" s="25"/>
@@ -11740,7 +11776,9 @@
       <c r="E8" s="25" t="s">
         <v>77</v>
       </c>
-      <c r="F8" s="31"/>
+      <c r="F8" s="25" t="s">
+        <v>96</v>
+      </c>
       <c r="G8" s="31"/>
       <c r="H8" s="25"/>
       <c r="I8" s="25"/>
@@ -11761,29 +11799,34 @@
       <c r="E9" s="25" t="s">
         <v>55</v>
       </c>
-      <c r="F9" s="25"/>
+      <c r="F9" s="25" t="s">
+        <v>55</v>
+      </c>
       <c r="H9" s="25"/>
       <c r="I9" s="25"/>
     </row>
-    <row r="10" spans="1:10" ht="52.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" ht="87.5" x14ac:dyDescent="0.35">
       <c r="A10" s="45"/>
       <c r="B10" s="36" t="s">
         <v>8</v>
       </c>
       <c r="C10" s="25" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D10" s="25" t="s">
         <v>55</v>
       </c>
       <c r="E10" s="25" t="s">
         <v>55</v>
+      </c>
+      <c r="F10" s="37" t="s">
+        <v>97</v>
       </c>
       <c r="G10" s="25"/>
       <c r="H10" s="25"/>
       <c r="I10" s="25"/>
     </row>
-    <row r="11" spans="1:10" ht="52.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10" ht="70" x14ac:dyDescent="0.35">
       <c r="A11" s="45"/>
       <c r="B11" s="36" t="s">
         <v>9</v>
@@ -11797,7 +11840,9 @@
       <c r="E11" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="F11" s="25"/>
+      <c r="F11" s="25" t="s">
+        <v>100</v>
+      </c>
       <c r="G11" s="25"/>
       <c r="H11" s="25"/>
       <c r="I11" s="25"/>
@@ -11818,12 +11863,14 @@
       <c r="E12" s="25" t="s">
         <v>55</v>
       </c>
-      <c r="F12" s="25"/>
+      <c r="F12" s="25" t="s">
+        <v>55</v>
+      </c>
       <c r="G12" s="25"/>
       <c r="H12" s="25"/>
       <c r="I12" s="25"/>
     </row>
-    <row r="13" spans="1:10" ht="52.5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:10" ht="87.5" x14ac:dyDescent="0.35">
       <c r="A13" s="45"/>
       <c r="B13" s="36" t="s">
         <v>8</v>
@@ -11837,7 +11884,9 @@
       <c r="E13" s="25" t="s">
         <v>55</v>
       </c>
-      <c r="F13" s="25"/>
+      <c r="F13" s="25" t="s">
+        <v>99</v>
+      </c>
       <c r="G13" s="25"/>
       <c r="H13" s="25"/>
       <c r="I13" s="25"/>
@@ -11856,6 +11905,9 @@
       <c r="E14" s="25" t="s">
         <v>77</v>
       </c>
+      <c r="F14" s="25" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="15" spans="1:10" ht="87.5" x14ac:dyDescent="0.35">
       <c r="A15" s="44" t="s">
@@ -11873,7 +11925,9 @@
       <c r="E15" s="25" t="s">
         <v>55</v>
       </c>
-      <c r="F15" s="25"/>
+      <c r="F15" s="25" t="s">
+        <v>55</v>
+      </c>
       <c r="H15" s="25"/>
       <c r="I15" s="25"/>
       <c r="J15" s="25"/>
@@ -11892,6 +11946,9 @@
       <c r="E16" s="25" t="s">
         <v>55</v>
       </c>
+      <c r="F16" s="37" t="s">
+        <v>98</v>
+      </c>
       <c r="G16" s="25"/>
       <c r="H16" s="25"/>
       <c r="I16" s="25"/>
@@ -11911,7 +11968,9 @@
       <c r="E17" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="F17" s="25"/>
+      <c r="F17" s="25" t="s">
+        <v>30</v>
+      </c>
       <c r="G17" s="25"/>
       <c r="H17" s="25"/>
       <c r="I17" s="25"/>

</xml_diff>

<commit_message>
updated du (week 10 fri)
</commit_message>
<xml_diff>
--- a/metrics/du.xlsx
+++ b/metrics/du.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\project-g4t6\metrics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C33732E2-82DA-486C-904E-B4B971FED7F6}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{658C6A68-3435-45F5-84B1-2047A7E5AD22}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="859" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="874" uniqueCount="101">
   <si>
     <t>Question</t>
   </si>
@@ -540,15 +540,15 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -876,36 +876,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="40" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="40" t="s">
+      <c r="C1" s="43" t="s">
         <v>18</v>
       </c>
-      <c r="D1" s="40"/>
-      <c r="E1" s="40"/>
-      <c r="F1" s="40"/>
-      <c r="G1" s="40"/>
-      <c r="H1" s="40"/>
-      <c r="I1" s="40"/>
-      <c r="J1" s="43" t="s">
+      <c r="D1" s="43"/>
+      <c r="E1" s="43"/>
+      <c r="F1" s="43"/>
+      <c r="G1" s="43"/>
+      <c r="H1" s="43"/>
+      <c r="I1" s="43"/>
+      <c r="J1" s="40" t="s">
         <v>1</v>
       </c>
       <c r="K1" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="L1" s="40" t="s">
+      <c r="L1" s="43" t="s">
         <v>40</v>
       </c>
-      <c r="M1" s="40"/>
-      <c r="N1" s="40"/>
-      <c r="O1" s="40"/>
-      <c r="P1" s="40"/>
-      <c r="Q1" s="40"/>
-      <c r="R1" s="40"/>
+      <c r="M1" s="43"/>
+      <c r="N1" s="43"/>
+      <c r="O1" s="43"/>
+      <c r="P1" s="43"/>
+      <c r="Q1" s="43"/>
+      <c r="R1" s="43"/>
       <c r="S1" s="1"/>
       <c r="T1" s="1"/>
       <c r="U1" s="1"/>
@@ -5589,6 +5589,11 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="K1:K2"/>
+    <mergeCell ref="L1:R1"/>
+    <mergeCell ref="J3:J5"/>
+    <mergeCell ref="J6:J8"/>
+    <mergeCell ref="C1:I1"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="J15:J17"/>
@@ -5600,11 +5605,6 @@
     <mergeCell ref="A3:A5"/>
     <mergeCell ref="A6:A8"/>
     <mergeCell ref="A9:A11"/>
-    <mergeCell ref="K1:K2"/>
-    <mergeCell ref="L1:R1"/>
-    <mergeCell ref="J3:J5"/>
-    <mergeCell ref="J6:J8"/>
-    <mergeCell ref="C1:I1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -5638,7 +5638,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="40" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="38" t="s">
@@ -5647,15 +5647,15 @@
       <c r="C1" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="40" t="s">
+      <c r="D1" s="43" t="s">
         <v>41</v>
       </c>
-      <c r="E1" s="40"/>
-      <c r="F1" s="40"/>
-      <c r="G1" s="40"/>
-      <c r="H1" s="40"/>
-      <c r="I1" s="40"/>
-      <c r="J1" s="40"/>
+      <c r="E1" s="43"/>
+      <c r="F1" s="43"/>
+      <c r="G1" s="43"/>
+      <c r="H1" s="43"/>
+      <c r="I1" s="43"/>
+      <c r="J1" s="43"/>
       <c r="S1" s="1"/>
       <c r="T1" s="1"/>
       <c r="U1" s="1"/>
@@ -11595,8 +11595,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B35242D0-2AD6-442D-ABA4-BF0550EDBCE1}">
   <dimension ref="A1:J17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.453125" defaultRowHeight="17.5" x14ac:dyDescent="0.35"/>
@@ -11672,7 +11672,9 @@
       <c r="F3" s="25" t="s">
         <v>55</v>
       </c>
-      <c r="G3" s="25"/>
+      <c r="G3" s="25" t="s">
+        <v>55</v>
+      </c>
       <c r="H3" s="25"/>
       <c r="I3" s="25"/>
     </row>
@@ -11693,7 +11695,9 @@
       <c r="F4" s="25" t="s">
         <v>94</v>
       </c>
-      <c r="G4" s="25"/>
+      <c r="G4" s="25" t="s">
+        <v>55</v>
+      </c>
       <c r="H4" s="25"/>
       <c r="I4" s="25"/>
     </row>
@@ -11714,7 +11718,9 @@
       <c r="F5" s="25" t="s">
         <v>77</v>
       </c>
-      <c r="G5" s="31"/>
+      <c r="G5" s="25" t="s">
+        <v>30</v>
+      </c>
       <c r="H5" s="25"/>
       <c r="I5" s="25"/>
     </row>
@@ -11737,7 +11743,9 @@
       <c r="F6" s="25" t="s">
         <v>55</v>
       </c>
-      <c r="G6" s="25"/>
+      <c r="G6" s="25" t="s">
+        <v>55</v>
+      </c>
       <c r="H6" s="25"/>
       <c r="I6" s="25"/>
     </row>
@@ -11758,7 +11766,9 @@
       <c r="F7" s="25" t="s">
         <v>95</v>
       </c>
-      <c r="G7" s="25"/>
+      <c r="G7" s="25" t="s">
+        <v>55</v>
+      </c>
       <c r="H7" s="25"/>
       <c r="I7" s="25"/>
     </row>
@@ -11779,7 +11789,9 @@
       <c r="F8" s="25" t="s">
         <v>96</v>
       </c>
-      <c r="G8" s="31"/>
+      <c r="G8" s="25" t="s">
+        <v>30</v>
+      </c>
       <c r="H8" s="25"/>
       <c r="I8" s="25"/>
     </row>
@@ -11800,6 +11812,9 @@
         <v>55</v>
       </c>
       <c r="F9" s="25" t="s">
+        <v>55</v>
+      </c>
+      <c r="G9" s="25" t="s">
         <v>55</v>
       </c>
       <c r="H9" s="25"/>
@@ -11822,7 +11837,9 @@
       <c r="F10" s="37" t="s">
         <v>97</v>
       </c>
-      <c r="G10" s="25"/>
+      <c r="G10" s="25" t="s">
+        <v>55</v>
+      </c>
       <c r="H10" s="25"/>
       <c r="I10" s="25"/>
     </row>
@@ -11843,7 +11860,9 @@
       <c r="F11" s="25" t="s">
         <v>100</v>
       </c>
-      <c r="G11" s="25"/>
+      <c r="G11" s="25" t="s">
+        <v>30</v>
+      </c>
       <c r="H11" s="25"/>
       <c r="I11" s="25"/>
     </row>
@@ -11866,7 +11885,9 @@
       <c r="F12" s="25" t="s">
         <v>55</v>
       </c>
-      <c r="G12" s="25"/>
+      <c r="G12" s="25" t="s">
+        <v>55</v>
+      </c>
       <c r="H12" s="25"/>
       <c r="I12" s="25"/>
     </row>
@@ -11887,7 +11908,9 @@
       <c r="F13" s="25" t="s">
         <v>99</v>
       </c>
-      <c r="G13" s="25"/>
+      <c r="G13" s="25" t="s">
+        <v>55</v>
+      </c>
       <c r="H13" s="25"/>
       <c r="I13" s="25"/>
     </row>
@@ -11908,6 +11931,9 @@
       <c r="F14" s="25" t="s">
         <v>77</v>
       </c>
+      <c r="G14" s="25" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="15" spans="1:10" ht="87.5" x14ac:dyDescent="0.35">
       <c r="A15" s="44" t="s">
@@ -11926,6 +11952,9 @@
         <v>55</v>
       </c>
       <c r="F15" s="25" t="s">
+        <v>55</v>
+      </c>
+      <c r="G15" s="25" t="s">
         <v>55</v>
       </c>
       <c r="H15" s="25"/>
@@ -11949,7 +11978,9 @@
       <c r="F16" s="37" t="s">
         <v>98</v>
       </c>
-      <c r="G16" s="25"/>
+      <c r="G16" s="25" t="s">
+        <v>55</v>
+      </c>
       <c r="H16" s="25"/>
       <c r="I16" s="25"/>
       <c r="J16" s="25"/>
@@ -11971,7 +12002,9 @@
       <c r="F17" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="G17" s="25"/>
+      <c r="G17" s="25" t="s">
+        <v>30</v>
+      </c>
       <c r="H17" s="25"/>
       <c r="I17" s="25"/>
       <c r="J17" s="25"/>

</xml_diff>

<commit_message>
updated du (week 10 sat)
</commit_message>
<xml_diff>
--- a/metrics/du.xlsx
+++ b/metrics/du.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\project-g4t6\metrics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{658C6A68-3435-45F5-84B1-2047A7E5AD22}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{567A711A-B88F-4DB6-B1A0-41724EBB6439}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="874" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="889" uniqueCount="101">
   <si>
     <t>Question</t>
   </si>
@@ -540,15 +540,15 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -876,36 +876,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="43" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="43" t="s">
+      <c r="C1" s="40" t="s">
         <v>18</v>
       </c>
-      <c r="D1" s="43"/>
-      <c r="E1" s="43"/>
-      <c r="F1" s="43"/>
-      <c r="G1" s="43"/>
-      <c r="H1" s="43"/>
-      <c r="I1" s="43"/>
-      <c r="J1" s="40" t="s">
+      <c r="D1" s="40"/>
+      <c r="E1" s="40"/>
+      <c r="F1" s="40"/>
+      <c r="G1" s="40"/>
+      <c r="H1" s="40"/>
+      <c r="I1" s="40"/>
+      <c r="J1" s="43" t="s">
         <v>1</v>
       </c>
       <c r="K1" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="L1" s="43" t="s">
+      <c r="L1" s="40" t="s">
         <v>40</v>
       </c>
-      <c r="M1" s="43"/>
-      <c r="N1" s="43"/>
-      <c r="O1" s="43"/>
-      <c r="P1" s="43"/>
-      <c r="Q1" s="43"/>
-      <c r="R1" s="43"/>
+      <c r="M1" s="40"/>
+      <c r="N1" s="40"/>
+      <c r="O1" s="40"/>
+      <c r="P1" s="40"/>
+      <c r="Q1" s="40"/>
+      <c r="R1" s="40"/>
       <c r="S1" s="1"/>
       <c r="T1" s="1"/>
       <c r="U1" s="1"/>
@@ -5589,11 +5589,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="K1:K2"/>
-    <mergeCell ref="L1:R1"/>
-    <mergeCell ref="J3:J5"/>
-    <mergeCell ref="J6:J8"/>
-    <mergeCell ref="C1:I1"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="J15:J17"/>
@@ -5605,6 +5600,11 @@
     <mergeCell ref="A3:A5"/>
     <mergeCell ref="A6:A8"/>
     <mergeCell ref="A9:A11"/>
+    <mergeCell ref="K1:K2"/>
+    <mergeCell ref="L1:R1"/>
+    <mergeCell ref="J3:J5"/>
+    <mergeCell ref="J6:J8"/>
+    <mergeCell ref="C1:I1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -5638,7 +5638,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="43" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="38" t="s">
@@ -5647,15 +5647,15 @@
       <c r="C1" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="43" t="s">
+      <c r="D1" s="40" t="s">
         <v>41</v>
       </c>
-      <c r="E1" s="43"/>
-      <c r="F1" s="43"/>
-      <c r="G1" s="43"/>
-      <c r="H1" s="43"/>
-      <c r="I1" s="43"/>
-      <c r="J1" s="43"/>
+      <c r="E1" s="40"/>
+      <c r="F1" s="40"/>
+      <c r="G1" s="40"/>
+      <c r="H1" s="40"/>
+      <c r="I1" s="40"/>
+      <c r="J1" s="40"/>
       <c r="S1" s="1"/>
       <c r="T1" s="1"/>
       <c r="U1" s="1"/>
@@ -11595,8 +11595,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B35242D0-2AD6-442D-ABA4-BF0550EDBCE1}">
   <dimension ref="A1:J17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.453125" defaultRowHeight="17.5" x14ac:dyDescent="0.35"/>
@@ -11675,7 +11675,9 @@
       <c r="G3" s="25" t="s">
         <v>55</v>
       </c>
-      <c r="H3" s="25"/>
+      <c r="H3" s="25" t="s">
+        <v>55</v>
+      </c>
       <c r="I3" s="25"/>
     </row>
     <row r="4" spans="1:10" ht="35" x14ac:dyDescent="0.35">
@@ -11698,7 +11700,9 @@
       <c r="G4" s="25" t="s">
         <v>55</v>
       </c>
-      <c r="H4" s="25"/>
+      <c r="H4" s="25" t="s">
+        <v>55</v>
+      </c>
       <c r="I4" s="25"/>
     </row>
     <row r="5" spans="1:10" ht="52.5" x14ac:dyDescent="0.35">
@@ -11721,7 +11725,9 @@
       <c r="G5" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="H5" s="25"/>
+      <c r="H5" s="25" t="s">
+        <v>30</v>
+      </c>
       <c r="I5" s="25"/>
     </row>
     <row r="6" spans="1:10" ht="87.5" x14ac:dyDescent="0.35">
@@ -11746,7 +11752,9 @@
       <c r="G6" s="25" t="s">
         <v>55</v>
       </c>
-      <c r="H6" s="25"/>
+      <c r="H6" s="25" t="s">
+        <v>55</v>
+      </c>
       <c r="I6" s="25"/>
     </row>
     <row r="7" spans="1:10" ht="52.5" x14ac:dyDescent="0.35">
@@ -11769,7 +11777,9 @@
       <c r="G7" s="25" t="s">
         <v>55</v>
       </c>
-      <c r="H7" s="25"/>
+      <c r="H7" s="25" t="s">
+        <v>55</v>
+      </c>
       <c r="I7" s="25"/>
     </row>
     <row r="8" spans="1:10" ht="52.5" x14ac:dyDescent="0.35">
@@ -11792,7 +11802,9 @@
       <c r="G8" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="H8" s="25"/>
+      <c r="H8" s="25" t="s">
+        <v>30</v>
+      </c>
       <c r="I8" s="25"/>
     </row>
     <row r="9" spans="1:10" ht="105" x14ac:dyDescent="0.35">
@@ -11817,7 +11829,9 @@
       <c r="G9" s="25" t="s">
         <v>55</v>
       </c>
-      <c r="H9" s="25"/>
+      <c r="H9" s="25" t="s">
+        <v>55</v>
+      </c>
       <c r="I9" s="25"/>
     </row>
     <row r="10" spans="1:10" ht="87.5" x14ac:dyDescent="0.35">
@@ -11840,7 +11854,9 @@
       <c r="G10" s="25" t="s">
         <v>55</v>
       </c>
-      <c r="H10" s="25"/>
+      <c r="H10" s="25" t="s">
+        <v>55</v>
+      </c>
       <c r="I10" s="25"/>
     </row>
     <row r="11" spans="1:10" ht="70" x14ac:dyDescent="0.35">
@@ -11863,7 +11879,9 @@
       <c r="G11" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="H11" s="25"/>
+      <c r="H11" s="25" t="s">
+        <v>30</v>
+      </c>
       <c r="I11" s="25"/>
     </row>
     <row r="12" spans="1:10" ht="35" x14ac:dyDescent="0.35">
@@ -11888,7 +11906,9 @@
       <c r="G12" s="25" t="s">
         <v>55</v>
       </c>
-      <c r="H12" s="25"/>
+      <c r="H12" s="25" t="s">
+        <v>55</v>
+      </c>
       <c r="I12" s="25"/>
     </row>
     <row r="13" spans="1:10" ht="87.5" x14ac:dyDescent="0.35">
@@ -11911,7 +11931,9 @@
       <c r="G13" s="25" t="s">
         <v>55</v>
       </c>
-      <c r="H13" s="25"/>
+      <c r="H13" s="25" t="s">
+        <v>55</v>
+      </c>
       <c r="I13" s="25"/>
     </row>
     <row r="14" spans="1:10" ht="52.5" x14ac:dyDescent="0.35">
@@ -11934,6 +11956,9 @@
       <c r="G14" s="25" t="s">
         <v>30</v>
       </c>
+      <c r="H14" s="25" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="15" spans="1:10" ht="87.5" x14ac:dyDescent="0.35">
       <c r="A15" s="44" t="s">
@@ -11957,7 +11982,9 @@
       <c r="G15" s="25" t="s">
         <v>55</v>
       </c>
-      <c r="H15" s="25"/>
+      <c r="H15" s="25" t="s">
+        <v>55</v>
+      </c>
       <c r="I15" s="25"/>
       <c r="J15" s="25"/>
     </row>
@@ -11981,7 +12008,9 @@
       <c r="G16" s="25" t="s">
         <v>55</v>
       </c>
-      <c r="H16" s="25"/>
+      <c r="H16" s="25" t="s">
+        <v>55</v>
+      </c>
       <c r="I16" s="25"/>
       <c r="J16" s="25"/>
     </row>
@@ -12005,7 +12034,9 @@
       <c r="G17" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="H17" s="25"/>
+      <c r="H17" s="25" t="s">
+        <v>30</v>
+      </c>
       <c r="I17" s="25"/>
       <c r="J17" s="25"/>
     </row>

</xml_diff>

<commit_message>
update du (week10 sun)
</commit_message>
<xml_diff>
--- a/metrics/du.xlsx
+++ b/metrics/du.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\project-g4t6\metrics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{567A711A-B88F-4DB6-B1A0-41724EBB6439}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{604417F3-0936-41BF-B873-39AD6A6B1FC0}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="889" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="904" uniqueCount="103">
   <si>
     <t>Question</t>
   </si>
@@ -351,6 +351,12 @@
   <si>
     <t>coming up woth sound and consistent logic for the naming conventionf or task ID</t>
   </si>
+  <si>
+    <t xml:space="preserve">Made changes to testcares for section.csv </t>
+  </si>
+  <si>
+    <t>JSON- dump(bids)</t>
+  </si>
 </sst>
 </file>
 
@@ -540,15 +546,15 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -876,36 +882,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="40" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="40" t="s">
+      <c r="C1" s="43" t="s">
         <v>18</v>
       </c>
-      <c r="D1" s="40"/>
-      <c r="E1" s="40"/>
-      <c r="F1" s="40"/>
-      <c r="G1" s="40"/>
-      <c r="H1" s="40"/>
-      <c r="I1" s="40"/>
-      <c r="J1" s="43" t="s">
+      <c r="D1" s="43"/>
+      <c r="E1" s="43"/>
+      <c r="F1" s="43"/>
+      <c r="G1" s="43"/>
+      <c r="H1" s="43"/>
+      <c r="I1" s="43"/>
+      <c r="J1" s="40" t="s">
         <v>1</v>
       </c>
       <c r="K1" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="L1" s="40" t="s">
+      <c r="L1" s="43" t="s">
         <v>40</v>
       </c>
-      <c r="M1" s="40"/>
-      <c r="N1" s="40"/>
-      <c r="O1" s="40"/>
-      <c r="P1" s="40"/>
-      <c r="Q1" s="40"/>
-      <c r="R1" s="40"/>
+      <c r="M1" s="43"/>
+      <c r="N1" s="43"/>
+      <c r="O1" s="43"/>
+      <c r="P1" s="43"/>
+      <c r="Q1" s="43"/>
+      <c r="R1" s="43"/>
       <c r="S1" s="1"/>
       <c r="T1" s="1"/>
       <c r="U1" s="1"/>
@@ -5589,6 +5595,11 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="K1:K2"/>
+    <mergeCell ref="L1:R1"/>
+    <mergeCell ref="J3:J5"/>
+    <mergeCell ref="J6:J8"/>
+    <mergeCell ref="C1:I1"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="J15:J17"/>
@@ -5600,11 +5611,6 @@
     <mergeCell ref="A3:A5"/>
     <mergeCell ref="A6:A8"/>
     <mergeCell ref="A9:A11"/>
-    <mergeCell ref="K1:K2"/>
-    <mergeCell ref="L1:R1"/>
-    <mergeCell ref="J3:J5"/>
-    <mergeCell ref="J6:J8"/>
-    <mergeCell ref="C1:I1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -5638,7 +5644,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="40" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="38" t="s">
@@ -5647,15 +5653,15 @@
       <c r="C1" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="40" t="s">
+      <c r="D1" s="43" t="s">
         <v>41</v>
       </c>
-      <c r="E1" s="40"/>
-      <c r="F1" s="40"/>
-      <c r="G1" s="40"/>
-      <c r="H1" s="40"/>
-      <c r="I1" s="40"/>
-      <c r="J1" s="40"/>
+      <c r="E1" s="43"/>
+      <c r="F1" s="43"/>
+      <c r="G1" s="43"/>
+      <c r="H1" s="43"/>
+      <c r="I1" s="43"/>
+      <c r="J1" s="43"/>
       <c r="S1" s="1"/>
       <c r="T1" s="1"/>
       <c r="U1" s="1"/>
@@ -11595,8 +11601,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B35242D0-2AD6-442D-ABA4-BF0550EDBCE1}">
   <dimension ref="A1:J17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.453125" defaultRowHeight="17.5" x14ac:dyDescent="0.35"/>
@@ -11678,7 +11684,9 @@
       <c r="H3" s="25" t="s">
         <v>55</v>
       </c>
-      <c r="I3" s="25"/>
+      <c r="I3" s="25" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="4" spans="1:10" ht="35" x14ac:dyDescent="0.35">
       <c r="A4" s="45"/>
@@ -11703,7 +11711,9 @@
       <c r="H4" s="25" t="s">
         <v>55</v>
       </c>
-      <c r="I4" s="25"/>
+      <c r="I4" s="25" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="5" spans="1:10" ht="52.5" x14ac:dyDescent="0.35">
       <c r="A5" s="45"/>
@@ -11728,7 +11738,9 @@
       <c r="H5" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="I5" s="25"/>
+      <c r="I5" s="25" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="6" spans="1:10" ht="87.5" x14ac:dyDescent="0.35">
       <c r="A6" s="44" t="s">
@@ -11755,7 +11767,9 @@
       <c r="H6" s="25" t="s">
         <v>55</v>
       </c>
-      <c r="I6" s="25"/>
+      <c r="I6" s="25" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="7" spans="1:10" ht="52.5" x14ac:dyDescent="0.35">
       <c r="A7" s="45"/>
@@ -11780,7 +11794,9 @@
       <c r="H7" s="25" t="s">
         <v>55</v>
       </c>
-      <c r="I7" s="25"/>
+      <c r="I7" s="25" t="s">
+        <v>102</v>
+      </c>
     </row>
     <row r="8" spans="1:10" ht="52.5" x14ac:dyDescent="0.35">
       <c r="A8" s="45"/>
@@ -11805,7 +11821,9 @@
       <c r="H8" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="I8" s="25"/>
+      <c r="I8" s="25" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="9" spans="1:10" ht="105" x14ac:dyDescent="0.35">
       <c r="A9" s="44" t="s">
@@ -11832,7 +11850,9 @@
       <c r="H9" s="25" t="s">
         <v>55</v>
       </c>
-      <c r="I9" s="25"/>
+      <c r="I9" s="25" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="10" spans="1:10" ht="87.5" x14ac:dyDescent="0.35">
       <c r="A10" s="45"/>
@@ -11857,7 +11877,9 @@
       <c r="H10" s="25" t="s">
         <v>55</v>
       </c>
-      <c r="I10" s="25"/>
+      <c r="I10" s="25" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="11" spans="1:10" ht="70" x14ac:dyDescent="0.35">
       <c r="A11" s="45"/>
@@ -11882,7 +11904,9 @@
       <c r="H11" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="I11" s="25"/>
+      <c r="I11" s="25" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="12" spans="1:10" ht="35" x14ac:dyDescent="0.35">
       <c r="A12" s="44" t="s">
@@ -11909,7 +11933,9 @@
       <c r="H12" s="25" t="s">
         <v>55</v>
       </c>
-      <c r="I12" s="25"/>
+      <c r="I12" s="25" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="13" spans="1:10" ht="87.5" x14ac:dyDescent="0.35">
       <c r="A13" s="45"/>
@@ -11934,7 +11960,9 @@
       <c r="H13" s="25" t="s">
         <v>55</v>
       </c>
-      <c r="I13" s="25"/>
+      <c r="I13" s="25" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="14" spans="1:10" ht="52.5" x14ac:dyDescent="0.35">
       <c r="A14" s="45"/>
@@ -11959,6 +11987,9 @@
       <c r="H14" s="25" t="s">
         <v>30</v>
       </c>
+      <c r="I14" s="25" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="15" spans="1:10" ht="87.5" x14ac:dyDescent="0.35">
       <c r="A15" s="44" t="s">
@@ -11985,7 +12016,9 @@
       <c r="H15" s="25" t="s">
         <v>55</v>
       </c>
-      <c r="I15" s="25"/>
+      <c r="I15" s="25" t="s">
+        <v>55</v>
+      </c>
       <c r="J15" s="25"/>
     </row>
     <row r="16" spans="1:10" ht="52.5" x14ac:dyDescent="0.35">
@@ -12011,7 +12044,9 @@
       <c r="H16" s="25" t="s">
         <v>55</v>
       </c>
-      <c r="I16" s="25"/>
+      <c r="I16" s="25" t="s">
+        <v>55</v>
+      </c>
       <c r="J16" s="25"/>
     </row>
     <row r="17" spans="1:10" ht="52.5" x14ac:dyDescent="0.35">
@@ -12037,7 +12072,9 @@
       <c r="H17" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="I17" s="25"/>
+      <c r="I17" s="25" t="s">
+        <v>30</v>
+      </c>
       <c r="J17" s="25"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update du (week11 mon)
</commit_message>
<xml_diff>
--- a/metrics/du.xlsx
+++ b/metrics/du.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\project-g4t6\metrics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{604417F3-0936-41BF-B873-39AD6A6B1FC0}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B1F98EF-A727-44D8-B297-6027C5137F90}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Week 5" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="Week 8" sheetId="5" r:id="rId4"/>
     <sheet name="Week 9" sheetId="6" r:id="rId5"/>
     <sheet name="Week 10" sheetId="7" r:id="rId6"/>
+    <sheet name="Week 11" sheetId="9" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="904" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="949" uniqueCount="103">
   <si>
     <t>Question</t>
   </si>
@@ -435,7 +436,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -542,19 +543,25 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -882,36 +889,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="45" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="38" t="s">
+      <c r="B1" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="43" t="s">
+      <c r="C1" s="42" t="s">
         <v>18</v>
       </c>
-      <c r="D1" s="43"/>
-      <c r="E1" s="43"/>
-      <c r="F1" s="43"/>
-      <c r="G1" s="43"/>
-      <c r="H1" s="43"/>
-      <c r="I1" s="43"/>
-      <c r="J1" s="40" t="s">
+      <c r="D1" s="42"/>
+      <c r="E1" s="42"/>
+      <c r="F1" s="42"/>
+      <c r="G1" s="42"/>
+      <c r="H1" s="42"/>
+      <c r="I1" s="42"/>
+      <c r="J1" s="45" t="s">
         <v>1</v>
       </c>
-      <c r="K1" s="38" t="s">
+      <c r="K1" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="L1" s="43" t="s">
+      <c r="L1" s="42" t="s">
         <v>40</v>
       </c>
-      <c r="M1" s="43"/>
-      <c r="N1" s="43"/>
-      <c r="O1" s="43"/>
-      <c r="P1" s="43"/>
-      <c r="Q1" s="43"/>
-      <c r="R1" s="43"/>
+      <c r="M1" s="42"/>
+      <c r="N1" s="42"/>
+      <c r="O1" s="42"/>
+      <c r="P1" s="42"/>
+      <c r="Q1" s="42"/>
+      <c r="R1" s="42"/>
       <c r="S1" s="1"/>
       <c r="T1" s="1"/>
       <c r="U1" s="1"/>
@@ -922,8 +929,8 @@
       <c r="Z1" s="1"/>
     </row>
     <row r="2" spans="1:26" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="39"/>
-      <c r="B2" s="39"/>
+      <c r="A2" s="41"/>
+      <c r="B2" s="41"/>
       <c r="C2" s="3" t="s">
         <v>2</v>
       </c>
@@ -945,8 +952,8 @@
       <c r="I2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="J2" s="39"/>
-      <c r="K2" s="39"/>
+      <c r="J2" s="41"/>
+      <c r="K2" s="41"/>
       <c r="L2" s="3" t="s">
         <v>2</v>
       </c>
@@ -978,7 +985,7 @@
       <c r="Z2" s="1"/>
     </row>
     <row r="3" spans="1:26" ht="47.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="41" t="s">
+      <c r="A3" s="43" t="s">
         <v>13</v>
       </c>
       <c r="B3" s="4" t="s">
@@ -997,7 +1004,7 @@
       <c r="I3" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="J3" s="41" t="s">
+      <c r="J3" s="43" t="s">
         <v>13</v>
       </c>
       <c r="K3" s="4" t="s">
@@ -1026,7 +1033,7 @@
       </c>
     </row>
     <row r="4" spans="1:26" ht="63" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="42"/>
+      <c r="A4" s="44"/>
       <c r="B4" s="4" t="s">
         <v>12</v>
       </c>
@@ -1043,7 +1050,7 @@
       <c r="I4" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="J4" s="42"/>
+      <c r="J4" s="44"/>
       <c r="K4" s="4" t="s">
         <v>12</v>
       </c>
@@ -1070,7 +1077,7 @@
       </c>
     </row>
     <row r="5" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="42"/>
+      <c r="A5" s="44"/>
       <c r="B5" s="4" t="s">
         <v>9</v>
       </c>
@@ -1087,7 +1094,7 @@
       <c r="I5" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="J5" s="42"/>
+      <c r="J5" s="44"/>
       <c r="K5" s="4" t="s">
         <v>9</v>
       </c>
@@ -1114,7 +1121,7 @@
       </c>
     </row>
     <row r="6" spans="1:26" ht="62.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="41" t="s">
+      <c r="A6" s="43" t="s">
         <v>14</v>
       </c>
       <c r="B6" s="4" t="s">
@@ -1133,7 +1140,7 @@
       <c r="I6" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="J6" s="41" t="s">
+      <c r="J6" s="43" t="s">
         <v>14</v>
       </c>
       <c r="K6" s="4" t="s">
@@ -1162,7 +1169,7 @@
       </c>
     </row>
     <row r="7" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="42"/>
+      <c r="A7" s="44"/>
       <c r="B7" s="4" t="s">
         <v>8</v>
       </c>
@@ -1179,7 +1186,7 @@
       <c r="I7" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="J7" s="42"/>
+      <c r="J7" s="44"/>
       <c r="K7" s="4" t="s">
         <v>8</v>
       </c>
@@ -1206,7 +1213,7 @@
       </c>
     </row>
     <row r="8" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="42"/>
+      <c r="A8" s="44"/>
       <c r="B8" s="4" t="s">
         <v>9</v>
       </c>
@@ -1223,7 +1230,7 @@
       <c r="I8" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="J8" s="42"/>
+      <c r="J8" s="44"/>
       <c r="K8" s="4" t="s">
         <v>9</v>
       </c>
@@ -1250,7 +1257,7 @@
       </c>
     </row>
     <row r="9" spans="1:26" ht="64.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="41" t="s">
+      <c r="A9" s="43" t="s">
         <v>15</v>
       </c>
       <c r="B9" s="4" t="s">
@@ -1269,7 +1276,7 @@
       <c r="I9" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="J9" s="41" t="s">
+      <c r="J9" s="43" t="s">
         <v>15</v>
       </c>
       <c r="K9" s="4" t="s">
@@ -1298,7 +1305,7 @@
       </c>
     </row>
     <row r="10" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="42"/>
+      <c r="A10" s="44"/>
       <c r="B10" s="4" t="s">
         <v>8</v>
       </c>
@@ -1315,7 +1322,7 @@
       <c r="I10" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="J10" s="42"/>
+      <c r="J10" s="44"/>
       <c r="K10" s="4" t="s">
         <v>8</v>
       </c>
@@ -1342,7 +1349,7 @@
       </c>
     </row>
     <row r="11" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="42"/>
+      <c r="A11" s="44"/>
       <c r="B11" s="4" t="s">
         <v>9</v>
       </c>
@@ -1359,7 +1366,7 @@
       <c r="I11" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="J11" s="42"/>
+      <c r="J11" s="44"/>
       <c r="K11" s="4" t="s">
         <v>9</v>
       </c>
@@ -1386,7 +1393,7 @@
       </c>
     </row>
     <row r="12" spans="1:26" ht="64.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="41" t="s">
+      <c r="A12" s="43" t="s">
         <v>16</v>
       </c>
       <c r="B12" s="4" t="s">
@@ -1405,7 +1412,7 @@
       <c r="I12" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="J12" s="41" t="s">
+      <c r="J12" s="43" t="s">
         <v>16</v>
       </c>
       <c r="K12" s="4" t="s">
@@ -1434,7 +1441,7 @@
       </c>
     </row>
     <row r="13" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="42"/>
+      <c r="A13" s="44"/>
       <c r="B13" s="4" t="s">
         <v>8</v>
       </c>
@@ -1451,7 +1458,7 @@
       <c r="I13" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="J13" s="42"/>
+      <c r="J13" s="44"/>
       <c r="K13" s="4" t="s">
         <v>8</v>
       </c>
@@ -1478,7 +1485,7 @@
       </c>
     </row>
     <row r="14" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="42"/>
+      <c r="A14" s="44"/>
       <c r="B14" s="4" t="s">
         <v>9</v>
       </c>
@@ -1495,7 +1502,7 @@
       <c r="I14" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="J14" s="42"/>
+      <c r="J14" s="44"/>
       <c r="K14" s="4" t="s">
         <v>9</v>
       </c>
@@ -1522,7 +1529,7 @@
       </c>
     </row>
     <row r="15" spans="1:26" ht="64.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="41" t="s">
+      <c r="A15" s="43" t="s">
         <v>17</v>
       </c>
       <c r="B15" s="4" t="s">
@@ -1541,7 +1548,7 @@
       <c r="I15" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="J15" s="41" t="s">
+      <c r="J15" s="43" t="s">
         <v>17</v>
       </c>
       <c r="K15" s="4" t="s">
@@ -1570,7 +1577,7 @@
       </c>
     </row>
     <row r="16" spans="1:26" ht="77.400000000000006" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="42"/>
+      <c r="A16" s="44"/>
       <c r="B16" s="4" t="s">
         <v>8</v>
       </c>
@@ -1587,7 +1594,7 @@
       <c r="I16" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="J16" s="42"/>
+      <c r="J16" s="44"/>
       <c r="K16" s="4" t="s">
         <v>8</v>
       </c>
@@ -1614,7 +1621,7 @@
       </c>
     </row>
     <row r="17" spans="1:18" ht="63.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="42"/>
+      <c r="A17" s="44"/>
       <c r="B17" s="4" t="s">
         <v>9</v>
       </c>
@@ -1631,7 +1638,7 @@
       <c r="I17" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="J17" s="42"/>
+      <c r="J17" s="44"/>
       <c r="K17" s="4" t="s">
         <v>9</v>
       </c>
@@ -5595,11 +5602,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="K1:K2"/>
-    <mergeCell ref="L1:R1"/>
-    <mergeCell ref="J3:J5"/>
-    <mergeCell ref="J6:J8"/>
-    <mergeCell ref="C1:I1"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="J15:J17"/>
@@ -5611,6 +5613,11 @@
     <mergeCell ref="A3:A5"/>
     <mergeCell ref="A6:A8"/>
     <mergeCell ref="A9:A11"/>
+    <mergeCell ref="K1:K2"/>
+    <mergeCell ref="L1:R1"/>
+    <mergeCell ref="J3:J5"/>
+    <mergeCell ref="J6:J8"/>
+    <mergeCell ref="C1:I1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -5644,24 +5651,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="45" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="38" t="s">
+      <c r="B1" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="38" t="s">
+      <c r="C1" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="43" t="s">
+      <c r="D1" s="42" t="s">
         <v>41</v>
       </c>
-      <c r="E1" s="43"/>
-      <c r="F1" s="43"/>
-      <c r="G1" s="43"/>
-      <c r="H1" s="43"/>
-      <c r="I1" s="43"/>
-      <c r="J1" s="43"/>
+      <c r="E1" s="42"/>
+      <c r="F1" s="42"/>
+      <c r="G1" s="42"/>
+      <c r="H1" s="42"/>
+      <c r="I1" s="42"/>
+      <c r="J1" s="42"/>
       <c r="S1" s="1"/>
       <c r="T1" s="1"/>
       <c r="U1" s="1"/>
@@ -5672,9 +5679,9 @@
       <c r="Z1" s="1"/>
     </row>
     <row r="2" spans="1:26" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="39"/>
-      <c r="B2" s="39"/>
-      <c r="C2" s="39"/>
+      <c r="A2" s="41"/>
+      <c r="B2" s="41"/>
+      <c r="C2" s="41"/>
       <c r="D2" s="3" t="s">
         <v>2</v>
       </c>
@@ -5706,7 +5713,7 @@
       <c r="Z2" s="1"/>
     </row>
     <row r="3" spans="1:26" ht="47.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="41" t="s">
+      <c r="A3" s="43" t="s">
         <v>13</v>
       </c>
       <c r="B3" s="4" t="s">
@@ -5738,7 +5745,7 @@
       </c>
     </row>
     <row r="4" spans="1:26" ht="63" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="42"/>
+      <c r="A4" s="44"/>
       <c r="B4" s="4" t="s">
         <v>12</v>
       </c>
@@ -5768,7 +5775,7 @@
       </c>
     </row>
     <row r="5" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="42"/>
+      <c r="A5" s="44"/>
       <c r="B5" s="4" t="s">
         <v>9</v>
       </c>
@@ -5798,7 +5805,7 @@
       </c>
     </row>
     <row r="6" spans="1:26" ht="62.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="41" t="s">
+      <c r="A6" s="43" t="s">
         <v>14</v>
       </c>
       <c r="B6" s="4" t="s">
@@ -5830,7 +5837,7 @@
       </c>
     </row>
     <row r="7" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="42"/>
+      <c r="A7" s="44"/>
       <c r="B7" s="4" t="s">
         <v>8</v>
       </c>
@@ -5860,7 +5867,7 @@
       </c>
     </row>
     <row r="8" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="42"/>
+      <c r="A8" s="44"/>
       <c r="B8" s="4" t="s">
         <v>9</v>
       </c>
@@ -5890,7 +5897,7 @@
       </c>
     </row>
     <row r="9" spans="1:26" ht="64.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="41" t="s">
+      <c r="A9" s="43" t="s">
         <v>15</v>
       </c>
       <c r="B9" s="4" t="s">
@@ -5922,7 +5929,7 @@
       </c>
     </row>
     <row r="10" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="42"/>
+      <c r="A10" s="44"/>
       <c r="B10" s="4" t="s">
         <v>8</v>
       </c>
@@ -5952,7 +5959,7 @@
       </c>
     </row>
     <row r="11" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="42"/>
+      <c r="A11" s="44"/>
       <c r="B11" s="4" t="s">
         <v>9</v>
       </c>
@@ -5982,7 +5989,7 @@
       </c>
     </row>
     <row r="12" spans="1:26" ht="64.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="41" t="s">
+      <c r="A12" s="43" t="s">
         <v>16</v>
       </c>
       <c r="B12" s="4" t="s">
@@ -6014,7 +6021,7 @@
       </c>
     </row>
     <row r="13" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="42"/>
+      <c r="A13" s="44"/>
       <c r="B13" s="4" t="s">
         <v>8</v>
       </c>
@@ -6044,7 +6051,7 @@
       </c>
     </row>
     <row r="14" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="42"/>
+      <c r="A14" s="44"/>
       <c r="B14" s="4" t="s">
         <v>9</v>
       </c>
@@ -6074,7 +6081,7 @@
       </c>
     </row>
     <row r="15" spans="1:26" ht="64.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="41" t="s">
+      <c r="A15" s="43" t="s">
         <v>17</v>
       </c>
       <c r="B15" s="4" t="s">
@@ -6106,7 +6113,7 @@
       </c>
     </row>
     <row r="16" spans="1:26" ht="77.400000000000006" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="42"/>
+      <c r="A16" s="44"/>
       <c r="B16" s="4" t="s">
         <v>8</v>
       </c>
@@ -6136,7 +6143,7 @@
       </c>
     </row>
     <row r="17" spans="1:10" ht="63.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="42"/>
+      <c r="A17" s="44"/>
       <c r="B17" s="4" t="s">
         <v>9</v>
       </c>
@@ -10132,25 +10139,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="18" x14ac:dyDescent="0.4">
-      <c r="A1" s="47" t="s">
+      <c r="A1" s="49" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="47" t="s">
+      <c r="B1" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="46" t="s">
+      <c r="C1" s="48" t="s">
         <v>42</v>
       </c>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
-      <c r="F1" s="46"/>
-      <c r="G1" s="46"/>
-      <c r="H1" s="46"/>
-      <c r="I1" s="46"/>
+      <c r="D1" s="48"/>
+      <c r="E1" s="48"/>
+      <c r="F1" s="48"/>
+      <c r="G1" s="48"/>
+      <c r="H1" s="48"/>
+      <c r="I1" s="48"/>
     </row>
     <row r="2" spans="1:9" ht="18" x14ac:dyDescent="0.4">
-      <c r="A2" s="48"/>
-      <c r="B2" s="48"/>
+      <c r="A2" s="50"/>
+      <c r="B2" s="50"/>
       <c r="C2" s="14" t="s">
         <v>2</v>
       </c>
@@ -10174,7 +10181,7 @@
       </c>
     </row>
     <row r="3" spans="1:9" ht="87.5" x14ac:dyDescent="0.35">
-      <c r="A3" s="44" t="s">
+      <c r="A3" s="46" t="s">
         <v>13</v>
       </c>
       <c r="B3" s="15" t="s">
@@ -10203,7 +10210,7 @@
       </c>
     </row>
     <row r="4" spans="1:9" ht="105" x14ac:dyDescent="0.35">
-      <c r="A4" s="45"/>
+      <c r="A4" s="47"/>
       <c r="B4" s="15" t="s">
         <v>12</v>
       </c>
@@ -10230,7 +10237,7 @@
       </c>
     </row>
     <row r="5" spans="1:9" ht="52.5" x14ac:dyDescent="0.35">
-      <c r="A5" s="45"/>
+      <c r="A5" s="47"/>
       <c r="B5" s="15" t="s">
         <v>9</v>
       </c>
@@ -10257,7 +10264,7 @@
       </c>
     </row>
     <row r="6" spans="1:9" ht="157.5" x14ac:dyDescent="0.35">
-      <c r="A6" s="44" t="s">
+      <c r="A6" s="46" t="s">
         <v>14</v>
       </c>
       <c r="B6" s="15" t="s">
@@ -10286,7 +10293,7 @@
       </c>
     </row>
     <row r="7" spans="1:9" ht="157.5" x14ac:dyDescent="0.35">
-      <c r="A7" s="45"/>
+      <c r="A7" s="47"/>
       <c r="B7" s="15" t="s">
         <v>8</v>
       </c>
@@ -10313,7 +10320,7 @@
       </c>
     </row>
     <row r="8" spans="1:9" ht="70" x14ac:dyDescent="0.35">
-      <c r="A8" s="45"/>
+      <c r="A8" s="47"/>
       <c r="B8" s="15" t="s">
         <v>9</v>
       </c>
@@ -10340,7 +10347,7 @@
       </c>
     </row>
     <row r="9" spans="1:9" ht="140" x14ac:dyDescent="0.35">
-      <c r="A9" s="44" t="s">
+      <c r="A9" s="46" t="s">
         <v>15</v>
       </c>
       <c r="B9" s="15" t="s">
@@ -10369,7 +10376,7 @@
       </c>
     </row>
     <row r="10" spans="1:9" ht="157.5" x14ac:dyDescent="0.35">
-      <c r="A10" s="45"/>
+      <c r="A10" s="47"/>
       <c r="B10" s="15" t="s">
         <v>8</v>
       </c>
@@ -10396,7 +10403,7 @@
       </c>
     </row>
     <row r="11" spans="1:9" ht="70" x14ac:dyDescent="0.35">
-      <c r="A11" s="45"/>
+      <c r="A11" s="47"/>
       <c r="B11" s="15" t="s">
         <v>9</v>
       </c>
@@ -10423,7 +10430,7 @@
       </c>
     </row>
     <row r="12" spans="1:9" ht="157.5" x14ac:dyDescent="0.35">
-      <c r="A12" s="44" t="s">
+      <c r="A12" s="46" t="s">
         <v>16</v>
       </c>
       <c r="B12" s="15" t="s">
@@ -10452,7 +10459,7 @@
       </c>
     </row>
     <row r="13" spans="1:9" ht="157.5" x14ac:dyDescent="0.35">
-      <c r="A13" s="45"/>
+      <c r="A13" s="47"/>
       <c r="B13" s="15" t="s">
         <v>8</v>
       </c>
@@ -10479,7 +10486,7 @@
       </c>
     </row>
     <row r="14" spans="1:9" ht="175" x14ac:dyDescent="0.35">
-      <c r="A14" s="45"/>
+      <c r="A14" s="47"/>
       <c r="B14" s="15" t="s">
         <v>9</v>
       </c>
@@ -10506,7 +10513,7 @@
       </c>
     </row>
     <row r="15" spans="1:9" ht="105" x14ac:dyDescent="0.35">
-      <c r="A15" s="44" t="s">
+      <c r="A15" s="46" t="s">
         <v>17</v>
       </c>
       <c r="B15" s="15" t="s">
@@ -10535,7 +10542,7 @@
       </c>
     </row>
     <row r="16" spans="1:9" ht="157.5" x14ac:dyDescent="0.35">
-      <c r="A16" s="45"/>
+      <c r="A16" s="47"/>
       <c r="B16" s="15" t="s">
         <v>8</v>
       </c>
@@ -10562,7 +10569,7 @@
       </c>
     </row>
     <row r="17" spans="1:9" ht="70" x14ac:dyDescent="0.35">
-      <c r="A17" s="45"/>
+      <c r="A17" s="47"/>
       <c r="B17" s="15" t="s">
         <v>9</v>
       </c>
@@ -10623,25 +10630,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="18" x14ac:dyDescent="0.4">
-      <c r="A1" s="47" t="s">
+      <c r="A1" s="49" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="47" t="s">
+      <c r="B1" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="46" t="s">
+      <c r="C1" s="48" t="s">
         <v>64</v>
       </c>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
-      <c r="F1" s="46"/>
-      <c r="G1" s="46"/>
-      <c r="H1" s="46"/>
-      <c r="I1" s="46"/>
+      <c r="D1" s="48"/>
+      <c r="E1" s="48"/>
+      <c r="F1" s="48"/>
+      <c r="G1" s="48"/>
+      <c r="H1" s="48"/>
+      <c r="I1" s="48"/>
     </row>
     <row r="2" spans="1:9" ht="18" x14ac:dyDescent="0.4">
-      <c r="A2" s="48"/>
-      <c r="B2" s="48"/>
+      <c r="A2" s="50"/>
+      <c r="B2" s="50"/>
       <c r="C2" s="14" t="s">
         <v>2</v>
       </c>
@@ -10665,7 +10672,7 @@
       </c>
     </row>
     <row r="3" spans="1:9" ht="105" x14ac:dyDescent="0.35">
-      <c r="A3" s="44" t="s">
+      <c r="A3" s="46" t="s">
         <v>13</v>
       </c>
       <c r="B3" s="21" t="s">
@@ -10694,7 +10701,7 @@
       </c>
     </row>
     <row r="4" spans="1:9" ht="105" x14ac:dyDescent="0.35">
-      <c r="A4" s="45"/>
+      <c r="A4" s="47"/>
       <c r="B4" s="21" t="s">
         <v>12</v>
       </c>
@@ -10721,7 +10728,7 @@
       </c>
     </row>
     <row r="5" spans="1:9" ht="87.5" x14ac:dyDescent="0.35">
-      <c r="A5" s="45"/>
+      <c r="A5" s="47"/>
       <c r="B5" s="21" t="s">
         <v>9</v>
       </c>
@@ -10748,7 +10755,7 @@
       </c>
     </row>
     <row r="6" spans="1:9" ht="122.5" x14ac:dyDescent="0.35">
-      <c r="A6" s="44" t="s">
+      <c r="A6" s="46" t="s">
         <v>14</v>
       </c>
       <c r="B6" s="21" t="s">
@@ -10777,7 +10784,7 @@
       </c>
     </row>
     <row r="7" spans="1:9" ht="105" x14ac:dyDescent="0.35">
-      <c r="A7" s="45"/>
+      <c r="A7" s="47"/>
       <c r="B7" s="21" t="s">
         <v>8</v>
       </c>
@@ -10804,7 +10811,7 @@
       </c>
     </row>
     <row r="8" spans="1:9" ht="105" x14ac:dyDescent="0.35">
-      <c r="A8" s="45"/>
+      <c r="A8" s="47"/>
       <c r="B8" s="21" t="s">
         <v>9</v>
       </c>
@@ -10831,7 +10838,7 @@
       </c>
     </row>
     <row r="9" spans="1:9" ht="70" x14ac:dyDescent="0.35">
-      <c r="A9" s="44" t="s">
+      <c r="A9" s="46" t="s">
         <v>15</v>
       </c>
       <c r="B9" s="21" t="s">
@@ -10860,7 +10867,7 @@
       </c>
     </row>
     <row r="10" spans="1:9" ht="52.5" x14ac:dyDescent="0.35">
-      <c r="A10" s="45"/>
+      <c r="A10" s="47"/>
       <c r="B10" s="21" t="s">
         <v>8</v>
       </c>
@@ -10887,7 +10894,7 @@
       </c>
     </row>
     <row r="11" spans="1:9" ht="157.5" x14ac:dyDescent="0.35">
-      <c r="A11" s="45"/>
+      <c r="A11" s="47"/>
       <c r="B11" s="21" t="s">
         <v>9</v>
       </c>
@@ -10914,7 +10921,7 @@
       </c>
     </row>
     <row r="12" spans="1:9" ht="192.5" x14ac:dyDescent="0.35">
-      <c r="A12" s="44" t="s">
+      <c r="A12" s="46" t="s">
         <v>16</v>
       </c>
       <c r="B12" s="21" t="s">
@@ -10943,7 +10950,7 @@
       </c>
     </row>
     <row r="13" spans="1:9" ht="192.5" x14ac:dyDescent="0.35">
-      <c r="A13" s="45"/>
+      <c r="A13" s="47"/>
       <c r="B13" s="21" t="s">
         <v>8</v>
       </c>
@@ -10970,7 +10977,7 @@
       </c>
     </row>
     <row r="14" spans="1:9" ht="87.5" x14ac:dyDescent="0.35">
-      <c r="A14" s="45"/>
+      <c r="A14" s="47"/>
       <c r="B14" s="21" t="s">
         <v>9</v>
       </c>
@@ -10997,7 +11004,7 @@
       </c>
     </row>
     <row r="15" spans="1:9" ht="70" x14ac:dyDescent="0.35">
-      <c r="A15" s="44" t="s">
+      <c r="A15" s="46" t="s">
         <v>17</v>
       </c>
       <c r="B15" s="21" t="s">
@@ -11026,7 +11033,7 @@
       </c>
     </row>
     <row r="16" spans="1:9" ht="52.5" x14ac:dyDescent="0.35">
-      <c r="A16" s="45"/>
+      <c r="A16" s="47"/>
       <c r="B16" s="21" t="s">
         <v>8</v>
       </c>
@@ -11053,7 +11060,7 @@
       </c>
     </row>
     <row r="17" spans="1:9" ht="157.5" x14ac:dyDescent="0.35">
-      <c r="A17" s="45"/>
+      <c r="A17" s="47"/>
       <c r="B17" s="21" t="s">
         <v>9</v>
       </c>
@@ -11116,25 +11123,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="18" x14ac:dyDescent="0.4">
-      <c r="A1" s="47" t="s">
+      <c r="A1" s="49" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="47" t="s">
+      <c r="B1" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="46" t="s">
+      <c r="C1" s="48" t="s">
         <v>64</v>
       </c>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
-      <c r="F1" s="46"/>
-      <c r="G1" s="46"/>
-      <c r="H1" s="46"/>
-      <c r="I1" s="46"/>
+      <c r="D1" s="48"/>
+      <c r="E1" s="48"/>
+      <c r="F1" s="48"/>
+      <c r="G1" s="48"/>
+      <c r="H1" s="48"/>
+      <c r="I1" s="48"/>
     </row>
     <row r="2" spans="1:10" ht="18" x14ac:dyDescent="0.4">
-      <c r="A2" s="48"/>
-      <c r="B2" s="48"/>
+      <c r="A2" s="50"/>
+      <c r="B2" s="50"/>
       <c r="C2" s="14" t="s">
         <v>2</v>
       </c>
@@ -11158,7 +11165,7 @@
       </c>
     </row>
     <row r="3" spans="1:10" ht="192.5" x14ac:dyDescent="0.35">
-      <c r="A3" s="44" t="s">
+      <c r="A3" s="46" t="s">
         <v>13</v>
       </c>
       <c r="B3" s="23" t="s">
@@ -11187,7 +11194,7 @@
       </c>
     </row>
     <row r="4" spans="1:10" ht="140" x14ac:dyDescent="0.35">
-      <c r="A4" s="45"/>
+      <c r="A4" s="47"/>
       <c r="B4" s="23" t="s">
         <v>12</v>
       </c>
@@ -11214,7 +11221,7 @@
       </c>
     </row>
     <row r="5" spans="1:10" ht="52.5" x14ac:dyDescent="0.35">
-      <c r="A5" s="45"/>
+      <c r="A5" s="47"/>
       <c r="B5" s="23" t="s">
         <v>9</v>
       </c>
@@ -11241,7 +11248,7 @@
       </c>
     </row>
     <row r="6" spans="1:10" ht="192.5" x14ac:dyDescent="0.35">
-      <c r="A6" s="44" t="s">
+      <c r="A6" s="46" t="s">
         <v>14</v>
       </c>
       <c r="B6" s="23" t="s">
@@ -11270,7 +11277,7 @@
       </c>
     </row>
     <row r="7" spans="1:10" ht="140" x14ac:dyDescent="0.35">
-      <c r="A7" s="45"/>
+      <c r="A7" s="47"/>
       <c r="B7" s="23" t="s">
         <v>8</v>
       </c>
@@ -11297,7 +11304,7 @@
       </c>
     </row>
     <row r="8" spans="1:10" ht="52.5" x14ac:dyDescent="0.35">
-      <c r="A8" s="45"/>
+      <c r="A8" s="47"/>
       <c r="B8" s="23" t="s">
         <v>9</v>
       </c>
@@ -11324,7 +11331,7 @@
       </c>
     </row>
     <row r="9" spans="1:10" ht="157.5" x14ac:dyDescent="0.35">
-      <c r="A9" s="44" t="s">
+      <c r="A9" s="46" t="s">
         <v>15</v>
       </c>
       <c r="B9" s="23" t="s">
@@ -11353,7 +11360,7 @@
       </c>
     </row>
     <row r="10" spans="1:10" ht="140" x14ac:dyDescent="0.35">
-      <c r="A10" s="45"/>
+      <c r="A10" s="47"/>
       <c r="B10" s="23" t="s">
         <v>8</v>
       </c>
@@ -11380,7 +11387,7 @@
       </c>
     </row>
     <row r="11" spans="1:10" ht="52.5" x14ac:dyDescent="0.35">
-      <c r="A11" s="45"/>
+      <c r="A11" s="47"/>
       <c r="B11" s="23" t="s">
         <v>9</v>
       </c>
@@ -11407,7 +11414,7 @@
       </c>
     </row>
     <row r="12" spans="1:10" ht="192.5" x14ac:dyDescent="0.35">
-      <c r="A12" s="44" t="s">
+      <c r="A12" s="46" t="s">
         <v>16</v>
       </c>
       <c r="B12" s="23" t="s">
@@ -11436,7 +11443,7 @@
       </c>
     </row>
     <row r="13" spans="1:10" ht="140" x14ac:dyDescent="0.35">
-      <c r="A13" s="45"/>
+      <c r="A13" s="47"/>
       <c r="B13" s="23" t="s">
         <v>8</v>
       </c>
@@ -11463,7 +11470,7 @@
       </c>
     </row>
     <row r="14" spans="1:10" ht="52.5" x14ac:dyDescent="0.35">
-      <c r="A14" s="45"/>
+      <c r="A14" s="47"/>
       <c r="B14" s="23" t="s">
         <v>9</v>
       </c>
@@ -11490,7 +11497,7 @@
       </c>
     </row>
     <row r="15" spans="1:10" ht="192.5" x14ac:dyDescent="0.35">
-      <c r="A15" s="44" t="s">
+      <c r="A15" s="46" t="s">
         <v>17</v>
       </c>
       <c r="B15" s="23" t="s">
@@ -11522,7 +11529,7 @@
       </c>
     </row>
     <row r="16" spans="1:10" ht="157.5" x14ac:dyDescent="0.35">
-      <c r="A16" s="45"/>
+      <c r="A16" s="47"/>
       <c r="B16" s="23" t="s">
         <v>8</v>
       </c>
@@ -11552,7 +11559,7 @@
       </c>
     </row>
     <row r="17" spans="1:10" ht="52.5" x14ac:dyDescent="0.35">
-      <c r="A17" s="45"/>
+      <c r="A17" s="47"/>
       <c r="B17" s="23" t="s">
         <v>9</v>
       </c>
@@ -11601,8 +11608,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B35242D0-2AD6-442D-ABA4-BF0550EDBCE1}">
   <dimension ref="A1:J17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.453125" defaultRowHeight="17.5" x14ac:dyDescent="0.35"/>
@@ -11618,25 +11625,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="18" x14ac:dyDescent="0.4">
-      <c r="A1" s="47" t="s">
+      <c r="A1" s="49" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="47" t="s">
+      <c r="B1" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="46" t="s">
+      <c r="C1" s="48" t="s">
         <v>64</v>
       </c>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
-      <c r="F1" s="46"/>
-      <c r="G1" s="46"/>
-      <c r="H1" s="46"/>
-      <c r="I1" s="46"/>
+      <c r="D1" s="48"/>
+      <c r="E1" s="48"/>
+      <c r="F1" s="48"/>
+      <c r="G1" s="48"/>
+      <c r="H1" s="48"/>
+      <c r="I1" s="48"/>
     </row>
     <row r="2" spans="1:10" ht="18" x14ac:dyDescent="0.4">
-      <c r="A2" s="48"/>
-      <c r="B2" s="48"/>
+      <c r="A2" s="50"/>
+      <c r="B2" s="50"/>
       <c r="C2" s="14" t="s">
         <v>2</v>
       </c>
@@ -11660,7 +11667,7 @@
       </c>
     </row>
     <row r="3" spans="1:10" ht="35" x14ac:dyDescent="0.35">
-      <c r="A3" s="44" t="s">
+      <c r="A3" s="46" t="s">
         <v>13</v>
       </c>
       <c r="B3" s="36" t="s">
@@ -11689,7 +11696,7 @@
       </c>
     </row>
     <row r="4" spans="1:10" ht="35" x14ac:dyDescent="0.35">
-      <c r="A4" s="45"/>
+      <c r="A4" s="47"/>
       <c r="B4" s="36" t="s">
         <v>12</v>
       </c>
@@ -11716,7 +11723,7 @@
       </c>
     </row>
     <row r="5" spans="1:10" ht="52.5" x14ac:dyDescent="0.35">
-      <c r="A5" s="45"/>
+      <c r="A5" s="47"/>
       <c r="B5" s="36" t="s">
         <v>9</v>
       </c>
@@ -11743,7 +11750,7 @@
       </c>
     </row>
     <row r="6" spans="1:10" ht="87.5" x14ac:dyDescent="0.35">
-      <c r="A6" s="44" t="s">
+      <c r="A6" s="46" t="s">
         <v>14</v>
       </c>
       <c r="B6" s="36" t="s">
@@ -11772,7 +11779,7 @@
       </c>
     </row>
     <row r="7" spans="1:10" ht="52.5" x14ac:dyDescent="0.35">
-      <c r="A7" s="45"/>
+      <c r="A7" s="47"/>
       <c r="B7" s="36" t="s">
         <v>8</v>
       </c>
@@ -11799,7 +11806,7 @@
       </c>
     </row>
     <row r="8" spans="1:10" ht="52.5" x14ac:dyDescent="0.35">
-      <c r="A8" s="45"/>
+      <c r="A8" s="47"/>
       <c r="B8" s="36" t="s">
         <v>9</v>
       </c>
@@ -11826,7 +11833,7 @@
       </c>
     </row>
     <row r="9" spans="1:10" ht="105" x14ac:dyDescent="0.35">
-      <c r="A9" s="44" t="s">
+      <c r="A9" s="46" t="s">
         <v>15</v>
       </c>
       <c r="B9" s="36" t="s">
@@ -11855,7 +11862,7 @@
       </c>
     </row>
     <row r="10" spans="1:10" ht="87.5" x14ac:dyDescent="0.35">
-      <c r="A10" s="45"/>
+      <c r="A10" s="47"/>
       <c r="B10" s="36" t="s">
         <v>8</v>
       </c>
@@ -11882,7 +11889,7 @@
       </c>
     </row>
     <row r="11" spans="1:10" ht="70" x14ac:dyDescent="0.35">
-      <c r="A11" s="45"/>
+      <c r="A11" s="47"/>
       <c r="B11" s="36" t="s">
         <v>9</v>
       </c>
@@ -11909,7 +11916,7 @@
       </c>
     </row>
     <row r="12" spans="1:10" ht="35" x14ac:dyDescent="0.35">
-      <c r="A12" s="44" t="s">
+      <c r="A12" s="46" t="s">
         <v>16</v>
       </c>
       <c r="B12" s="36" t="s">
@@ -11938,7 +11945,7 @@
       </c>
     </row>
     <row r="13" spans="1:10" ht="87.5" x14ac:dyDescent="0.35">
-      <c r="A13" s="45"/>
+      <c r="A13" s="47"/>
       <c r="B13" s="36" t="s">
         <v>8</v>
       </c>
@@ -11965,7 +11972,7 @@
       </c>
     </row>
     <row r="14" spans="1:10" ht="52.5" x14ac:dyDescent="0.35">
-      <c r="A14" s="45"/>
+      <c r="A14" s="47"/>
       <c r="B14" s="36" t="s">
         <v>9</v>
       </c>
@@ -11992,7 +11999,7 @@
       </c>
     </row>
     <row r="15" spans="1:10" ht="87.5" x14ac:dyDescent="0.35">
-      <c r="A15" s="44" t="s">
+      <c r="A15" s="46" t="s">
         <v>17</v>
       </c>
       <c r="B15" s="36" t="s">
@@ -12022,7 +12029,7 @@
       <c r="J15" s="25"/>
     </row>
     <row r="16" spans="1:10" ht="52.5" x14ac:dyDescent="0.35">
-      <c r="A16" s="45"/>
+      <c r="A16" s="47"/>
       <c r="B16" s="36" t="s">
         <v>8</v>
       </c>
@@ -12050,7 +12057,7 @@
       <c r="J16" s="25"/>
     </row>
     <row r="17" spans="1:10" ht="52.5" x14ac:dyDescent="0.35">
-      <c r="A17" s="45"/>
+      <c r="A17" s="47"/>
       <c r="B17" s="36" t="s">
         <v>9</v>
       </c>
@@ -12075,6 +12082,320 @@
       <c r="I17" s="25" t="s">
         <v>30</v>
       </c>
+      <c r="J17" s="25"/>
+    </row>
+  </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="A12:A14"/>
+    <mergeCell ref="A15:A17"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:I1"/>
+    <mergeCell ref="A3:A5"/>
+    <mergeCell ref="A6:A8"/>
+    <mergeCell ref="A9:A11"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA7F8344-AAAE-454A-B8B2-31F07E61DB11}">
+  <dimension ref="A1:J17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10:C11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="17.453125" defaultRowHeight="17.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="2" width="17.453125" style="39"/>
+    <col min="3" max="3" width="20.54296875" style="39" customWidth="1"/>
+    <col min="4" max="4" width="36.90625" style="39" customWidth="1"/>
+    <col min="5" max="5" width="26.6328125" style="39" customWidth="1"/>
+    <col min="6" max="6" width="26.36328125" style="39" customWidth="1"/>
+    <col min="7" max="7" width="23.54296875" style="39" customWidth="1"/>
+    <col min="8" max="8" width="20.81640625" style="39" customWidth="1"/>
+    <col min="9" max="16384" width="17.453125" style="39"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="18" x14ac:dyDescent="0.4">
+      <c r="A1" s="49" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="49" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="48" t="s">
+        <v>64</v>
+      </c>
+      <c r="D1" s="48"/>
+      <c r="E1" s="48"/>
+      <c r="F1" s="48"/>
+      <c r="G1" s="48"/>
+      <c r="H1" s="48"/>
+      <c r="I1" s="48"/>
+    </row>
+    <row r="2" spans="1:10" ht="18" x14ac:dyDescent="0.4">
+      <c r="A2" s="50"/>
+      <c r="B2" s="50"/>
+      <c r="C2" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="I2" s="14" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="35" x14ac:dyDescent="0.35">
+      <c r="A3" s="46" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="38" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="25" t="s">
+        <v>55</v>
+      </c>
+      <c r="D3" s="25"/>
+      <c r="E3" s="25"/>
+      <c r="F3" s="25"/>
+      <c r="G3" s="25"/>
+      <c r="H3" s="25"/>
+      <c r="I3" s="25"/>
+    </row>
+    <row r="4" spans="1:10" ht="35" x14ac:dyDescent="0.35">
+      <c r="A4" s="47"/>
+      <c r="B4" s="38" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="25" t="s">
+        <v>55</v>
+      </c>
+      <c r="D4" s="25"/>
+      <c r="E4" s="25"/>
+      <c r="F4" s="25"/>
+      <c r="G4" s="25"/>
+      <c r="H4" s="25"/>
+      <c r="I4" s="25"/>
+    </row>
+    <row r="5" spans="1:10" ht="52.5" x14ac:dyDescent="0.35">
+      <c r="A5" s="47"/>
+      <c r="B5" s="38" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="D5" s="25"/>
+      <c r="E5" s="25"/>
+      <c r="F5" s="25"/>
+      <c r="G5" s="25"/>
+      <c r="H5" s="25"/>
+      <c r="I5" s="25"/>
+    </row>
+    <row r="6" spans="1:10" ht="35" x14ac:dyDescent="0.35">
+      <c r="A6" s="46" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="38" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="25" t="s">
+        <v>102</v>
+      </c>
+      <c r="D6" s="25"/>
+      <c r="E6" s="25"/>
+      <c r="F6" s="25"/>
+      <c r="G6" s="25"/>
+      <c r="H6" s="25"/>
+      <c r="I6" s="25"/>
+    </row>
+    <row r="7" spans="1:10" ht="52.5" x14ac:dyDescent="0.35">
+      <c r="A7" s="47"/>
+      <c r="B7" s="38" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="25" t="s">
+        <v>102</v>
+      </c>
+      <c r="D7" s="25"/>
+      <c r="E7" s="25"/>
+      <c r="F7" s="25"/>
+      <c r="G7" s="25"/>
+      <c r="H7" s="25"/>
+      <c r="I7" s="25"/>
+    </row>
+    <row r="8" spans="1:10" ht="52.5" x14ac:dyDescent="0.35">
+      <c r="A8" s="47"/>
+      <c r="B8" s="38" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" s="25"/>
+      <c r="E8" s="25"/>
+      <c r="F8" s="25"/>
+      <c r="G8" s="25"/>
+      <c r="H8" s="25"/>
+      <c r="I8" s="25"/>
+    </row>
+    <row r="9" spans="1:10" ht="52.5" x14ac:dyDescent="0.35">
+      <c r="A9" s="46" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="38" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="25" t="s">
+        <v>101</v>
+      </c>
+      <c r="D9" s="25"/>
+      <c r="E9" s="25"/>
+      <c r="F9" s="25"/>
+      <c r="G9" s="25"/>
+      <c r="H9" s="25"/>
+      <c r="I9" s="25"/>
+    </row>
+    <row r="10" spans="1:10" ht="52.5" x14ac:dyDescent="0.35">
+      <c r="A10" s="47"/>
+      <c r="B10" s="38" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="25" t="s">
+        <v>55</v>
+      </c>
+      <c r="D10" s="25"/>
+      <c r="E10" s="25"/>
+      <c r="G10" s="25"/>
+      <c r="H10" s="25"/>
+      <c r="I10" s="25"/>
+    </row>
+    <row r="11" spans="1:10" ht="52.5" x14ac:dyDescent="0.35">
+      <c r="A11" s="47"/>
+      <c r="B11" s="38" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="D11" s="25"/>
+      <c r="E11" s="25"/>
+      <c r="F11" s="25"/>
+      <c r="G11" s="25"/>
+      <c r="H11" s="25"/>
+      <c r="I11" s="25"/>
+    </row>
+    <row r="12" spans="1:10" ht="35" x14ac:dyDescent="0.35">
+      <c r="A12" s="46" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" s="38" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" s="25" t="s">
+        <v>55</v>
+      </c>
+      <c r="D12" s="25"/>
+      <c r="E12" s="25"/>
+      <c r="F12" s="25"/>
+      <c r="G12" s="25"/>
+      <c r="H12" s="25"/>
+      <c r="I12" s="25"/>
+    </row>
+    <row r="13" spans="1:10" ht="52.5" x14ac:dyDescent="0.35">
+      <c r="A13" s="47"/>
+      <c r="B13" s="38" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" s="25" t="s">
+        <v>55</v>
+      </c>
+      <c r="D13" s="25"/>
+      <c r="E13" s="25"/>
+      <c r="F13" s="25"/>
+      <c r="G13" s="25"/>
+      <c r="H13" s="25"/>
+      <c r="I13" s="25"/>
+    </row>
+    <row r="14" spans="1:10" ht="52.5" x14ac:dyDescent="0.35">
+      <c r="A14" s="47"/>
+      <c r="B14" s="38" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="D14" s="25"/>
+      <c r="E14" s="25"/>
+      <c r="F14" s="25"/>
+      <c r="G14" s="25"/>
+      <c r="H14" s="25"/>
+      <c r="I14" s="25"/>
+    </row>
+    <row r="15" spans="1:10" ht="35" x14ac:dyDescent="0.35">
+      <c r="A15" s="46" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15" s="38" t="s">
+        <v>7</v>
+      </c>
+      <c r="C15" s="25" t="s">
+        <v>55</v>
+      </c>
+      <c r="D15" s="25"/>
+      <c r="E15" s="25"/>
+      <c r="F15" s="25"/>
+      <c r="G15" s="25"/>
+      <c r="H15" s="25"/>
+      <c r="I15" s="25"/>
+      <c r="J15" s="25"/>
+    </row>
+    <row r="16" spans="1:10" ht="52.5" x14ac:dyDescent="0.35">
+      <c r="A16" s="47"/>
+      <c r="B16" s="38" t="s">
+        <v>8</v>
+      </c>
+      <c r="C16" s="25" t="s">
+        <v>55</v>
+      </c>
+      <c r="D16" s="25"/>
+      <c r="E16" s="25"/>
+      <c r="G16" s="25"/>
+      <c r="H16" s="25"/>
+      <c r="I16" s="25"/>
+      <c r="J16" s="25"/>
+    </row>
+    <row r="17" spans="1:10" ht="52.5" x14ac:dyDescent="0.35">
+      <c r="A17" s="47"/>
+      <c r="B17" s="38" t="s">
+        <v>9</v>
+      </c>
+      <c r="C17" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="D17" s="25"/>
+      <c r="E17" s="25"/>
+      <c r="F17" s="25"/>
+      <c r="G17" s="25"/>
+      <c r="H17" s="25"/>
+      <c r="I17" s="25"/>
       <c r="J17" s="25"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated du (week11 tues)
</commit_message>
<xml_diff>
--- a/metrics/du.xlsx
+++ b/metrics/du.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\project-g4t6\metrics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B1F98EF-A727-44D8-B297-6027C5137F90}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A451A0B-0335-490C-93B9-F0F7B47D963E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="949" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="964" uniqueCount="109">
   <si>
     <t>Question</t>
   </si>
@@ -156,15 +156,6 @@
     <t>Continued coding the boostrap validation implementation</t>
   </si>
   <si>
-    <t>Week: 15/09/2019 to 21/09/2019</t>
-  </si>
-  <si>
-    <t>Week: 22/09/2019 to 28/09/2019</t>
-  </si>
-  <si>
-    <t>Week: 29/09/2019 to 05/10/2019</t>
-  </si>
-  <si>
     <t>Conducted a meeting with the team. See minutes for more details</t>
   </si>
   <si>
@@ -226,9 +217,6 @@
   </si>
   <si>
     <t xml:space="preserve">Team Meeting. Refer to minutes for more details &amp; redirect login page for admin </t>
-  </si>
-  <si>
-    <t>Week: 6/10/2019 to 12/10/2019</t>
   </si>
   <si>
     <t xml:space="preserve">Had difficulty retrieving data as output was none from a method from the bids table through the BidDAO’s retrieveStudentBidsWithInfo($userid) was resolve after an hour. </t>
@@ -357,6 +345,38 @@
   </si>
   <si>
     <t>JSON- dump(bids)</t>
+  </si>
+  <si>
+    <t>Week: 28/10/2019 to 03/11/2019</t>
+  </si>
+  <si>
+    <t>Week: 21/10/2019 to 27/10/2019</t>
+  </si>
+  <si>
+    <t>Week: 14/10/2019 to 20/10/2019</t>
+  </si>
+  <si>
+    <t>Week: 7/10/2019 to 13/10/2019</t>
+  </si>
+  <si>
+    <t>Week: 30/09/2019 to 06/10/2019</t>
+  </si>
+  <si>
+    <t>Week: 23/09/2019 to 29/09/2019</t>
+  </si>
+  <si>
+    <t>Week: 16/09/2019 to 22/09/2019</t>
+  </si>
+  <si>
+    <t>Auto-testcases</t>
+  </si>
+  <si>
+    <t>Manual testcases
+Updated Schedule</t>
+  </si>
+  <si>
+    <t>Not a working day 
+Updated Schedule</t>
   </si>
 </sst>
 </file>
@@ -553,15 +573,15 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -863,7 +883,7 @@
   </sheetPr>
   <dimension ref="A1:Z1001"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="83" zoomScaleNormal="130" workbookViewId="0">
       <pane xSplit="2" topLeftCell="L1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="L1" sqref="L1:R1"/>
     </sheetView>
@@ -889,36 +909,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="42" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="42" t="s">
+      <c r="C1" s="45" t="s">
         <v>18</v>
       </c>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42"/>
-      <c r="G1" s="42"/>
-      <c r="H1" s="42"/>
-      <c r="I1" s="42"/>
-      <c r="J1" s="45" t="s">
+      <c r="D1" s="45"/>
+      <c r="E1" s="45"/>
+      <c r="F1" s="45"/>
+      <c r="G1" s="45"/>
+      <c r="H1" s="45"/>
+      <c r="I1" s="45"/>
+      <c r="J1" s="42" t="s">
         <v>1</v>
       </c>
       <c r="K1" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="L1" s="42" t="s">
-        <v>40</v>
-      </c>
-      <c r="M1" s="42"/>
-      <c r="N1" s="42"/>
-      <c r="O1" s="42"/>
-      <c r="P1" s="42"/>
-      <c r="Q1" s="42"/>
-      <c r="R1" s="42"/>
+      <c r="L1" s="45" t="s">
+        <v>105</v>
+      </c>
+      <c r="M1" s="45"/>
+      <c r="N1" s="45"/>
+      <c r="O1" s="45"/>
+      <c r="P1" s="45"/>
+      <c r="Q1" s="45"/>
+      <c r="R1" s="45"/>
       <c r="S1" s="1"/>
       <c r="T1" s="1"/>
       <c r="U1" s="1"/>
@@ -5602,6 +5622,11 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="K1:K2"/>
+    <mergeCell ref="L1:R1"/>
+    <mergeCell ref="J3:J5"/>
+    <mergeCell ref="J6:J8"/>
+    <mergeCell ref="C1:I1"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="J15:J17"/>
@@ -5613,11 +5638,6 @@
     <mergeCell ref="A3:A5"/>
     <mergeCell ref="A6:A8"/>
     <mergeCell ref="A9:A11"/>
-    <mergeCell ref="K1:K2"/>
-    <mergeCell ref="L1:R1"/>
-    <mergeCell ref="J3:J5"/>
-    <mergeCell ref="J6:J8"/>
-    <mergeCell ref="C1:I1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -5631,9 +5651,9 @@
   </sheetPr>
   <dimension ref="A1:Z1001"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="79" zoomScaleNormal="130" workbookViewId="0">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="F8" sqref="F8"/>
+      <selection pane="topRight" activeCell="D1" sqref="D1:J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -5651,7 +5671,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="42" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="40" t="s">
@@ -5660,15 +5680,15 @@
       <c r="C1" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="42" t="s">
-        <v>41</v>
-      </c>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42"/>
-      <c r="G1" s="42"/>
-      <c r="H1" s="42"/>
-      <c r="I1" s="42"/>
-      <c r="J1" s="42"/>
+      <c r="D1" s="45" t="s">
+        <v>104</v>
+      </c>
+      <c r="E1" s="45"/>
+      <c r="F1" s="45"/>
+      <c r="G1" s="45"/>
+      <c r="H1" s="45"/>
+      <c r="I1" s="45"/>
+      <c r="J1" s="45"/>
       <c r="S1" s="1"/>
       <c r="T1" s="1"/>
       <c r="U1" s="1"/>
@@ -10129,8 +10149,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32A3AA99-F4D2-4A92-BF2C-95E1F810A93F}">
   <dimension ref="A1:I17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.453125" defaultRowHeight="17.5" x14ac:dyDescent="0.35"/>
@@ -10146,7 +10166,7 @@
         <v>0</v>
       </c>
       <c r="C1" s="48" t="s">
-        <v>42</v>
+        <v>103</v>
       </c>
       <c r="D1" s="48"/>
       <c r="E1" s="48"/>
@@ -10191,22 +10211,22 @@
         <v>19</v>
       </c>
       <c r="D3" s="25" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E3" s="25" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="F3" s="25" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="G3" s="25" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="H3" s="25" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="I3" s="25" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="105" x14ac:dyDescent="0.35">
@@ -10215,25 +10235,25 @@
         <v>12</v>
       </c>
       <c r="C4" s="25" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D4" s="25" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="E4" s="25" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="F4" s="25" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="G4" s="25" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="H4" s="25" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="I4" s="25" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="52.5" x14ac:dyDescent="0.35">
@@ -10245,22 +10265,22 @@
         <v>30</v>
       </c>
       <c r="D5" s="25" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="E5" s="25" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="F5" s="29" t="s">
         <v>30</v>
       </c>
       <c r="G5" s="25" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="H5" s="25" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="I5" s="25" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="157.5" x14ac:dyDescent="0.35">
@@ -10274,22 +10294,22 @@
         <v>39</v>
       </c>
       <c r="D6" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="E6" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="E6" s="25" t="s">
-        <v>49</v>
-      </c>
       <c r="F6" s="25" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="G6" s="25" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="H6" s="25" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="I6" s="25" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="157.5" x14ac:dyDescent="0.35">
@@ -10298,25 +10318,25 @@
         <v>8</v>
       </c>
       <c r="C7" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="D7" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="D7" s="25" t="s">
-        <v>49</v>
-      </c>
       <c r="E7" s="25" t="s">
+        <v>57</v>
+      </c>
+      <c r="F7" s="25" t="s">
         <v>60</v>
       </c>
-      <c r="F7" s="25" t="s">
-        <v>63</v>
-      </c>
       <c r="G7" s="25" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="H7" s="25" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="I7" s="25" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="70" x14ac:dyDescent="0.35">
@@ -10325,10 +10345,10 @@
         <v>9</v>
       </c>
       <c r="C8" s="25" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D8" s="25" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E8" s="29" t="s">
         <v>30</v>
@@ -10337,13 +10357,13 @@
         <v>30</v>
       </c>
       <c r="G8" s="25" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="H8" s="25" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="I8" s="25" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="140" x14ac:dyDescent="0.35">
@@ -10357,22 +10377,22 @@
         <v>39</v>
       </c>
       <c r="D9" s="25" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="E9" s="25" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="F9" s="25" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="G9" s="25" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="H9" s="25" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="I9" s="25" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="157.5" x14ac:dyDescent="0.35">
@@ -10381,25 +10401,25 @@
         <v>8</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D10" s="25" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E10" s="25" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="F10" s="25" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="G10" s="25" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="H10" s="25" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="I10" s="25" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="70" x14ac:dyDescent="0.35">
@@ -10408,25 +10428,25 @@
         <v>9</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D11" s="27" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E11" s="27" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="F11" s="20" t="s">
         <v>30</v>
       </c>
       <c r="G11" s="27" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="H11" s="27" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="I11" s="27" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="157.5" x14ac:dyDescent="0.35">
@@ -10440,22 +10460,22 @@
         <v>39</v>
       </c>
       <c r="D12" s="12" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="E12" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="F12" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="G12" s="17" t="s">
         <v>58</v>
       </c>
-      <c r="F12" s="16" t="s">
-        <v>55</v>
-      </c>
-      <c r="G12" s="17" t="s">
-        <v>61</v>
-      </c>
       <c r="H12" s="18" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="I12" s="18" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="157.5" x14ac:dyDescent="0.35">
@@ -10464,25 +10484,25 @@
         <v>8</v>
       </c>
       <c r="C13" s="25" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D13" s="25" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="E13" s="25" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="F13" s="25" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="G13" s="25" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="H13" s="25" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="I13" s="25" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="175" x14ac:dyDescent="0.35">
@@ -10491,25 +10511,25 @@
         <v>9</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D14" s="12" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="E14" s="13" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="F14" s="20" t="s">
         <v>30</v>
       </c>
       <c r="G14" s="27" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="H14" s="27" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="I14" s="27" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="105" x14ac:dyDescent="0.35">
@@ -10523,22 +10543,22 @@
         <v>39</v>
       </c>
       <c r="D15" s="12" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="E15" s="13" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="F15" s="16" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="G15" s="17" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="H15" s="18" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="I15" s="18" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="157.5" x14ac:dyDescent="0.35">
@@ -10547,25 +10567,25 @@
         <v>8</v>
       </c>
       <c r="C16" s="12" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D16" s="12" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="E16" s="13" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="F16" s="12" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="G16" s="17" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="H16" s="18" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="I16" s="18" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="70" x14ac:dyDescent="0.35">
@@ -10574,25 +10594,25 @@
         <v>9</v>
       </c>
       <c r="C17" s="12" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D17" s="12" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="E17" s="13" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="F17" s="20" t="s">
         <v>30</v>
       </c>
       <c r="G17" s="27" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="H17" s="27" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="I17" s="27" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -10615,8 +10635,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4B6745F-6AD3-49D1-88C7-6568265E6BB1}">
   <dimension ref="A1:I17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.453125" defaultRowHeight="17.5" x14ac:dyDescent="0.35"/>
@@ -10637,7 +10657,7 @@
         <v>0</v>
       </c>
       <c r="C1" s="48" t="s">
-        <v>64</v>
+        <v>102</v>
       </c>
       <c r="D1" s="48"/>
       <c r="E1" s="48"/>
@@ -10679,25 +10699,25 @@
         <v>7</v>
       </c>
       <c r="C3" s="25" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D3" s="25" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E3" s="25" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="F3" s="25" t="s">
+        <v>62</v>
+      </c>
+      <c r="G3" s="25" t="s">
         <v>66</v>
       </c>
-      <c r="G3" s="25" t="s">
-        <v>70</v>
-      </c>
       <c r="H3" s="25" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="I3" s="26" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="105" x14ac:dyDescent="0.35">
@@ -10706,25 +10726,25 @@
         <v>12</v>
       </c>
       <c r="C4" s="25" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D4" s="25" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E4" s="25" t="s">
+        <v>62</v>
+      </c>
+      <c r="F4" s="25" t="s">
         <v>66</v>
       </c>
-      <c r="F4" s="25" t="s">
-        <v>70</v>
-      </c>
       <c r="G4" s="25" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="H4" s="26" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="I4" s="25" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="87.5" x14ac:dyDescent="0.35">
@@ -10733,25 +10753,25 @@
         <v>9</v>
       </c>
       <c r="C5" s="25" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D5" s="25" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E5" s="25" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="F5" s="31" t="s">
         <v>30</v>
       </c>
       <c r="G5" s="25" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="H5" s="25" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="I5" s="19" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="122.5" x14ac:dyDescent="0.35">
@@ -10762,25 +10782,25 @@
         <v>7</v>
       </c>
       <c r="C6" s="19" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D6" s="19" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E6" s="28" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="F6" s="28" t="s">
+        <v>62</v>
+      </c>
+      <c r="G6" s="25" t="s">
         <v>66</v>
       </c>
-      <c r="G6" s="25" t="s">
-        <v>70</v>
-      </c>
       <c r="H6" s="25" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="I6" s="26" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="105" x14ac:dyDescent="0.35">
@@ -10789,25 +10809,25 @@
         <v>8</v>
       </c>
       <c r="C7" s="27" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D7" s="27" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E7" s="28" t="s">
+        <v>62</v>
+      </c>
+      <c r="F7" s="25" t="s">
         <v>66</v>
       </c>
-      <c r="F7" s="25" t="s">
-        <v>70</v>
-      </c>
       <c r="G7" s="25" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="H7" s="26" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="I7" s="25" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="105" x14ac:dyDescent="0.35">
@@ -10816,28 +10836,28 @@
         <v>9</v>
       </c>
       <c r="C8" s="28" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D8" s="28" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E8" s="28" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="F8" s="31" t="s">
         <v>30</v>
       </c>
       <c r="G8" s="25" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="H8" s="25" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="I8" s="24" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="70" x14ac:dyDescent="0.35">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="52.5" x14ac:dyDescent="0.35">
       <c r="A9" s="46" t="s">
         <v>15</v>
       </c>
@@ -10845,25 +10865,25 @@
         <v>7</v>
       </c>
       <c r="C9" s="19" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D9" s="19" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E9" s="25" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="F9" s="26" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="G9" s="24" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="H9" s="25" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="I9" s="25" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="52.5" x14ac:dyDescent="0.35">
@@ -10872,25 +10892,25 @@
         <v>8</v>
       </c>
       <c r="C10" s="19" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D10" s="19" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E10" s="26" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="F10" s="19" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="G10" s="25" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="H10" s="25" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="I10" s="25" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="157.5" x14ac:dyDescent="0.35">
@@ -10899,25 +10919,25 @@
         <v>9</v>
       </c>
       <c r="C11" s="27" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D11" s="27" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E11" s="28" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="F11" s="25" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="G11" s="25" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="H11" s="25" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="I11" s="25" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="192.5" x14ac:dyDescent="0.35">
@@ -10928,52 +10948,52 @@
         <v>7</v>
       </c>
       <c r="C12" s="25" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D12" s="25" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E12" s="25" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="F12" s="25" t="s">
+        <v>65</v>
+      </c>
+      <c r="G12" s="25" t="s">
         <v>69</v>
       </c>
-      <c r="G12" s="25" t="s">
-        <v>73</v>
-      </c>
       <c r="H12" s="25" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="I12" s="26" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" ht="192.5" x14ac:dyDescent="0.35">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="175" x14ac:dyDescent="0.35">
       <c r="A13" s="47"/>
       <c r="B13" s="21" t="s">
         <v>8</v>
       </c>
       <c r="C13" s="25" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D13" s="25" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E13" s="25" t="s">
+        <v>65</v>
+      </c>
+      <c r="F13" s="25" t="s">
         <v>69</v>
       </c>
-      <c r="F13" s="25" t="s">
-        <v>73</v>
-      </c>
       <c r="G13" s="25" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="H13" s="26" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="I13" s="25" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="87.5" x14ac:dyDescent="0.35">
@@ -10982,25 +11002,25 @@
         <v>9</v>
       </c>
       <c r="C14" s="19" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D14" s="19" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E14" s="22" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="F14" s="22" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="G14" s="24" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="H14" s="25" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="I14" s="24" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="70" x14ac:dyDescent="0.35">
@@ -11011,25 +11031,25 @@
         <v>7</v>
       </c>
       <c r="C15" s="19" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D15" s="19" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E15" s="25" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="F15" s="26" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="G15" s="24" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="H15" s="25" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="I15" s="25" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="52.5" x14ac:dyDescent="0.35">
@@ -11038,25 +11058,25 @@
         <v>8</v>
       </c>
       <c r="C16" s="19" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D16" s="19" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E16" s="26" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="F16" s="24" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="G16" s="25" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="H16" s="25" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="I16" s="25" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="157.5" x14ac:dyDescent="0.35">
@@ -11065,25 +11085,25 @@
         <v>9</v>
       </c>
       <c r="C17" s="25" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D17" s="25" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E17" s="28" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="F17" s="25" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="G17" s="25" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="H17" s="25" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="I17" s="25" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -11107,7 +11127,7 @@
   <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection sqref="A1:A2"/>
+      <selection activeCell="C1" sqref="C1:I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.453125" defaultRowHeight="17.5" x14ac:dyDescent="0.35"/>
@@ -11130,7 +11150,7 @@
         <v>0</v>
       </c>
       <c r="C1" s="48" t="s">
-        <v>64</v>
+        <v>101</v>
       </c>
       <c r="D1" s="48"/>
       <c r="E1" s="48"/>
@@ -11172,25 +11192,25 @@
         <v>7</v>
       </c>
       <c r="C3" s="25" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D3" s="25" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="E3" s="25" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="F3" s="25" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="G3" s="25" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="H3" s="25" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="I3" s="25" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="140" x14ac:dyDescent="0.35">
@@ -11199,25 +11219,25 @@
         <v>12</v>
       </c>
       <c r="C4" s="25" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="D4" s="25" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="E4" s="25" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="F4" s="25" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="G4" s="25" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="H4" s="25" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="I4" s="25" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="52.5" x14ac:dyDescent="0.35">
@@ -11226,13 +11246,13 @@
         <v>9</v>
       </c>
       <c r="C5" s="25" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="D5" s="25" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="E5" s="25" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="F5" s="31" t="s">
         <v>30</v>
@@ -11255,25 +11275,25 @@
         <v>7</v>
       </c>
       <c r="C6" s="25" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D6" s="25" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="E6" s="25" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="F6" s="25" t="s">
+        <v>77</v>
+      </c>
+      <c r="G6" s="25" t="s">
         <v>81</v>
       </c>
-      <c r="G6" s="25" t="s">
-        <v>85</v>
-      </c>
       <c r="H6" s="25" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="I6" s="25" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="140" x14ac:dyDescent="0.35">
@@ -11282,25 +11302,25 @@
         <v>8</v>
       </c>
       <c r="C7" s="25" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="D7" s="25" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="E7" s="25" t="s">
+        <v>77</v>
+      </c>
+      <c r="F7" s="25" t="s">
         <v>81</v>
       </c>
-      <c r="F7" s="25" t="s">
-        <v>85</v>
-      </c>
       <c r="G7" s="25" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="H7" s="25" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="I7" s="25" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="52.5" x14ac:dyDescent="0.35">
@@ -11309,13 +11329,13 @@
         <v>9</v>
       </c>
       <c r="C8" s="25" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="D8" s="25" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="E8" s="25" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="F8" s="31" t="s">
         <v>30</v>
@@ -11338,25 +11358,25 @@
         <v>7</v>
       </c>
       <c r="C9" s="25" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D9" s="25" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E9" s="25" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="F9" s="25" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="G9" s="33" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="H9" s="25" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="I9" s="25" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="140" x14ac:dyDescent="0.35">
@@ -11365,25 +11385,25 @@
         <v>8</v>
       </c>
       <c r="C10" s="25" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D10" s="25" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E10" s="25" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="F10" s="32" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="G10" s="25" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="H10" s="25" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="I10" s="25" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="52.5" x14ac:dyDescent="0.35">
@@ -11392,13 +11412,13 @@
         <v>9</v>
       </c>
       <c r="C11" s="25" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D11" s="25" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E11" s="25" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="F11" s="25" t="s">
         <v>30</v>
@@ -11421,25 +11441,25 @@
         <v>7</v>
       </c>
       <c r="C12" s="25" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D12" s="25" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="E12" s="25" t="s">
+        <v>75</v>
+      </c>
+      <c r="F12" s="25" t="s">
         <v>79</v>
       </c>
-      <c r="F12" s="25" t="s">
-        <v>83</v>
-      </c>
       <c r="G12" s="25" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="H12" s="25" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="I12" s="25" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="140" x14ac:dyDescent="0.35">
@@ -11448,25 +11468,25 @@
         <v>8</v>
       </c>
       <c r="C13" s="25" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="D13" s="25" t="s">
+        <v>75</v>
+      </c>
+      <c r="E13" s="25" t="s">
         <v>79</v>
       </c>
-      <c r="E13" s="25" t="s">
-        <v>83</v>
-      </c>
       <c r="F13" s="25" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="G13" s="25" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="H13" s="25" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="I13" s="25" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="52.5" x14ac:dyDescent="0.35">
@@ -11475,13 +11495,13 @@
         <v>9</v>
       </c>
       <c r="C14" s="25" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="D14" s="25" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="E14" s="25" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="F14" s="24" t="s">
         <v>30</v>
@@ -11504,28 +11524,28 @@
         <v>7</v>
       </c>
       <c r="C15" s="25" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D15" s="25" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E15" s="25" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="F15" s="25" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="G15" s="33" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="H15" s="25" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="I15" s="25" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="J15" s="25" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="157.5" x14ac:dyDescent="0.35">
@@ -11534,28 +11554,28 @@
         <v>8</v>
       </c>
       <c r="C16" s="25" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D16" s="25" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E16" s="25" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="F16" s="24" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="G16" s="25" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="H16" s="25" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="I16" s="25" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="J16" s="25" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="52.5" x14ac:dyDescent="0.35">
@@ -11564,13 +11584,13 @@
         <v>9</v>
       </c>
       <c r="C17" s="25" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D17" s="25" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E17" s="25" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="F17" s="25" t="s">
         <v>30</v>
@@ -11609,7 +11629,7 @@
   <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="C1" sqref="C1:I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.453125" defaultRowHeight="17.5" x14ac:dyDescent="0.35"/>
@@ -11632,7 +11652,7 @@
         <v>0</v>
       </c>
       <c r="C1" s="48" t="s">
-        <v>64</v>
+        <v>100</v>
       </c>
       <c r="D1" s="48"/>
       <c r="E1" s="48"/>
@@ -11674,25 +11694,25 @@
         <v>7</v>
       </c>
       <c r="C3" s="25" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="D3" s="25" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E3" s="25" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="F3" s="25" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="G3" s="25" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="H3" s="25" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="I3" s="25" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="35" x14ac:dyDescent="0.35">
@@ -11701,25 +11721,25 @@
         <v>12</v>
       </c>
       <c r="C4" s="25" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D4" s="25" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E4" s="25" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="F4" s="25" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="G4" s="25" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="H4" s="25" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="I4" s="25" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="52.5" x14ac:dyDescent="0.35">
@@ -11728,16 +11748,16 @@
         <v>9</v>
       </c>
       <c r="C5" s="25" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="D5" s="25" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="E5" s="25" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="F5" s="25" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="G5" s="25" t="s">
         <v>30</v>
@@ -11757,25 +11777,25 @@
         <v>7</v>
       </c>
       <c r="C6" s="25" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="D6" s="25" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E6" s="25" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="F6" s="25" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="G6" s="25" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="H6" s="25" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="I6" s="25" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="52.5" x14ac:dyDescent="0.35">
@@ -11784,25 +11804,25 @@
         <v>8</v>
       </c>
       <c r="C7" s="25" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D7" s="25" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E7" s="25" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="F7" s="25" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="G7" s="25" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="H7" s="25" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="I7" s="25" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="52.5" x14ac:dyDescent="0.35">
@@ -11811,16 +11831,16 @@
         <v>9</v>
       </c>
       <c r="C8" s="25" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="D8" s="25" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="E8" s="25" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="F8" s="25" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="G8" s="25" t="s">
         <v>30</v>
@@ -11840,25 +11860,25 @@
         <v>7</v>
       </c>
       <c r="C9" s="25" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="D9" s="25" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="E9" s="25" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="F9" s="25" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="G9" s="25" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="H9" s="25" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="I9" s="25" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="87.5" x14ac:dyDescent="0.35">
@@ -11867,25 +11887,25 @@
         <v>8</v>
       </c>
       <c r="C10" s="25" t="s">
+        <v>89</v>
+      </c>
+      <c r="D10" s="25" t="s">
+        <v>52</v>
+      </c>
+      <c r="E10" s="25" t="s">
+        <v>52</v>
+      </c>
+      <c r="F10" s="37" t="s">
         <v>93</v>
       </c>
-      <c r="D10" s="25" t="s">
-        <v>55</v>
-      </c>
-      <c r="E10" s="25" t="s">
-        <v>55</v>
-      </c>
-      <c r="F10" s="37" t="s">
+      <c r="G10" s="25" t="s">
+        <v>52</v>
+      </c>
+      <c r="H10" s="25" t="s">
+        <v>52</v>
+      </c>
+      <c r="I10" s="25" t="s">
         <v>97</v>
-      </c>
-      <c r="G10" s="25" t="s">
-        <v>55</v>
-      </c>
-      <c r="H10" s="25" t="s">
-        <v>55</v>
-      </c>
-      <c r="I10" s="25" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="70" x14ac:dyDescent="0.35">
@@ -11903,7 +11923,7 @@
         <v>30</v>
       </c>
       <c r="F11" s="25" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="G11" s="25" t="s">
         <v>30</v>
@@ -11923,25 +11943,25 @@
         <v>7</v>
       </c>
       <c r="C12" s="25" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="D12" s="25" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E12" s="25" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="F12" s="25" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="G12" s="25" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="H12" s="25" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="I12" s="25" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="87.5" x14ac:dyDescent="0.35">
@@ -11950,25 +11970,25 @@
         <v>8</v>
       </c>
       <c r="C13" s="25" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D13" s="25" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E13" s="25" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="F13" s="25" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="G13" s="25" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="H13" s="25" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="I13" s="25" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="52.5" x14ac:dyDescent="0.35">
@@ -11977,16 +11997,16 @@
         <v>9</v>
       </c>
       <c r="C14" s="25" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="D14" s="25" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="E14" s="25" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="F14" s="25" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="G14" s="25" t="s">
         <v>30</v>
@@ -12006,25 +12026,25 @@
         <v>7</v>
       </c>
       <c r="C15" s="25" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="D15" s="25" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E15" s="25" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="F15" s="25" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="G15" s="25" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="H15" s="25" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="I15" s="25" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="J15" s="25"/>
     </row>
@@ -12034,25 +12054,25 @@
         <v>8</v>
       </c>
       <c r="C16" s="25" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D16" s="25" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E16" s="25" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="F16" s="37" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="G16" s="25" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="H16" s="25" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="I16" s="25" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="J16" s="25"/>
     </row>
@@ -12104,8 +12124,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA7F8344-AAAE-454A-B8B2-31F07E61DB11}">
   <dimension ref="A1:J17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10:C11"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.453125" defaultRowHeight="17.5" x14ac:dyDescent="0.35"/>
@@ -12128,7 +12148,7 @@
         <v>0</v>
       </c>
       <c r="C1" s="48" t="s">
-        <v>64</v>
+        <v>99</v>
       </c>
       <c r="D1" s="48"/>
       <c r="E1" s="48"/>
@@ -12170,9 +12190,11 @@
         <v>7</v>
       </c>
       <c r="C3" s="25" t="s">
-        <v>55</v>
-      </c>
-      <c r="D3" s="25"/>
+        <v>52</v>
+      </c>
+      <c r="D3" s="25" t="s">
+        <v>52</v>
+      </c>
       <c r="E3" s="25"/>
       <c r="F3" s="25"/>
       <c r="G3" s="25"/>
@@ -12185,9 +12207,11 @@
         <v>12</v>
       </c>
       <c r="C4" s="25" t="s">
-        <v>55</v>
-      </c>
-      <c r="D4" s="25"/>
+        <v>52</v>
+      </c>
+      <c r="D4" s="25" t="s">
+        <v>52</v>
+      </c>
       <c r="E4" s="25"/>
       <c r="F4" s="25"/>
       <c r="G4" s="25"/>
@@ -12202,7 +12226,9 @@
       <c r="C5" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="D5" s="25"/>
+      <c r="D5" s="25" t="s">
+        <v>30</v>
+      </c>
       <c r="E5" s="25"/>
       <c r="F5" s="25"/>
       <c r="G5" s="25"/>
@@ -12217,9 +12243,11 @@
         <v>7</v>
       </c>
       <c r="C6" s="25" t="s">
-        <v>102</v>
-      </c>
-      <c r="D6" s="25"/>
+        <v>98</v>
+      </c>
+      <c r="D6" s="25" t="s">
+        <v>98</v>
+      </c>
       <c r="E6" s="25"/>
       <c r="F6" s="25"/>
       <c r="G6" s="25"/>
@@ -12232,9 +12260,11 @@
         <v>8</v>
       </c>
       <c r="C7" s="25" t="s">
-        <v>102</v>
-      </c>
-      <c r="D7" s="25"/>
+        <v>98</v>
+      </c>
+      <c r="D7" s="25" t="s">
+        <v>106</v>
+      </c>
       <c r="E7" s="25"/>
       <c r="F7" s="25"/>
       <c r="G7" s="25"/>
@@ -12249,7 +12279,9 @@
       <c r="C8" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="D8" s="25"/>
+      <c r="D8" s="25" t="s">
+        <v>30</v>
+      </c>
       <c r="E8" s="25"/>
       <c r="F8" s="25"/>
       <c r="G8" s="25"/>
@@ -12264,9 +12296,11 @@
         <v>7</v>
       </c>
       <c r="C9" s="25" t="s">
-        <v>101</v>
-      </c>
-      <c r="D9" s="25"/>
+        <v>97</v>
+      </c>
+      <c r="D9" s="25" t="s">
+        <v>52</v>
+      </c>
       <c r="E9" s="25"/>
       <c r="F9" s="25"/>
       <c r="G9" s="25"/>
@@ -12279,9 +12313,11 @@
         <v>8</v>
       </c>
       <c r="C10" s="25" t="s">
-        <v>55</v>
-      </c>
-      <c r="D10" s="25"/>
+        <v>52</v>
+      </c>
+      <c r="D10" s="25" t="s">
+        <v>107</v>
+      </c>
       <c r="E10" s="25"/>
       <c r="G10" s="25"/>
       <c r="H10" s="25"/>
@@ -12295,7 +12331,9 @@
       <c r="C11" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="D11" s="25"/>
+      <c r="D11" s="25" t="s">
+        <v>30</v>
+      </c>
       <c r="E11" s="25"/>
       <c r="F11" s="25"/>
       <c r="G11" s="25"/>
@@ -12310,9 +12348,11 @@
         <v>7</v>
       </c>
       <c r="C12" s="25" t="s">
-        <v>55</v>
-      </c>
-      <c r="D12" s="25"/>
+        <v>52</v>
+      </c>
+      <c r="D12" s="25" t="s">
+        <v>52</v>
+      </c>
       <c r="E12" s="25"/>
       <c r="F12" s="25"/>
       <c r="G12" s="25"/>
@@ -12325,9 +12365,11 @@
         <v>8</v>
       </c>
       <c r="C13" s="25" t="s">
-        <v>55</v>
-      </c>
-      <c r="D13" s="25"/>
+        <v>52</v>
+      </c>
+      <c r="D13" s="25" t="s">
+        <v>108</v>
+      </c>
       <c r="E13" s="25"/>
       <c r="F13" s="25"/>
       <c r="G13" s="25"/>
@@ -12342,7 +12384,9 @@
       <c r="C14" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="D14" s="25"/>
+      <c r="D14" s="25" t="s">
+        <v>30</v>
+      </c>
       <c r="E14" s="25"/>
       <c r="F14" s="25"/>
       <c r="G14" s="25"/>
@@ -12357,9 +12401,11 @@
         <v>7</v>
       </c>
       <c r="C15" s="25" t="s">
-        <v>55</v>
-      </c>
-      <c r="D15" s="25"/>
+        <v>52</v>
+      </c>
+      <c r="D15" s="25" t="s">
+        <v>52</v>
+      </c>
       <c r="E15" s="25"/>
       <c r="F15" s="25"/>
       <c r="G15" s="25"/>
@@ -12373,9 +12419,11 @@
         <v>8</v>
       </c>
       <c r="C16" s="25" t="s">
-        <v>55</v>
-      </c>
-      <c r="D16" s="25"/>
+        <v>52</v>
+      </c>
+      <c r="D16" s="25" t="s">
+        <v>52</v>
+      </c>
       <c r="E16" s="25"/>
       <c r="G16" s="25"/>
       <c r="H16" s="25"/>
@@ -12390,7 +12438,9 @@
       <c r="C17" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="D17" s="25"/>
+      <c r="D17" s="25" t="s">
+        <v>30</v>
+      </c>
       <c r="E17" s="25"/>
       <c r="F17" s="25"/>
       <c r="G17" s="25"/>

</xml_diff>

<commit_message>
update du (week 11 wed)
</commit_message>
<xml_diff>
--- a/metrics/du.xlsx
+++ b/metrics/du.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\project-g4t6\metrics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A451A0B-0335-490C-93B9-F0F7B47D963E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{544C9081-373C-4663-8FF8-96E9E51AE043}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="964" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="979" uniqueCount="112">
   <si>
     <t>Question</t>
   </si>
@@ -378,6 +378,16 @@
     <t>Not a working day 
 Updated Schedule</t>
   </si>
+  <si>
+    <t>Prepare for UAT</t>
+  </si>
+  <si>
+    <t>1. Prepare for UAT
+2. manual testcases</t>
+  </si>
+  <si>
+    <t>Preare for UAT</t>
+  </si>
 </sst>
 </file>
 
@@ -573,15 +583,15 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -909,36 +919,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="45" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="45" t="s">
+      <c r="C1" s="42" t="s">
         <v>18</v>
       </c>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45"/>
-      <c r="G1" s="45"/>
-      <c r="H1" s="45"/>
-      <c r="I1" s="45"/>
-      <c r="J1" s="42" t="s">
+      <c r="D1" s="42"/>
+      <c r="E1" s="42"/>
+      <c r="F1" s="42"/>
+      <c r="G1" s="42"/>
+      <c r="H1" s="42"/>
+      <c r="I1" s="42"/>
+      <c r="J1" s="45" t="s">
         <v>1</v>
       </c>
       <c r="K1" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="L1" s="45" t="s">
+      <c r="L1" s="42" t="s">
         <v>105</v>
       </c>
-      <c r="M1" s="45"/>
-      <c r="N1" s="45"/>
-      <c r="O1" s="45"/>
-      <c r="P1" s="45"/>
-      <c r="Q1" s="45"/>
-      <c r="R1" s="45"/>
+      <c r="M1" s="42"/>
+      <c r="N1" s="42"/>
+      <c r="O1" s="42"/>
+      <c r="P1" s="42"/>
+      <c r="Q1" s="42"/>
+      <c r="R1" s="42"/>
       <c r="S1" s="1"/>
       <c r="T1" s="1"/>
       <c r="U1" s="1"/>
@@ -5622,11 +5632,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="K1:K2"/>
-    <mergeCell ref="L1:R1"/>
-    <mergeCell ref="J3:J5"/>
-    <mergeCell ref="J6:J8"/>
-    <mergeCell ref="C1:I1"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="J15:J17"/>
@@ -5638,6 +5643,11 @@
     <mergeCell ref="A3:A5"/>
     <mergeCell ref="A6:A8"/>
     <mergeCell ref="A9:A11"/>
+    <mergeCell ref="K1:K2"/>
+    <mergeCell ref="L1:R1"/>
+    <mergeCell ref="J3:J5"/>
+    <mergeCell ref="J6:J8"/>
+    <mergeCell ref="C1:I1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -5671,7 +5681,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="45" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="40" t="s">
@@ -5680,15 +5690,15 @@
       <c r="C1" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="45" t="s">
+      <c r="D1" s="42" t="s">
         <v>104</v>
       </c>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45"/>
-      <c r="G1" s="45"/>
-      <c r="H1" s="45"/>
-      <c r="I1" s="45"/>
-      <c r="J1" s="45"/>
+      <c r="E1" s="42"/>
+      <c r="F1" s="42"/>
+      <c r="G1" s="42"/>
+      <c r="H1" s="42"/>
+      <c r="I1" s="42"/>
+      <c r="J1" s="42"/>
       <c r="S1" s="1"/>
       <c r="T1" s="1"/>
       <c r="U1" s="1"/>
@@ -10857,7 +10867,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="52.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" ht="70" x14ac:dyDescent="0.35">
       <c r="A9" s="46" t="s">
         <v>15</v>
       </c>
@@ -10969,7 +10979,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="175" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" ht="192.5" x14ac:dyDescent="0.35">
       <c r="A13" s="47"/>
       <c r="B13" s="21" t="s">
         <v>8</v>
@@ -12124,8 +12134,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA7F8344-AAAE-454A-B8B2-31F07E61DB11}">
   <dimension ref="A1:J17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.453125" defaultRowHeight="17.5" x14ac:dyDescent="0.35"/>
@@ -12195,7 +12205,9 @@
       <c r="D3" s="25" t="s">
         <v>52</v>
       </c>
-      <c r="E3" s="25"/>
+      <c r="E3" s="25" t="s">
+        <v>52</v>
+      </c>
       <c r="F3" s="25"/>
       <c r="G3" s="25"/>
       <c r="H3" s="25"/>
@@ -12212,7 +12224,9 @@
       <c r="D4" s="25" t="s">
         <v>52</v>
       </c>
-      <c r="E4" s="25"/>
+      <c r="E4" s="25" t="s">
+        <v>109</v>
+      </c>
       <c r="F4" s="25"/>
       <c r="G4" s="25"/>
       <c r="H4" s="25"/>
@@ -12229,7 +12243,9 @@
       <c r="D5" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="E5" s="25"/>
+      <c r="E5" s="25" t="s">
+        <v>30</v>
+      </c>
       <c r="F5" s="25"/>
       <c r="G5" s="25"/>
       <c r="H5" s="25"/>
@@ -12248,7 +12264,9 @@
       <c r="D6" s="25" t="s">
         <v>98</v>
       </c>
-      <c r="E6" s="25"/>
+      <c r="E6" s="25" t="s">
+        <v>106</v>
+      </c>
       <c r="F6" s="25"/>
       <c r="G6" s="25"/>
       <c r="H6" s="25"/>
@@ -12265,7 +12283,9 @@
       <c r="D7" s="25" t="s">
         <v>106</v>
       </c>
-      <c r="E7" s="25"/>
+      <c r="E7" s="25" t="s">
+        <v>111</v>
+      </c>
       <c r="F7" s="25"/>
       <c r="G7" s="25"/>
       <c r="H7" s="25"/>
@@ -12282,7 +12302,9 @@
       <c r="D8" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="E8" s="25"/>
+      <c r="E8" s="25" t="s">
+        <v>30</v>
+      </c>
       <c r="F8" s="25"/>
       <c r="G8" s="25"/>
       <c r="H8" s="25"/>
@@ -12301,7 +12323,9 @@
       <c r="D9" s="25" t="s">
         <v>52</v>
       </c>
-      <c r="E9" s="25"/>
+      <c r="E9" s="25" t="s">
+        <v>107</v>
+      </c>
       <c r="F9" s="25"/>
       <c r="G9" s="25"/>
       <c r="H9" s="25"/>
@@ -12318,7 +12342,9 @@
       <c r="D10" s="25" t="s">
         <v>107</v>
       </c>
-      <c r="E10" s="25"/>
+      <c r="E10" s="25" t="s">
+        <v>110</v>
+      </c>
       <c r="G10" s="25"/>
       <c r="H10" s="25"/>
       <c r="I10" s="25"/>
@@ -12334,7 +12360,9 @@
       <c r="D11" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="E11" s="25"/>
+      <c r="E11" s="25" t="s">
+        <v>30</v>
+      </c>
       <c r="F11" s="25"/>
       <c r="G11" s="25"/>
       <c r="H11" s="25"/>
@@ -12353,7 +12381,9 @@
       <c r="D12" s="25" t="s">
         <v>52</v>
       </c>
-      <c r="E12" s="25"/>
+      <c r="E12" s="25" t="s">
+        <v>108</v>
+      </c>
       <c r="F12" s="25"/>
       <c r="G12" s="25"/>
       <c r="H12" s="25"/>
@@ -12370,7 +12400,9 @@
       <c r="D13" s="25" t="s">
         <v>108</v>
       </c>
-      <c r="E13" s="25"/>
+      <c r="E13" s="25" t="s">
+        <v>109</v>
+      </c>
       <c r="F13" s="25"/>
       <c r="G13" s="25"/>
       <c r="H13" s="25"/>
@@ -12387,7 +12419,9 @@
       <c r="D14" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="E14" s="25"/>
+      <c r="E14" s="25" t="s">
+        <v>30</v>
+      </c>
       <c r="F14" s="25"/>
       <c r="G14" s="25"/>
       <c r="H14" s="25"/>
@@ -12406,7 +12440,9 @@
       <c r="D15" s="25" t="s">
         <v>52</v>
       </c>
-      <c r="E15" s="25"/>
+      <c r="E15" s="25" t="s">
+        <v>52</v>
+      </c>
       <c r="F15" s="25"/>
       <c r="G15" s="25"/>
       <c r="H15" s="25"/>
@@ -12424,7 +12460,9 @@
       <c r="D16" s="25" t="s">
         <v>52</v>
       </c>
-      <c r="E16" s="25"/>
+      <c r="E16" s="25" t="s">
+        <v>109</v>
+      </c>
       <c r="G16" s="25"/>
       <c r="H16" s="25"/>
       <c r="I16" s="25"/>
@@ -12441,7 +12479,9 @@
       <c r="D17" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="E17" s="25"/>
+      <c r="E17" s="25" t="s">
+        <v>30</v>
+      </c>
       <c r="F17" s="25"/>
       <c r="G17" s="25"/>
       <c r="H17" s="25"/>

</xml_diff>

<commit_message>
update du (week 11 thurs)
</commit_message>
<xml_diff>
--- a/metrics/du.xlsx
+++ b/metrics/du.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\project-g4t6\metrics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{544C9081-373C-4663-8FF8-96E9E51AE043}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C0E46C7-E928-4D11-A623-17613F5AF162}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="979" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="994" uniqueCount="114">
   <si>
     <t>Question</t>
   </si>
@@ -388,6 +388,12 @@
   <si>
     <t>Preare for UAT</t>
   </si>
+  <si>
+    <t>Debugging and reviewing codes for UAT</t>
+  </si>
+  <si>
+    <t>Update Manual testcases</t>
+  </si>
 </sst>
 </file>
 
@@ -583,15 +589,15 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -919,36 +925,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="42" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="42" t="s">
+      <c r="C1" s="45" t="s">
         <v>18</v>
       </c>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42"/>
-      <c r="G1" s="42"/>
-      <c r="H1" s="42"/>
-      <c r="I1" s="42"/>
-      <c r="J1" s="45" t="s">
+      <c r="D1" s="45"/>
+      <c r="E1" s="45"/>
+      <c r="F1" s="45"/>
+      <c r="G1" s="45"/>
+      <c r="H1" s="45"/>
+      <c r="I1" s="45"/>
+      <c r="J1" s="42" t="s">
         <v>1</v>
       </c>
       <c r="K1" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="L1" s="42" t="s">
+      <c r="L1" s="45" t="s">
         <v>105</v>
       </c>
-      <c r="M1" s="42"/>
-      <c r="N1" s="42"/>
-      <c r="O1" s="42"/>
-      <c r="P1" s="42"/>
-      <c r="Q1" s="42"/>
-      <c r="R1" s="42"/>
+      <c r="M1" s="45"/>
+      <c r="N1" s="45"/>
+      <c r="O1" s="45"/>
+      <c r="P1" s="45"/>
+      <c r="Q1" s="45"/>
+      <c r="R1" s="45"/>
       <c r="S1" s="1"/>
       <c r="T1" s="1"/>
       <c r="U1" s="1"/>
@@ -5632,6 +5638,11 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="K1:K2"/>
+    <mergeCell ref="L1:R1"/>
+    <mergeCell ref="J3:J5"/>
+    <mergeCell ref="J6:J8"/>
+    <mergeCell ref="C1:I1"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="J15:J17"/>
@@ -5643,11 +5654,6 @@
     <mergeCell ref="A3:A5"/>
     <mergeCell ref="A6:A8"/>
     <mergeCell ref="A9:A11"/>
-    <mergeCell ref="K1:K2"/>
-    <mergeCell ref="L1:R1"/>
-    <mergeCell ref="J3:J5"/>
-    <mergeCell ref="J6:J8"/>
-    <mergeCell ref="C1:I1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -5681,7 +5687,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="42" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="40" t="s">
@@ -5690,15 +5696,15 @@
       <c r="C1" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="42" t="s">
+      <c r="D1" s="45" t="s">
         <v>104</v>
       </c>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42"/>
-      <c r="G1" s="42"/>
-      <c r="H1" s="42"/>
-      <c r="I1" s="42"/>
-      <c r="J1" s="42"/>
+      <c r="E1" s="45"/>
+      <c r="F1" s="45"/>
+      <c r="G1" s="45"/>
+      <c r="H1" s="45"/>
+      <c r="I1" s="45"/>
+      <c r="J1" s="45"/>
       <c r="S1" s="1"/>
       <c r="T1" s="1"/>
       <c r="U1" s="1"/>
@@ -12134,8 +12140,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA7F8344-AAAE-454A-B8B2-31F07E61DB11}">
   <dimension ref="A1:J17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.453125" defaultRowHeight="17.5" x14ac:dyDescent="0.35"/>
@@ -12208,7 +12214,9 @@
       <c r="E3" s="25" t="s">
         <v>52</v>
       </c>
-      <c r="F3" s="25"/>
+      <c r="F3" s="25" t="s">
+        <v>109</v>
+      </c>
       <c r="G3" s="25"/>
       <c r="H3" s="25"/>
       <c r="I3" s="25"/>
@@ -12227,7 +12235,9 @@
       <c r="E4" s="25" t="s">
         <v>109</v>
       </c>
-      <c r="F4" s="25"/>
+      <c r="F4" s="25" t="s">
+        <v>52</v>
+      </c>
       <c r="G4" s="25"/>
       <c r="H4" s="25"/>
       <c r="I4" s="25"/>
@@ -12246,12 +12256,14 @@
       <c r="E5" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="F5" s="25"/>
+      <c r="F5" s="25" t="s">
+        <v>30</v>
+      </c>
       <c r="G5" s="25"/>
       <c r="H5" s="25"/>
       <c r="I5" s="25"/>
     </row>
-    <row r="6" spans="1:10" ht="35" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" ht="52.5" x14ac:dyDescent="0.35">
       <c r="A6" s="46" t="s">
         <v>14</v>
       </c>
@@ -12267,7 +12279,9 @@
       <c r="E6" s="25" t="s">
         <v>106</v>
       </c>
-      <c r="F6" s="25"/>
+      <c r="F6" s="25" t="s">
+        <v>112</v>
+      </c>
       <c r="G6" s="25"/>
       <c r="H6" s="25"/>
       <c r="I6" s="25"/>
@@ -12284,9 +12298,11 @@
         <v>106</v>
       </c>
       <c r="E7" s="25" t="s">
+        <v>112</v>
+      </c>
+      <c r="F7" s="25" t="s">
         <v>111</v>
       </c>
-      <c r="F7" s="25"/>
       <c r="G7" s="25"/>
       <c r="H7" s="25"/>
       <c r="I7" s="25"/>
@@ -12305,7 +12321,9 @@
       <c r="E8" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="F8" s="25"/>
+      <c r="F8" s="25" t="s">
+        <v>30</v>
+      </c>
       <c r="G8" s="25"/>
       <c r="H8" s="25"/>
       <c r="I8" s="25"/>
@@ -12326,7 +12344,9 @@
       <c r="E9" s="25" t="s">
         <v>107</v>
       </c>
-      <c r="F9" s="25"/>
+      <c r="F9" s="25" t="s">
+        <v>110</v>
+      </c>
       <c r="G9" s="25"/>
       <c r="H9" s="25"/>
       <c r="I9" s="25"/>
@@ -12345,6 +12365,9 @@
       <c r="E10" s="25" t="s">
         <v>110</v>
       </c>
+      <c r="F10" s="39" t="s">
+        <v>109</v>
+      </c>
       <c r="G10" s="25"/>
       <c r="H10" s="25"/>
       <c r="I10" s="25"/>
@@ -12363,7 +12386,9 @@
       <c r="E11" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="F11" s="25"/>
+      <c r="F11" s="25" t="s">
+        <v>30</v>
+      </c>
       <c r="G11" s="25"/>
       <c r="H11" s="25"/>
       <c r="I11" s="25"/>
@@ -12384,7 +12409,9 @@
       <c r="E12" s="25" t="s">
         <v>108</v>
       </c>
-      <c r="F12" s="25"/>
+      <c r="F12" s="25" t="s">
+        <v>109</v>
+      </c>
       <c r="G12" s="25"/>
       <c r="H12" s="25"/>
       <c r="I12" s="25"/>
@@ -12403,7 +12430,9 @@
       <c r="E13" s="25" t="s">
         <v>109</v>
       </c>
-      <c r="F13" s="25"/>
+      <c r="F13" s="25" t="s">
+        <v>113</v>
+      </c>
       <c r="G13" s="25"/>
       <c r="H13" s="25"/>
       <c r="I13" s="25"/>
@@ -12422,12 +12451,14 @@
       <c r="E14" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="F14" s="25"/>
+      <c r="F14" s="25" t="s">
+        <v>30</v>
+      </c>
       <c r="G14" s="25"/>
       <c r="H14" s="25"/>
       <c r="I14" s="25"/>
     </row>
-    <row r="15" spans="1:10" ht="35" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:10" ht="52.5" x14ac:dyDescent="0.35">
       <c r="A15" s="46" t="s">
         <v>17</v>
       </c>
@@ -12443,7 +12474,9 @@
       <c r="E15" s="25" t="s">
         <v>52</v>
       </c>
-      <c r="F15" s="25"/>
+      <c r="F15" s="25" t="s">
+        <v>112</v>
+      </c>
       <c r="G15" s="25"/>
       <c r="H15" s="25"/>
       <c r="I15" s="25"/>
@@ -12461,7 +12494,10 @@
         <v>52</v>
       </c>
       <c r="E16" s="25" t="s">
-        <v>109</v>
+        <v>112</v>
+      </c>
+      <c r="F16" s="25" t="s">
+        <v>111</v>
       </c>
       <c r="G16" s="25"/>
       <c r="H16" s="25"/>
@@ -12482,7 +12518,9 @@
       <c r="E17" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="F17" s="25"/>
+      <c r="F17" s="25" t="s">
+        <v>30</v>
+      </c>
       <c r="G17" s="25"/>
       <c r="H17" s="25"/>
       <c r="I17" s="25"/>

</xml_diff>